<commit_message>
Added period label and tweaked Table 1 Ref file
</commit_message>
<xml_diff>
--- a/reference_files/Table1-HSMR.xlsx
+++ b/reference_files/Table1-HSMR.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\github\hsmr\reference_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Isdsf00d03\quality_indicators\hsmr\quarter_cycle\Robyn\reference_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="122">
   <si>
     <t>V217H</t>
   </si>
@@ -253,9 +253,6 @@
     <t>Hospital Standardised Mortality Ratios in Scotland</t>
   </si>
   <si>
-    <t>Select 12 month period:</t>
-  </si>
-  <si>
     <t>HB</t>
   </si>
   <si>
@@ -304,9 +301,6 @@
     <t>NHS Greater Glasgow &amp; Clyde</t>
   </si>
   <si>
-    <t>S08000021</t>
-  </si>
-  <si>
     <t>NHS Highland</t>
   </si>
   <si>
@@ -314,9 +308,6 @@
   </si>
   <si>
     <t>NHS Lanarkshire</t>
-  </si>
-  <si>
-    <t>S08000023</t>
   </si>
   <si>
     <t>NHS Lothian</t>
@@ -399,14 +390,21 @@
   <si>
     <t>lookup</t>
   </si>
+  <si>
+    <t>S08000031</t>
+  </si>
+  <si>
+    <t>S08000032</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#.00"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="27" x14ac:knownFonts="1">
     <font>
@@ -575,6 +573,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -640,7 +639,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -730,9 +729,6 @@
     <xf numFmtId="2" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="14" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -749,6 +745,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="18" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="23" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2800,7 +2800,7 @@
         <c:axId val="553192216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="2500"/>
+          <c:max val="2800"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -2843,7 +2843,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2958,7 +2957,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3036,7 +3034,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3651,71 +3648,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="16" fmlaLink="$A$5" fmlaRange="period_lookup!$A$1:$A$9" noThreeD="1" sel="3" val="0"/>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>57150</xdr:colOff>
-          <xdr:row>6</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>533400</xdr:colOff>
-          <xdr:row>7</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="56323" name="Drop Down 3" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s56323"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4504,7 +4437,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AA84"/>
   <sheetViews>
@@ -4522,19 +4455,19 @@
     <row r="1" spans="1:27" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="47"/>
       <c r="B1" s="8"/>
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
+      <c r="M1" s="66"/>
     </row>
     <row r="2" spans="1:27" s="9" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="47"/>
@@ -4609,8 +4542,9 @@
     <row r="6" spans="1:27" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="48"/>
       <c r="B6" s="15"/>
-      <c r="C6" s="14" t="s">
-        <v>74</v>
+      <c r="C6" s="14">
+        <f>period_lookup!A1</f>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
@@ -4633,24 +4567,24 @@
     <row r="10" spans="1:27" ht="34.5" x14ac:dyDescent="0.25">
       <c r="C10" s="42"/>
       <c r="D10" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="E10" s="43" t="s">
+        <v>104</v>
+      </c>
+      <c r="F10" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="G10" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="E10" s="43" t="s">
+      <c r="H10" s="43" t="s">
         <v>107</v>
-      </c>
-      <c r="F10" s="43" t="s">
-        <v>108</v>
-      </c>
-      <c r="G10" s="43" t="s">
-        <v>109</v>
-      </c>
-      <c r="H10" s="43" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11" s="38" t="s">
         <v>24</v>
@@ -4674,7 +4608,7 @@
         <f>VLOOKUP($B11&amp;$A$5,funnel_data!$A:$X,5,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H11" s="56" t="e">
+      <c r="H11" s="67" t="e">
         <f>VLOOKUP($B11&amp;$A$5,funnel_data!$A:$X,7,FALSE)</f>
         <v>#N/A</v>
       </c>
@@ -4689,13 +4623,13 @@
     </row>
     <row r="13" spans="1:27" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D13" s="39" t="e">
         <f>VLOOKUP($B13&amp;$A$5,funnel_data!$A:$X,3,FALSE)</f>
@@ -4723,10 +4657,10 @@
         <v>60</v>
       </c>
       <c r="B14" s="38" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D14" s="40" t="e">
         <f>VLOOKUP($B14&amp;$A$5,funnel_data!$A:$X,3,FALSE)</f>
@@ -4813,13 +4747,13 @@
     </row>
     <row r="17" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B17" s="38" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D17" s="39" t="e">
         <f>VLOOKUP($B17&amp;$A$5,funnel_data!$A:$X,3,FALSE)</f>
@@ -4875,13 +4809,13 @@
     </row>
     <row r="19" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B19" s="38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C19" s="32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D19" s="39" t="e">
         <f>VLOOKUP($B19&amp;$A$5,funnel_data!$A:$X,3,FALSE)</f>
@@ -4940,10 +4874,10 @@
         <v>60</v>
       </c>
       <c r="B21" s="38" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C21" s="33" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D21" s="40" t="e">
         <f>VLOOKUP($B21&amp;$A$5,funnel_data!$A:$X,3,FALSE)</f>
@@ -4968,13 +4902,13 @@
     </row>
     <row r="22" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B22" s="38" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C22" s="32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D22" s="39" t="e">
         <f>VLOOKUP($B22&amp;$A$5,funnel_data!$A:$X,3,FALSE)</f>
@@ -5002,10 +4936,10 @@
         <v>60</v>
       </c>
       <c r="B23" s="38" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C23" s="33" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D23" s="40" t="e">
         <f>VLOOKUP($B23&amp;$A$5,funnel_data!$A:$X,3,FALSE)</f>
@@ -5036,7 +4970,7 @@
         <v>9</v>
       </c>
       <c r="C24" s="33" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D24" s="40" t="e">
         <f>VLOOKUP($B24&amp;$A$5,funnel_data!$A:$X,3,FALSE)</f>
@@ -5061,13 +4995,13 @@
     </row>
     <row r="25" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B25" s="38" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C25" s="32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D25" s="39" t="e">
         <f>VLOOKUP($B25&amp;$A$5,funnel_data!$A:$X,3,FALSE)</f>
@@ -5123,13 +5057,13 @@
     </row>
     <row r="27" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B27" s="38" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C27" s="32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D27" s="39" t="e">
         <f>VLOOKUP($B27&amp;$A$5,funnel_data!$A:$X,3,FALSE)</f>
@@ -5218,13 +5152,13 @@
     </row>
     <row r="30" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B30" s="38" t="s">
-        <v>91</v>
+        <v>120</v>
       </c>
       <c r="C30" s="32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D30" s="39" t="e">
         <f>VLOOKUP($B30&amp;$A$5,funnel_data!$A:$X,3,FALSE)</f>
@@ -5348,7 +5282,7 @@
         <v>7</v>
       </c>
       <c r="C34" s="33" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D34" s="40" t="e">
         <f>VLOOKUP($B34&amp;$A$5,funnel_data!$A:$X,3,FALSE)</f>
@@ -5373,13 +5307,13 @@
     </row>
     <row r="35" spans="1:8" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B35" s="38" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C35" s="32" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D35" s="39" t="e">
         <f>VLOOKUP($B35&amp;$A$5,funnel_data!$A:$X,3,FALSE)</f>
@@ -5528,13 +5462,13 @@
     </row>
     <row r="40" spans="1:8" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B40" s="38" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="C40" s="32" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D40" s="39" t="e">
         <f>VLOOKUP($B40&amp;$A$5,funnel_data!$A:$X,3,FALSE)</f>
@@ -5652,13 +5586,13 @@
     </row>
     <row r="44" spans="1:8" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B44" s="38" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C44" s="32" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D44" s="39" t="e">
         <f>VLOOKUP($B44&amp;$A$5,funnel_data!$A:$X,3,FALSE)</f>
@@ -5776,13 +5710,13 @@
     </row>
     <row r="48" spans="1:8" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B48" s="38" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C48" s="32" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D48" s="39" t="e">
         <f>VLOOKUP($B48&amp;$A$5,funnel_data!$A:$X,3,FALSE)</f>
@@ -5838,13 +5772,13 @@
     </row>
     <row r="50" spans="1:8" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B50" s="38" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C50" s="32" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D50" s="39" t="e">
         <f>VLOOKUP($B50&amp;$A$5,funnel_data!$A:$X,3,FALSE)</f>
@@ -5900,13 +5834,13 @@
     </row>
     <row r="52" spans="1:8" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B52" s="38" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C52" s="32" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D52" s="39" t="e">
         <f>VLOOKUP($B52&amp;$A$5,funnel_data!$A:$X,3,FALSE)</f>
@@ -6024,13 +5958,13 @@
     </row>
     <row r="56" spans="1:8" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B56" s="38" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C56" s="32" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D56" s="39" t="e">
         <f>VLOOKUP($B56&amp;$A$5,funnel_data!$A:$X,3,FALSE)</f>
@@ -6086,13 +6020,13 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="49" t="s">
+        <v>74</v>
+      </c>
+      <c r="B58" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="C58" s="32" t="s">
         <v>75</v>
-      </c>
-      <c r="B58" s="38" t="s">
-        <v>77</v>
-      </c>
-      <c r="C58" s="32" t="s">
-        <v>76</v>
       </c>
       <c r="D58" s="39" t="e">
         <f>VLOOKUP($B58&amp;$A$5,funnel_data!$A:$X,3,FALSE)</f>
@@ -6163,12 +6097,12 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C63" s="33" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C64" s="33" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
@@ -6195,36 +6129,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x14">
-      <controls>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="56323" r:id="rId4" name="Drop Down 3">
-              <controlPr defaultSize="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>2</xdr:col>
-                    <xdr:colOff>57150</xdr:colOff>
-                    <xdr:row>6</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>3</xdr:col>
-                    <xdr:colOff>533400</xdr:colOff>
-                    <xdr:row>7</xdr:row>
-                    <xdr:rowOff>57150</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-      </controls>
-    </mc:Choice>
-  </mc:AlternateContent>
 </worksheet>
 </file>
 
@@ -6235,7 +6139,9 @@
   </sheetPr>
   <dimension ref="A1:AK121"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AQ29" sqref="AQ29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6252,19 +6158,19 @@
   <sheetData>
     <row r="1" spans="1:36" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
     </row>
     <row r="2" spans="1:36" s="9" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
@@ -6313,8 +6219,8 @@
     <row r="4" spans="1:36" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="14" t="str">
-        <f>"Hospital Standardised Mortality Ratio (Funnel Plot); " &amp; A5</f>
-        <v>Hospital Standardised Mortality Ratio (Funnel Plot); January 2018 to December 2018</v>
+        <f>"Hospital Standardised Mortality Ratio (Funnel Plot); " &amp; period_lookup!A1</f>
+        <v>Hospital Standardised Mortality Ratio (Funnel Plot); 0</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
@@ -6329,7 +6235,7 @@
     </row>
     <row r="5" spans="1:36" s="15" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:36" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8631,37 +8537,37 @@
     </row>
     <row r="81" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B81" s="45"/>
-      <c r="C81" s="61"/>
-      <c r="D81" s="61"/>
-      <c r="E81" s="61"/>
-      <c r="F81" s="61"/>
-      <c r="G81" s="61"/>
-      <c r="H81" s="61"/>
-      <c r="I81" s="61"/>
+      <c r="C81" s="60"/>
+      <c r="D81" s="60"/>
+      <c r="E81" s="60"/>
+      <c r="F81" s="60"/>
+      <c r="G81" s="60"/>
+      <c r="H81" s="60"/>
+      <c r="I81" s="60"/>
     </row>
     <row r="82" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B82" s="15">
         <v>1</v>
       </c>
-      <c r="C82" s="62">
+      <c r="C82" s="61">
         <v>4</v>
       </c>
-      <c r="D82" s="62">
+      <c r="D82" s="61">
         <v>10</v>
       </c>
-      <c r="E82" s="62">
+      <c r="E82" s="61">
         <v>6</v>
       </c>
-      <c r="F82" s="62">
+      <c r="F82" s="61">
         <v>19</v>
       </c>
-      <c r="G82" s="62">
+      <c r="G82" s="61">
         <v>21</v>
       </c>
-      <c r="H82" s="62">
+      <c r="H82" s="61">
         <v>18</v>
       </c>
-      <c r="I82" s="63">
+      <c r="I82" s="62">
         <v>20</v>
       </c>
       <c r="Q82" s="50"/>
@@ -8670,7 +8576,7 @@
       <c r="T82" s="50"/>
       <c r="U82" s="50"/>
       <c r="V82" s="50"/>
-      <c r="W82" s="64"/>
+      <c r="W82" s="63"/>
     </row>
     <row r="83" spans="1:23" s="15" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B83" s="45" t="s">
@@ -8714,35 +8620,35 @@
       <c r="B84" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C84" s="65" t="e">
+      <c r="C84" s="64" t="e">
         <f>VLOOKUP($B84&amp;"3",funnel_data!$A:$X,C$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D84" s="65">
+      <c r="D84" s="64">
         <v>1</v>
       </c>
-      <c r="E84" s="65" t="e">
+      <c r="E84" s="64" t="e">
         <f>VLOOKUP($B84&amp;"3",funnel_data!$A:$X,E$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F84" s="65" t="e">
+      <c r="F84" s="64" t="e">
         <f>VLOOKUP($B84&amp;"3",funnel_data!$A:$X,F$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G84" s="65" t="e">
+      <c r="G84" s="64" t="e">
         <f>VLOOKUP($B84&amp;"3",funnel_data!$A:$X,G$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H84" s="65" t="e">
+      <c r="H84" s="64" t="e">
         <f>VLOOKUP($B84&amp;"3",funnel_data!$A:$X,H$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I84" s="65" t="e">
+      <c r="I84" s="64" t="e">
         <f>VLOOKUP($B84&amp;"3",funnel_data!$A:$X,I$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M84" s="66"/>
-      <c r="N84" s="66"/>
+      <c r="M84" s="65"/>
+      <c r="N84" s="65"/>
     </row>
     <row r="85" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="15" t="e">
@@ -8750,37 +8656,37 @@
         <v>#N/A</v>
       </c>
       <c r="B85" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="C85" s="65" t="e">
+        <v>109</v>
+      </c>
+      <c r="C85" s="64" t="e">
         <f>VLOOKUP($B85&amp;"3",funnel_data!$A:$X,C$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D85" s="65">
+      <c r="D85" s="64">
         <v>1</v>
       </c>
-      <c r="E85" s="65" t="e">
+      <c r="E85" s="64" t="e">
         <f>VLOOKUP($B85&amp;"3",funnel_data!$A:$X,E$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F85" s="65" t="e">
+      <c r="F85" s="64" t="e">
         <f>VLOOKUP($B85&amp;"3",funnel_data!$A:$X,F$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G85" s="65" t="e">
+      <c r="G85" s="64" t="e">
         <f>VLOOKUP($B85&amp;"3",funnel_data!$A:$X,G$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H85" s="65" t="e">
+      <c r="H85" s="64" t="e">
         <f>VLOOKUP($B85&amp;"3",funnel_data!$A:$X,H$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I85" s="65" t="e">
+      <c r="I85" s="64" t="e">
         <f>VLOOKUP($B85&amp;"3",funnel_data!$A:$X,I$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M85" s="66"/>
-      <c r="N85" s="66"/>
+      <c r="M85" s="65"/>
+      <c r="N85" s="65"/>
     </row>
     <row r="86" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="15" t="e">
@@ -8790,35 +8696,35 @@
       <c r="B86" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="C86" s="65" t="e">
+      <c r="C86" s="64" t="e">
         <f>VLOOKUP($B86&amp;"3",funnel_data!$A:$X,C$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D86" s="65">
+      <c r="D86" s="64">
         <v>1</v>
       </c>
-      <c r="E86" s="65" t="e">
+      <c r="E86" s="64" t="e">
         <f>VLOOKUP($B86&amp;"3",funnel_data!$A:$X,E$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F86" s="65" t="e">
+      <c r="F86" s="64" t="e">
         <f>VLOOKUP($B86&amp;"3",funnel_data!$A:$X,F$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G86" s="65" t="e">
+      <c r="G86" s="64" t="e">
         <f>VLOOKUP($B86&amp;"3",funnel_data!$A:$X,G$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H86" s="65" t="e">
+      <c r="H86" s="64" t="e">
         <f>VLOOKUP($B86&amp;"3",funnel_data!$A:$X,H$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I86" s="65" t="e">
+      <c r="I86" s="64" t="e">
         <f>VLOOKUP($B86&amp;"3",funnel_data!$A:$X,I$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M86" s="66"/>
-      <c r="N86" s="66"/>
+      <c r="M86" s="65"/>
+      <c r="N86" s="65"/>
     </row>
     <row r="87" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="15" t="e">
@@ -8828,35 +8734,35 @@
       <c r="B87" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="C87" s="65" t="e">
+      <c r="C87" s="64" t="e">
         <f>VLOOKUP($B87&amp;"3",funnel_data!$A:$X,C$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D87" s="65">
+      <c r="D87" s="64">
         <v>1</v>
       </c>
-      <c r="E87" s="65" t="e">
+      <c r="E87" s="64" t="e">
         <f>VLOOKUP($B87&amp;"3",funnel_data!$A:$X,E$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F87" s="65" t="e">
+      <c r="F87" s="64" t="e">
         <f>VLOOKUP($B87&amp;"3",funnel_data!$A:$X,F$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G87" s="65" t="e">
+      <c r="G87" s="64" t="e">
         <f>VLOOKUP($B87&amp;"3",funnel_data!$A:$X,G$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H87" s="65" t="e">
+      <c r="H87" s="64" t="e">
         <f>VLOOKUP($B87&amp;"3",funnel_data!$A:$X,H$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I87" s="65" t="e">
+      <c r="I87" s="64" t="e">
         <f>VLOOKUP($B87&amp;"3",funnel_data!$A:$X,I$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M87" s="66"/>
-      <c r="N87" s="66"/>
+      <c r="M87" s="65"/>
+      <c r="N87" s="65"/>
     </row>
     <row r="88" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="15" t="e">
@@ -8866,35 +8772,35 @@
       <c r="B88" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="C88" s="65" t="e">
+      <c r="C88" s="64" t="e">
         <f>VLOOKUP($B88&amp;"3",funnel_data!$A:$X,C$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D88" s="65">
+      <c r="D88" s="64">
         <v>1</v>
       </c>
-      <c r="E88" s="65" t="e">
+      <c r="E88" s="64" t="e">
         <f>VLOOKUP($B88&amp;"3",funnel_data!$A:$X,E$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F88" s="65" t="e">
+      <c r="F88" s="64" t="e">
         <f>VLOOKUP($B88&amp;"3",funnel_data!$A:$X,F$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G88" s="65" t="e">
+      <c r="G88" s="64" t="e">
         <f>VLOOKUP($B88&amp;"3",funnel_data!$A:$X,G$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H88" s="65" t="e">
+      <c r="H88" s="64" t="e">
         <f>VLOOKUP($B88&amp;"3",funnel_data!$A:$X,H$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I88" s="65" t="e">
+      <c r="I88" s="64" t="e">
         <f>VLOOKUP($B88&amp;"3",funnel_data!$A:$X,I$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M88" s="66"/>
-      <c r="N88" s="66"/>
+      <c r="M88" s="65"/>
+      <c r="N88" s="65"/>
     </row>
     <row r="89" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="15" t="e">
@@ -8904,35 +8810,35 @@
       <c r="B89" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="C89" s="65" t="e">
+      <c r="C89" s="64" t="e">
         <f>VLOOKUP($B89&amp;"3",funnel_data!$A:$X,C$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D89" s="65">
+      <c r="D89" s="64">
         <v>1</v>
       </c>
-      <c r="E89" s="65" t="e">
+      <c r="E89" s="64" t="e">
         <f>VLOOKUP($B89&amp;"3",funnel_data!$A:$X,E$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F89" s="65" t="e">
+      <c r="F89" s="64" t="e">
         <f>VLOOKUP($B89&amp;"3",funnel_data!$A:$X,F$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G89" s="65" t="e">
+      <c r="G89" s="64" t="e">
         <f>VLOOKUP($B89&amp;"3",funnel_data!$A:$X,G$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H89" s="65" t="e">
+      <c r="H89" s="64" t="e">
         <f>VLOOKUP($B89&amp;"3",funnel_data!$A:$X,H$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I89" s="65" t="e">
+      <c r="I89" s="64" t="e">
         <f>VLOOKUP($B89&amp;"3",funnel_data!$A:$X,I$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M89" s="66"/>
-      <c r="N89" s="66"/>
+      <c r="M89" s="65"/>
+      <c r="N89" s="65"/>
     </row>
     <row r="90" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="15" t="e">
@@ -8942,35 +8848,35 @@
       <c r="B90" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="C90" s="65" t="e">
+      <c r="C90" s="64" t="e">
         <f>VLOOKUP($B90&amp;"3",funnel_data!$A:$X,C$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D90" s="65">
+      <c r="D90" s="64">
         <v>1</v>
       </c>
-      <c r="E90" s="65" t="e">
+      <c r="E90" s="64" t="e">
         <f>VLOOKUP($B90&amp;"3",funnel_data!$A:$X,E$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F90" s="65" t="e">
+      <c r="F90" s="64" t="e">
         <f>VLOOKUP($B90&amp;"3",funnel_data!$A:$X,F$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G90" s="65" t="e">
+      <c r="G90" s="64" t="e">
         <f>VLOOKUP($B90&amp;"3",funnel_data!$A:$X,G$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H90" s="65" t="e">
+      <c r="H90" s="64" t="e">
         <f>VLOOKUP($B90&amp;"3",funnel_data!$A:$X,H$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I90" s="65" t="e">
+      <c r="I90" s="64" t="e">
         <f>VLOOKUP($B90&amp;"3",funnel_data!$A:$X,I$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M90" s="66"/>
-      <c r="N90" s="66"/>
+      <c r="M90" s="65"/>
+      <c r="N90" s="65"/>
     </row>
     <row r="91" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="15" t="e">
@@ -8980,35 +8886,35 @@
       <c r="B91" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="C91" s="65" t="e">
+      <c r="C91" s="64" t="e">
         <f>VLOOKUP($B91&amp;"3",funnel_data!$A:$X,C$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D91" s="65">
+      <c r="D91" s="64">
         <v>1</v>
       </c>
-      <c r="E91" s="65" t="e">
+      <c r="E91" s="64" t="e">
         <f>VLOOKUP($B91&amp;"3",funnel_data!$A:$X,E$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F91" s="65" t="e">
+      <c r="F91" s="64" t="e">
         <f>VLOOKUP($B91&amp;"3",funnel_data!$A:$X,F$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G91" s="65" t="e">
+      <c r="G91" s="64" t="e">
         <f>VLOOKUP($B91&amp;"3",funnel_data!$A:$X,G$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H91" s="65" t="e">
+      <c r="H91" s="64" t="e">
         <f>VLOOKUP($B91&amp;"3",funnel_data!$A:$X,H$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I91" s="65" t="e">
+      <c r="I91" s="64" t="e">
         <f>VLOOKUP($B91&amp;"3",funnel_data!$A:$X,I$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M91" s="66"/>
-      <c r="N91" s="66"/>
+      <c r="M91" s="65"/>
+      <c r="N91" s="65"/>
     </row>
     <row r="92" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="15" t="e">
@@ -9018,35 +8924,35 @@
       <c r="B92" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C92" s="65" t="e">
+      <c r="C92" s="64" t="e">
         <f>VLOOKUP($B92&amp;"3",funnel_data!$A:$X,C$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D92" s="65">
+      <c r="D92" s="64">
         <v>1</v>
       </c>
-      <c r="E92" s="65" t="e">
+      <c r="E92" s="64" t="e">
         <f>VLOOKUP($B92&amp;"3",funnel_data!$A:$X,E$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F92" s="65" t="e">
+      <c r="F92" s="64" t="e">
         <f>VLOOKUP($B92&amp;"3",funnel_data!$A:$X,F$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G92" s="65" t="e">
+      <c r="G92" s="64" t="e">
         <f>VLOOKUP($B92&amp;"3",funnel_data!$A:$X,G$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H92" s="65" t="e">
+      <c r="H92" s="64" t="e">
         <f>VLOOKUP($B92&amp;"3",funnel_data!$A:$X,H$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I92" s="65" t="e">
+      <c r="I92" s="64" t="e">
         <f>VLOOKUP($B92&amp;"3",funnel_data!$A:$X,I$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M92" s="66"/>
-      <c r="N92" s="66"/>
+      <c r="M92" s="65"/>
+      <c r="N92" s="65"/>
     </row>
     <row r="93" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="15" t="e">
@@ -9054,37 +8960,37 @@
         <v>#N/A</v>
       </c>
       <c r="B93" s="45" t="s">
-        <v>113</v>
-      </c>
-      <c r="C93" s="65" t="e">
+        <v>110</v>
+      </c>
+      <c r="C93" s="64" t="e">
         <f>VLOOKUP($B93&amp;"3",funnel_data!$A:$X,C$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D93" s="65">
+      <c r="D93" s="64">
         <v>1</v>
       </c>
-      <c r="E93" s="65" t="e">
+      <c r="E93" s="64" t="e">
         <f>VLOOKUP($B93&amp;"3",funnel_data!$A:$X,E$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F93" s="65" t="e">
+      <c r="F93" s="64" t="e">
         <f>VLOOKUP($B93&amp;"3",funnel_data!$A:$X,F$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G93" s="65" t="e">
+      <c r="G93" s="64" t="e">
         <f>VLOOKUP($B93&amp;"3",funnel_data!$A:$X,G$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H93" s="65" t="e">
+      <c r="H93" s="64" t="e">
         <f>VLOOKUP($B93&amp;"3",funnel_data!$A:$X,H$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I93" s="65" t="e">
+      <c r="I93" s="64" t="e">
         <f>VLOOKUP($B93&amp;"3",funnel_data!$A:$X,I$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M93" s="66"/>
-      <c r="N93" s="66"/>
+      <c r="M93" s="65"/>
+      <c r="N93" s="65"/>
     </row>
     <row r="94" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="15" t="e">
@@ -9094,35 +9000,35 @@
       <c r="B94" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="C94" s="65" t="e">
+      <c r="C94" s="64" t="e">
         <f>VLOOKUP($B94&amp;"3",funnel_data!$A:$X,C$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D94" s="65">
+      <c r="D94" s="64">
         <v>1</v>
       </c>
-      <c r="E94" s="65" t="e">
+      <c r="E94" s="64" t="e">
         <f>VLOOKUP($B94&amp;"3",funnel_data!$A:$X,E$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F94" s="65" t="e">
+      <c r="F94" s="64" t="e">
         <f>VLOOKUP($B94&amp;"3",funnel_data!$A:$X,F$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G94" s="65" t="e">
+      <c r="G94" s="64" t="e">
         <f>VLOOKUP($B94&amp;"3",funnel_data!$A:$X,G$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H94" s="65" t="e">
+      <c r="H94" s="64" t="e">
         <f>VLOOKUP($B94&amp;"3",funnel_data!$A:$X,H$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I94" s="65" t="e">
+      <c r="I94" s="64" t="e">
         <f>VLOOKUP($B94&amp;"3",funnel_data!$A:$X,I$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M94" s="66"/>
-      <c r="N94" s="66"/>
+      <c r="M94" s="65"/>
+      <c r="N94" s="65"/>
     </row>
     <row r="95" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="15" t="e">
@@ -9132,35 +9038,35 @@
       <c r="B95" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="C95" s="65" t="e">
+      <c r="C95" s="64" t="e">
         <f>VLOOKUP($B95&amp;"3",funnel_data!$A:$X,C$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D95" s="65">
+      <c r="D95" s="64">
         <v>1</v>
       </c>
-      <c r="E95" s="65" t="e">
+      <c r="E95" s="64" t="e">
         <f>VLOOKUP($B95&amp;"3",funnel_data!$A:$X,E$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F95" s="65" t="e">
+      <c r="F95" s="64" t="e">
         <f>VLOOKUP($B95&amp;"3",funnel_data!$A:$X,F$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G95" s="65" t="e">
+      <c r="G95" s="64" t="e">
         <f>VLOOKUP($B95&amp;"3",funnel_data!$A:$X,G$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H95" s="65" t="e">
+      <c r="H95" s="64" t="e">
         <f>VLOOKUP($B95&amp;"3",funnel_data!$A:$X,H$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I95" s="65" t="e">
+      <c r="I95" s="64" t="e">
         <f>VLOOKUP($B95&amp;"3",funnel_data!$A:$X,I$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M95" s="66"/>
-      <c r="N95" s="66"/>
+      <c r="M95" s="65"/>
+      <c r="N95" s="65"/>
     </row>
     <row r="96" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="15" t="e">
@@ -9170,35 +9076,35 @@
       <c r="B96" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="C96" s="65" t="e">
+      <c r="C96" s="64" t="e">
         <f>VLOOKUP($B96&amp;"3",funnel_data!$A:$X,C$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D96" s="65">
+      <c r="D96" s="64">
         <v>1</v>
       </c>
-      <c r="E96" s="65" t="e">
+      <c r="E96" s="64" t="e">
         <f>VLOOKUP($B96&amp;"3",funnel_data!$A:$X,E$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F96" s="65" t="e">
+      <c r="F96" s="64" t="e">
         <f>VLOOKUP($B96&amp;"3",funnel_data!$A:$X,F$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G96" s="65" t="e">
+      <c r="G96" s="64" t="e">
         <f>VLOOKUP($B96&amp;"3",funnel_data!$A:$X,G$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H96" s="65" t="e">
+      <c r="H96" s="64" t="e">
         <f>VLOOKUP($B96&amp;"3",funnel_data!$A:$X,H$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I96" s="65" t="e">
+      <c r="I96" s="64" t="e">
         <f>VLOOKUP($B96&amp;"3",funnel_data!$A:$X,I$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M96" s="66"/>
-      <c r="N96" s="66"/>
+      <c r="M96" s="65"/>
+      <c r="N96" s="65"/>
     </row>
     <row r="97" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="15" t="e">
@@ -9208,35 +9114,35 @@
       <c r="B97" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="C97" s="65" t="e">
+      <c r="C97" s="64" t="e">
         <f>VLOOKUP($B97&amp;"3",funnel_data!$A:$X,C$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D97" s="65">
+      <c r="D97" s="64">
         <v>1</v>
       </c>
-      <c r="E97" s="65" t="e">
+      <c r="E97" s="64" t="e">
         <f>VLOOKUP($B97&amp;"3",funnel_data!$A:$X,E$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F97" s="65" t="e">
+      <c r="F97" s="64" t="e">
         <f>VLOOKUP($B97&amp;"3",funnel_data!$A:$X,F$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G97" s="65" t="e">
+      <c r="G97" s="64" t="e">
         <f>VLOOKUP($B97&amp;"3",funnel_data!$A:$X,G$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H97" s="65" t="e">
+      <c r="H97" s="64" t="e">
         <f>VLOOKUP($B97&amp;"3",funnel_data!$A:$X,H$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I97" s="65" t="e">
+      <c r="I97" s="64" t="e">
         <f>VLOOKUP($B97&amp;"3",funnel_data!$A:$X,I$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M97" s="66"/>
-      <c r="N97" s="66"/>
+      <c r="M97" s="65"/>
+      <c r="N97" s="65"/>
     </row>
     <row r="98" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="15" t="e">
@@ -9246,35 +9152,35 @@
       <c r="B98" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="C98" s="65" t="e">
+      <c r="C98" s="64" t="e">
         <f>VLOOKUP($B98&amp;"3",funnel_data!$A:$X,C$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D98" s="65">
+      <c r="D98" s="64">
         <v>1</v>
       </c>
-      <c r="E98" s="65" t="e">
+      <c r="E98" s="64" t="e">
         <f>VLOOKUP($B98&amp;"3",funnel_data!$A:$X,E$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F98" s="65" t="e">
+      <c r="F98" s="64" t="e">
         <f>VLOOKUP($B98&amp;"3",funnel_data!$A:$X,F$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G98" s="65" t="e">
+      <c r="G98" s="64" t="e">
         <f>VLOOKUP($B98&amp;"3",funnel_data!$A:$X,G$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H98" s="65" t="e">
+      <c r="H98" s="64" t="e">
         <f>VLOOKUP($B98&amp;"3",funnel_data!$A:$X,H$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I98" s="65" t="e">
+      <c r="I98" s="64" t="e">
         <f>VLOOKUP($B98&amp;"3",funnel_data!$A:$X,I$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M98" s="66"/>
-      <c r="N98" s="66"/>
+      <c r="M98" s="65"/>
+      <c r="N98" s="65"/>
     </row>
     <row r="99" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="15" t="e">
@@ -9284,35 +9190,35 @@
       <c r="B99" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="C99" s="65" t="e">
+      <c r="C99" s="64" t="e">
         <f>VLOOKUP($B99&amp;"3",funnel_data!$A:$X,C$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D99" s="65">
+      <c r="D99" s="64">
         <v>1</v>
       </c>
-      <c r="E99" s="65" t="e">
+      <c r="E99" s="64" t="e">
         <f>VLOOKUP($B99&amp;"3",funnel_data!$A:$X,E$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F99" s="65" t="e">
+      <c r="F99" s="64" t="e">
         <f>VLOOKUP($B99&amp;"3",funnel_data!$A:$X,F$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G99" s="65" t="e">
+      <c r="G99" s="64" t="e">
         <f>VLOOKUP($B99&amp;"3",funnel_data!$A:$X,G$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H99" s="65" t="e">
+      <c r="H99" s="64" t="e">
         <f>VLOOKUP($B99&amp;"3",funnel_data!$A:$X,H$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I99" s="65" t="e">
+      <c r="I99" s="64" t="e">
         <f>VLOOKUP($B99&amp;"3",funnel_data!$A:$X,I$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M99" s="66"/>
-      <c r="N99" s="66"/>
+      <c r="M99" s="65"/>
+      <c r="N99" s="65"/>
     </row>
     <row r="100" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="15" t="e">
@@ -9322,35 +9228,35 @@
       <c r="B100" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="C100" s="65" t="e">
+      <c r="C100" s="64" t="e">
         <f>VLOOKUP($B100&amp;"3",funnel_data!$A:$X,C$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D100" s="65">
+      <c r="D100" s="64">
         <v>1</v>
       </c>
-      <c r="E100" s="65" t="e">
+      <c r="E100" s="64" t="e">
         <f>VLOOKUP($B100&amp;"3",funnel_data!$A:$X,E$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F100" s="65" t="e">
+      <c r="F100" s="64" t="e">
         <f>VLOOKUP($B100&amp;"3",funnel_data!$A:$X,F$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G100" s="65" t="e">
+      <c r="G100" s="64" t="e">
         <f>VLOOKUP($B100&amp;"3",funnel_data!$A:$X,G$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H100" s="65" t="e">
+      <c r="H100" s="64" t="e">
         <f>VLOOKUP($B100&amp;"3",funnel_data!$A:$X,H$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I100" s="65" t="e">
+      <c r="I100" s="64" t="e">
         <f>VLOOKUP($B100&amp;"3",funnel_data!$A:$X,I$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M100" s="66"/>
-      <c r="N100" s="66"/>
+      <c r="M100" s="65"/>
+      <c r="N100" s="65"/>
     </row>
     <row r="101" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A101" s="15" t="e">
@@ -9360,35 +9266,35 @@
       <c r="B101" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="C101" s="65" t="e">
+      <c r="C101" s="64" t="e">
         <f>VLOOKUP($B101&amp;"3",funnel_data!$A:$X,C$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D101" s="65">
+      <c r="D101" s="64">
         <v>1</v>
       </c>
-      <c r="E101" s="65" t="e">
+      <c r="E101" s="64" t="e">
         <f>VLOOKUP($B101&amp;"3",funnel_data!$A:$X,E$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F101" s="65" t="e">
+      <c r="F101" s="64" t="e">
         <f>VLOOKUP($B101&amp;"3",funnel_data!$A:$X,F$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G101" s="65" t="e">
+      <c r="G101" s="64" t="e">
         <f>VLOOKUP($B101&amp;"3",funnel_data!$A:$X,G$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H101" s="65" t="e">
+      <c r="H101" s="64" t="e">
         <f>VLOOKUP($B101&amp;"3",funnel_data!$A:$X,H$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I101" s="65" t="e">
+      <c r="I101" s="64" t="e">
         <f>VLOOKUP($B101&amp;"3",funnel_data!$A:$X,I$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M101" s="66"/>
-      <c r="N101" s="66"/>
+      <c r="M101" s="65"/>
+      <c r="N101" s="65"/>
     </row>
     <row r="102" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="15" t="e">
@@ -9396,37 +9302,37 @@
         <v>#N/A</v>
       </c>
       <c r="B102" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="C102" s="65" t="e">
+        <v>116</v>
+      </c>
+      <c r="C102" s="64" t="e">
         <f>VLOOKUP($B102&amp;"3",funnel_data!$A:$X,C$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D102" s="65">
+      <c r="D102" s="64">
         <v>1</v>
       </c>
-      <c r="E102" s="65" t="e">
+      <c r="E102" s="64" t="e">
         <f>VLOOKUP($B102&amp;"3",funnel_data!$A:$X,E$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F102" s="65" t="e">
+      <c r="F102" s="64" t="e">
         <f>VLOOKUP($B102&amp;"3",funnel_data!$A:$X,F$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G102" s="65" t="e">
+      <c r="G102" s="64" t="e">
         <f>VLOOKUP($B102&amp;"3",funnel_data!$A:$X,G$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H102" s="65" t="e">
+      <c r="H102" s="64" t="e">
         <f>VLOOKUP($B102&amp;"3",funnel_data!$A:$X,H$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I102" s="65" t="e">
+      <c r="I102" s="64" t="e">
         <f>VLOOKUP($B102&amp;"3",funnel_data!$A:$X,I$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M102" s="66"/>
-      <c r="N102" s="66"/>
+      <c r="M102" s="65"/>
+      <c r="N102" s="65"/>
     </row>
     <row r="103" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" s="15" t="e">
@@ -9436,35 +9342,35 @@
       <c r="B103" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="C103" s="65" t="e">
+      <c r="C103" s="64" t="e">
         <f>VLOOKUP($B103&amp;"3",funnel_data!$A:$X,C$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D103" s="65">
+      <c r="D103" s="64">
         <v>1</v>
       </c>
-      <c r="E103" s="65" t="e">
+      <c r="E103" s="64" t="e">
         <f>VLOOKUP($B103&amp;"3",funnel_data!$A:$X,E$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F103" s="65" t="e">
+      <c r="F103" s="64" t="e">
         <f>VLOOKUP($B103&amp;"3",funnel_data!$A:$X,F$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G103" s="65" t="e">
+      <c r="G103" s="64" t="e">
         <f>VLOOKUP($B103&amp;"3",funnel_data!$A:$X,G$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H103" s="65" t="e">
+      <c r="H103" s="64" t="e">
         <f>VLOOKUP($B103&amp;"3",funnel_data!$A:$X,H$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I103" s="65" t="e">
+      <c r="I103" s="64" t="e">
         <f>VLOOKUP($B103&amp;"3",funnel_data!$A:$X,I$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M103" s="66"/>
-      <c r="N103" s="66"/>
+      <c r="M103" s="65"/>
+      <c r="N103" s="65"/>
     </row>
     <row r="104" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A104" s="15" t="e">
@@ -9474,35 +9380,35 @@
       <c r="B104" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="C104" s="65" t="e">
+      <c r="C104" s="64" t="e">
         <f>VLOOKUP($B104&amp;"3",funnel_data!$A:$X,C$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D104" s="65">
+      <c r="D104" s="64">
         <v>1</v>
       </c>
-      <c r="E104" s="65" t="e">
+      <c r="E104" s="64" t="e">
         <f>VLOOKUP($B104&amp;"3",funnel_data!$A:$X,E$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F104" s="65" t="e">
+      <c r="F104" s="64" t="e">
         <f>VLOOKUP($B104&amp;"3",funnel_data!$A:$X,F$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G104" s="65" t="e">
+      <c r="G104" s="64" t="e">
         <f>VLOOKUP($B104&amp;"3",funnel_data!$A:$X,G$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H104" s="65" t="e">
+      <c r="H104" s="64" t="e">
         <f>VLOOKUP($B104&amp;"3",funnel_data!$A:$X,H$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I104" s="65" t="e">
+      <c r="I104" s="64" t="e">
         <f>VLOOKUP($B104&amp;"3",funnel_data!$A:$X,I$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M104" s="66"/>
-      <c r="N104" s="66"/>
+      <c r="M104" s="65"/>
+      <c r="N104" s="65"/>
     </row>
     <row r="105" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A105" s="15" t="e">
@@ -9512,35 +9418,35 @@
       <c r="B105" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="C105" s="65" t="e">
+      <c r="C105" s="64" t="e">
         <f>VLOOKUP($B105&amp;"3",funnel_data!$A:$X,C$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D105" s="65">
+      <c r="D105" s="64">
         <v>1</v>
       </c>
-      <c r="E105" s="65" t="e">
+      <c r="E105" s="64" t="e">
         <f>VLOOKUP($B105&amp;"3",funnel_data!$A:$X,E$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F105" s="65" t="e">
+      <c r="F105" s="64" t="e">
         <f>VLOOKUP($B105&amp;"3",funnel_data!$A:$X,F$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G105" s="65" t="e">
+      <c r="G105" s="64" t="e">
         <f>VLOOKUP($B105&amp;"3",funnel_data!$A:$X,G$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H105" s="65" t="e">
+      <c r="H105" s="64" t="e">
         <f>VLOOKUP($B105&amp;"3",funnel_data!$A:$X,H$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I105" s="65" t="e">
+      <c r="I105" s="64" t="e">
         <f>VLOOKUP($B105&amp;"3",funnel_data!$A:$X,I$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M105" s="66"/>
-      <c r="N105" s="66"/>
+      <c r="M105" s="65"/>
+      <c r="N105" s="65"/>
     </row>
     <row r="106" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A106" s="15" t="e">
@@ -9550,35 +9456,35 @@
       <c r="B106" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="C106" s="65" t="e">
+      <c r="C106" s="64" t="e">
         <f>VLOOKUP($B106&amp;"3",funnel_data!$A:$X,C$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D106" s="65">
+      <c r="D106" s="64">
         <v>1</v>
       </c>
-      <c r="E106" s="65" t="e">
+      <c r="E106" s="64" t="e">
         <f>VLOOKUP($B106&amp;"3",funnel_data!$A:$X,E$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F106" s="65" t="e">
+      <c r="F106" s="64" t="e">
         <f>VLOOKUP($B106&amp;"3",funnel_data!$A:$X,F$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G106" s="65" t="e">
+      <c r="G106" s="64" t="e">
         <f>VLOOKUP($B106&amp;"3",funnel_data!$A:$X,G$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H106" s="65" t="e">
+      <c r="H106" s="64" t="e">
         <f>VLOOKUP($B106&amp;"3",funnel_data!$A:$X,H$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I106" s="65" t="e">
+      <c r="I106" s="64" t="e">
         <f>VLOOKUP($B106&amp;"3",funnel_data!$A:$X,I$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M106" s="66"/>
-      <c r="N106" s="66"/>
+      <c r="M106" s="65"/>
+      <c r="N106" s="65"/>
     </row>
     <row r="107" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A107" s="15" t="e">
@@ -9588,35 +9494,35 @@
       <c r="B107" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="C107" s="65" t="e">
+      <c r="C107" s="64" t="e">
         <f>VLOOKUP($B107&amp;"3",funnel_data!$A:$X,C$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D107" s="65">
+      <c r="D107" s="64">
         <v>1</v>
       </c>
-      <c r="E107" s="65" t="e">
+      <c r="E107" s="64" t="e">
         <f>VLOOKUP($B107&amp;"3",funnel_data!$A:$X,E$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F107" s="65" t="e">
+      <c r="F107" s="64" t="e">
         <f>VLOOKUP($B107&amp;"3",funnel_data!$A:$X,F$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G107" s="65" t="e">
+      <c r="G107" s="64" t="e">
         <f>VLOOKUP($B107&amp;"3",funnel_data!$A:$X,G$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H107" s="65" t="e">
+      <c r="H107" s="64" t="e">
         <f>VLOOKUP($B107&amp;"3",funnel_data!$A:$X,H$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I107" s="65" t="e">
+      <c r="I107" s="64" t="e">
         <f>VLOOKUP($B107&amp;"3",funnel_data!$A:$X,I$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M107" s="66"/>
-      <c r="N107" s="66"/>
+      <c r="M107" s="65"/>
+      <c r="N107" s="65"/>
     </row>
     <row r="108" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A108" s="15" t="e">
@@ -9626,35 +9532,35 @@
       <c r="B108" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="C108" s="65" t="e">
+      <c r="C108" s="64" t="e">
         <f>VLOOKUP($B108&amp;"3",funnel_data!$A:$X,C$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D108" s="65">
+      <c r="D108" s="64">
         <v>1</v>
       </c>
-      <c r="E108" s="65" t="e">
+      <c r="E108" s="64" t="e">
         <f>VLOOKUP($B108&amp;"3",funnel_data!$A:$X,E$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F108" s="65" t="e">
+      <c r="F108" s="64" t="e">
         <f>VLOOKUP($B108&amp;"3",funnel_data!$A:$X,F$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G108" s="65" t="e">
+      <c r="G108" s="64" t="e">
         <f>VLOOKUP($B108&amp;"3",funnel_data!$A:$X,G$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H108" s="65" t="e">
+      <c r="H108" s="64" t="e">
         <f>VLOOKUP($B108&amp;"3",funnel_data!$A:$X,H$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I108" s="65" t="e">
+      <c r="I108" s="64" t="e">
         <f>VLOOKUP($B108&amp;"3",funnel_data!$A:$X,I$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M108" s="66"/>
-      <c r="N108" s="66"/>
+      <c r="M108" s="65"/>
+      <c r="N108" s="65"/>
     </row>
     <row r="109" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A109" s="15" t="e">
@@ -9664,35 +9570,35 @@
       <c r="B109" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C109" s="65" t="e">
+      <c r="C109" s="64" t="e">
         <f>VLOOKUP($B109&amp;"3",funnel_data!$A:$X,C$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D109" s="65">
+      <c r="D109" s="64">
         <v>1</v>
       </c>
-      <c r="E109" s="65" t="e">
+      <c r="E109" s="64" t="e">
         <f>VLOOKUP($B109&amp;"3",funnel_data!$A:$X,E$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F109" s="65" t="e">
+      <c r="F109" s="64" t="e">
         <f>VLOOKUP($B109&amp;"3",funnel_data!$A:$X,F$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G109" s="65" t="e">
+      <c r="G109" s="64" t="e">
         <f>VLOOKUP($B109&amp;"3",funnel_data!$A:$X,G$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H109" s="65" t="e">
+      <c r="H109" s="64" t="e">
         <f>VLOOKUP($B109&amp;"3",funnel_data!$A:$X,H$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I109" s="65" t="e">
+      <c r="I109" s="64" t="e">
         <f>VLOOKUP($B109&amp;"3",funnel_data!$A:$X,I$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M109" s="66"/>
-      <c r="N109" s="66"/>
+      <c r="M109" s="65"/>
+      <c r="N109" s="65"/>
     </row>
     <row r="110" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A110" s="15" t="e">
@@ -9702,35 +9608,35 @@
       <c r="B110" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="C110" s="65" t="e">
+      <c r="C110" s="64" t="e">
         <f>VLOOKUP($B110&amp;"3",funnel_data!$A:$X,C$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D110" s="65">
+      <c r="D110" s="64">
         <v>1</v>
       </c>
-      <c r="E110" s="65" t="e">
+      <c r="E110" s="64" t="e">
         <f>VLOOKUP($B110&amp;"3",funnel_data!$A:$X,E$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F110" s="65" t="e">
+      <c r="F110" s="64" t="e">
         <f>VLOOKUP($B110&amp;"3",funnel_data!$A:$X,F$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G110" s="65" t="e">
+      <c r="G110" s="64" t="e">
         <f>VLOOKUP($B110&amp;"3",funnel_data!$A:$X,G$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H110" s="65" t="e">
+      <c r="H110" s="64" t="e">
         <f>VLOOKUP($B110&amp;"3",funnel_data!$A:$X,H$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I110" s="65" t="e">
+      <c r="I110" s="64" t="e">
         <f>VLOOKUP($B110&amp;"3",funnel_data!$A:$X,I$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M110" s="66"/>
-      <c r="N110" s="66"/>
+      <c r="M110" s="65"/>
+      <c r="N110" s="65"/>
     </row>
     <row r="111" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A111" s="15" t="e">
@@ -9740,30 +9646,30 @@
       <c r="B111" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="C111" s="65" t="e">
+      <c r="C111" s="64" t="e">
         <f>VLOOKUP($B111&amp;"3",funnel_data!$A:$X,C$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D111" s="65">
+      <c r="D111" s="64">
         <v>1</v>
       </c>
-      <c r="E111" s="65" t="e">
+      <c r="E111" s="64" t="e">
         <f>VLOOKUP($B111&amp;"3",funnel_data!$A:$X,E$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F111" s="65" t="e">
+      <c r="F111" s="64" t="e">
         <f>VLOOKUP($B111&amp;"3",funnel_data!$A:$X,F$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G111" s="65" t="e">
+      <c r="G111" s="64" t="e">
         <f>VLOOKUP($B111&amp;"3",funnel_data!$A:$X,G$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H111" s="65" t="e">
+      <c r="H111" s="64" t="e">
         <f>VLOOKUP($B111&amp;"3",funnel_data!$A:$X,H$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I111" s="65" t="e">
+      <c r="I111" s="64" t="e">
         <f>VLOOKUP($B111&amp;"3",funnel_data!$A:$X,I$82,FALSE)</f>
         <v>#N/A</v>
       </c>
@@ -9776,30 +9682,30 @@
       <c r="B112" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="C112" s="65" t="e">
+      <c r="C112" s="64" t="e">
         <f>VLOOKUP($B112&amp;"3",funnel_data!$A:$X,C$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D112" s="65">
+      <c r="D112" s="64">
         <v>1</v>
       </c>
-      <c r="E112" s="65" t="e">
+      <c r="E112" s="64" t="e">
         <f>VLOOKUP($B112&amp;"3",funnel_data!$A:$X,E$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F112" s="65" t="e">
+      <c r="F112" s="64" t="e">
         <f>VLOOKUP($B112&amp;"3",funnel_data!$A:$X,F$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G112" s="65" t="e">
+      <c r="G112" s="64" t="e">
         <f>VLOOKUP($B112&amp;"3",funnel_data!$A:$X,G$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H112" s="65" t="e">
+      <c r="H112" s="64" t="e">
         <f>VLOOKUP($B112&amp;"3",funnel_data!$A:$X,H$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I112" s="65" t="e">
+      <c r="I112" s="64" t="e">
         <f>VLOOKUP($B112&amp;"3",funnel_data!$A:$X,I$82,FALSE)</f>
         <v>#N/A</v>
       </c>
@@ -9812,30 +9718,30 @@
       <c r="B113" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C113" s="65" t="e">
+      <c r="C113" s="64" t="e">
         <f>VLOOKUP($B113&amp;"3",funnel_data!$A:$X,C$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D113" s="65">
+      <c r="D113" s="64">
         <v>1</v>
       </c>
-      <c r="E113" s="65" t="e">
+      <c r="E113" s="64" t="e">
         <f>VLOOKUP($B113&amp;"3",funnel_data!$A:$X,E$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F113" s="65" t="e">
+      <c r="F113" s="64" t="e">
         <f>VLOOKUP($B113&amp;"3",funnel_data!$A:$X,F$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G113" s="65" t="e">
+      <c r="G113" s="64" t="e">
         <f>VLOOKUP($B113&amp;"3",funnel_data!$A:$X,G$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H113" s="65" t="e">
+      <c r="H113" s="64" t="e">
         <f>VLOOKUP($B113&amp;"3",funnel_data!$A:$X,H$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I113" s="65" t="e">
+      <c r="I113" s="64" t="e">
         <f>VLOOKUP($B113&amp;"3",funnel_data!$A:$X,I$82,FALSE)</f>
         <v>#N/A</v>
       </c>
@@ -9848,30 +9754,30 @@
       <c r="B114" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C114" s="65" t="e">
+      <c r="C114" s="64" t="e">
         <f>VLOOKUP($B114&amp;"3",funnel_data!$A:$X,C$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D114" s="65">
+      <c r="D114" s="64">
         <v>1</v>
       </c>
-      <c r="E114" s="65" t="e">
+      <c r="E114" s="64" t="e">
         <f>VLOOKUP($B114&amp;"3",funnel_data!$A:$X,E$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F114" s="65" t="e">
+      <c r="F114" s="64" t="e">
         <f>VLOOKUP($B114&amp;"3",funnel_data!$A:$X,F$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G114" s="65" t="e">
+      <c r="G114" s="64" t="e">
         <f>VLOOKUP($B114&amp;"3",funnel_data!$A:$X,G$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H114" s="65" t="e">
+      <c r="H114" s="64" t="e">
         <f>VLOOKUP($B114&amp;"3",funnel_data!$A:$X,H$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I114" s="65" t="e">
+      <c r="I114" s="64" t="e">
         <f>VLOOKUP($B114&amp;"3",funnel_data!$A:$X,I$82,FALSE)</f>
         <v>#N/A</v>
       </c>
@@ -9884,30 +9790,30 @@
       <c r="B115" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C115" s="65" t="e">
+      <c r="C115" s="64" t="e">
         <f>VLOOKUP($B115&amp;"3",funnel_data!$A:$X,C$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D115" s="65">
+      <c r="D115" s="64">
         <v>1</v>
       </c>
-      <c r="E115" s="65" t="e">
+      <c r="E115" s="64" t="e">
         <f>VLOOKUP($B115&amp;"3",funnel_data!$A:$X,E$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F115" s="65" t="e">
+      <c r="F115" s="64" t="e">
         <f>VLOOKUP($B115&amp;"3",funnel_data!$A:$X,F$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G115" s="65" t="e">
+      <c r="G115" s="64" t="e">
         <f>VLOOKUP($B115&amp;"3",funnel_data!$A:$X,G$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H115" s="65" t="e">
+      <c r="H115" s="64" t="e">
         <f>VLOOKUP($B115&amp;"3",funnel_data!$A:$X,H$82,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I115" s="65" t="e">
+      <c r="I115" s="64" t="e">
         <f>VLOOKUP($B115&amp;"3",funnel_data!$A:$X,I$82,FALSE)</f>
         <v>#N/A</v>
       </c>
@@ -9950,9 +9856,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:R1022"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A1022"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9962,7 +9866,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="O1"/>
     </row>
@@ -17298,10 +17202,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G3" s="5"/>
     </row>
@@ -17370,10 +17274,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G11" s="5"/>
     </row>
@@ -17453,10 +17357,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G20" s="5"/>
     </row>
@@ -17555,7 +17459,7 @@
         <v>9</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G31" s="5"/>
     </row>
@@ -17590,9 +17494,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -17601,8 +17503,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>116</v>
+      <c r="A1">
+        <f>funnel_data!V2</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to Excel Templates
</commit_message>
<xml_diff>
--- a/reference_files/Table1-HSMR.xlsx
+++ b/reference_files/Table1-HSMR.xlsx
@@ -15,8 +15,8 @@
     <sheet name="Table 1" sheetId="49" r:id="rId1"/>
     <sheet name="Chart 1" sheetId="43" r:id="rId2"/>
     <sheet name="funnel_data" sheetId="38" r:id="rId3"/>
-    <sheet name="hosp_lookup" sheetId="51" r:id="rId4"/>
-    <sheet name="period_lookup" sheetId="37" r:id="rId5"/>
+    <sheet name="hosp_lookup" sheetId="51" state="hidden" r:id="rId4"/>
+    <sheet name="period_lookup" sheetId="37" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">funnel_data!$A$1:$S$1022</definedName>
@@ -745,10 +745,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="18" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="23" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="23" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2800,7 +2800,7 @@
         <c:axId val="553192216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="2800"/>
+          <c:max val="3000"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -2843,6 +2843,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2957,6 +2958,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3034,6 +3036,15 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="6"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="7"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4455,19 +4466,19 @@
     <row r="1" spans="1:27" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="47"/>
       <c r="B1" s="8"/>
-      <c r="C1" s="66" t="s">
+      <c r="C1" s="67" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
-      <c r="M1" s="66"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
     </row>
     <row r="2" spans="1:27" s="9" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="47"/>
@@ -4608,7 +4619,7 @@
         <f>VLOOKUP($B11&amp;$A$5,funnel_data!$A:$X,5,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H11" s="67" t="e">
+      <c r="H11" s="66" t="e">
         <f>VLOOKUP($B11&amp;$A$5,funnel_data!$A:$X,7,FALSE)</f>
         <v>#N/A</v>
       </c>
@@ -6140,7 +6151,7 @@
   <dimension ref="A1:AK121"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AQ29" sqref="AQ29"/>
+      <selection activeCell="AL29" sqref="AL29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -6158,19 +6169,19 @@
   <sheetData>
     <row r="1" spans="1:36" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="67" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
     </row>
     <row r="2" spans="1:36" s="9" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
@@ -17494,7 +17505,9 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:IV34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Further edits to excel tables following comments from Lucinda
</commit_message>
<xml_diff>
--- a/reference_files/Table1-HSMR.xlsx
+++ b/reference_files/Table1-HSMR.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="123">
   <si>
     <t>V217H</t>
   </si>
@@ -395,6 +395,9 @@
   </si>
   <si>
     <t>S08000032</t>
+  </si>
+  <si>
+    <t>SMR</t>
   </si>
 </sst>
 </file>
@@ -2039,7 +2042,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>smr</c:v>
+                  <c:v>SMR</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3671,8 +3674,8 @@
     <xdr:to>
       <xdr:col>41</xdr:col>
       <xdr:colOff>425824</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>149036</xdr:rowOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>112059</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3681,8 +3684,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7584701" y="720536"/>
-          <a:ext cx="3856505" cy="2902324"/>
+          <a:off x="7495053" y="720536"/>
+          <a:ext cx="3856506" cy="3470464"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4040,6 +4043,110 @@
             <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
             <a:ea typeface="+mn-ea"/>
             <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1000">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>The table below the chart shows the hospitals as they appear on the chart left to right. Any</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> outliers are highlighted in </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>red</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> (over upper control limit) or </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>orange</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> (over upper warning limit).</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1000">
+            <a:effectLst/>
+            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
           </a:endParaRPr>
         </a:p>
         <a:p>
@@ -4530,7 +4637,7 @@
       <c r="A4" s="47"/>
       <c r="B4" s="8"/>
       <c r="C4" s="14" t="str">
-        <f>"Hospital Standardised Mortality Ratio (Funnel Plot); "&amp;B5</f>
+        <f>"Hospital Standardised Mortality Ratio (Funnel Plot); "</f>
         <v xml:space="preserve">Hospital Standardised Mortality Ratio (Funnel Plot); </v>
       </c>
       <c r="D4" s="28"/>
@@ -6150,9 +6257,7 @@
   </sheetPr>
   <dimension ref="A1:AK121"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AL29" sqref="AL29"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6182,6 +6287,22 @@
       <c r="J1" s="67"/>
       <c r="K1" s="67"/>
       <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="67"/>
+      <c r="R1" s="67"/>
+      <c r="S1" s="67"/>
+      <c r="T1" s="67"/>
+      <c r="U1" s="67"/>
+      <c r="V1" s="67"/>
+      <c r="W1" s="67"/>
+      <c r="X1" s="67"/>
+      <c r="Y1" s="67"/>
+      <c r="Z1" s="67"/>
+      <c r="AA1" s="67"/>
+      <c r="AB1" s="67"/>
     </row>
     <row r="2" spans="1:36" s="9" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
@@ -6580,7 +6701,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="34" spans="1:37" s="18" customFormat="1" ht="240.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:37" s="18" customFormat="1" ht="186" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C34" s="20" t="e">
         <f>VLOOKUP(VLOOKUP(C$32,$A$49:$B$80,2,FALSE),hosp_lookup!$A:$B,2,FALSE)</f>
         <v>#N/A</v>
@@ -6826,7 +6947,7 @@
         <v>59</v>
       </c>
       <c r="E48" s="51" t="s">
-        <v>53</v>
+        <v>122</v>
       </c>
       <c r="F48" s="51" t="s">
         <v>55</v>
@@ -9837,7 +9958,7 @@
     <row r="121" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:L1"/>
+    <mergeCell ref="B1:AB1"/>
   </mergeCells>
   <conditionalFormatting sqref="C33:AH33">
     <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
Revert "Further edits to excel tables following comments from Lucinda"
</commit_message>
<xml_diff>
--- a/reference_files/Table1-HSMR.xlsx
+++ b/reference_files/Table1-HSMR.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="122">
   <si>
     <t>V217H</t>
   </si>
@@ -395,9 +395,6 @@
   </si>
   <si>
     <t>S08000032</t>
-  </si>
-  <si>
-    <t>SMR</t>
   </si>
 </sst>
 </file>
@@ -2042,7 +2039,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>SMR</c:v>
+                  <c:v>smr</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3674,8 +3671,8 @@
     <xdr:to>
       <xdr:col>41</xdr:col>
       <xdr:colOff>425824</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>112059</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>149036</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3684,8 +3681,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7495053" y="720536"/>
-          <a:ext cx="3856506" cy="3470464"/>
+          <a:off x="7584701" y="720536"/>
+          <a:ext cx="3856505" cy="2902324"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4043,110 +4040,6 @@
             <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
             <a:ea typeface="+mn-ea"/>
             <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1000">
-            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>The table below the chart shows the hospitals as they appear on the chart left to right. Any</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> outliers are highlighted in </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="1" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="C00000"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>red</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> (over upper control limit) or </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="1" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>orange</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> (over upper warning limit).</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-GB" sz="1000">
-            <a:effectLst/>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
           </a:endParaRPr>
         </a:p>
         <a:p>
@@ -4637,7 +4530,7 @@
       <c r="A4" s="47"/>
       <c r="B4" s="8"/>
       <c r="C4" s="14" t="str">
-        <f>"Hospital Standardised Mortality Ratio (Funnel Plot); "</f>
+        <f>"Hospital Standardised Mortality Ratio (Funnel Plot); "&amp;B5</f>
         <v xml:space="preserve">Hospital Standardised Mortality Ratio (Funnel Plot); </v>
       </c>
       <c r="D4" s="28"/>
@@ -6257,7 +6150,9 @@
   </sheetPr>
   <dimension ref="A1:AK121"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AL29" sqref="AL29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6287,22 +6182,6 @@
       <c r="J1" s="67"/>
       <c r="K1" s="67"/>
       <c r="L1" s="67"/>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67"/>
-      <c r="P1" s="67"/>
-      <c r="Q1" s="67"/>
-      <c r="R1" s="67"/>
-      <c r="S1" s="67"/>
-      <c r="T1" s="67"/>
-      <c r="U1" s="67"/>
-      <c r="V1" s="67"/>
-      <c r="W1" s="67"/>
-      <c r="X1" s="67"/>
-      <c r="Y1" s="67"/>
-      <c r="Z1" s="67"/>
-      <c r="AA1" s="67"/>
-      <c r="AB1" s="67"/>
     </row>
     <row r="2" spans="1:36" s="9" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
@@ -6701,7 +6580,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="34" spans="1:37" s="18" customFormat="1" ht="186" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:37" s="18" customFormat="1" ht="240.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C34" s="20" t="e">
         <f>VLOOKUP(VLOOKUP(C$32,$A$49:$B$80,2,FALSE),hosp_lookup!$A:$B,2,FALSE)</f>
         <v>#N/A</v>
@@ -6947,7 +6826,7 @@
         <v>59</v>
       </c>
       <c r="E48" s="51" t="s">
-        <v>122</v>
+        <v>53</v>
       </c>
       <c r="F48" s="51" t="s">
         <v>55</v>
@@ -9958,7 +9837,7 @@
     <row r="121" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:AB1"/>
+    <mergeCell ref="B1:L1"/>
   </mergeCells>
   <conditionalFormatting sqref="C33:AH33">
     <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
Final Edits to Table 1 and 2
</commit_message>
<xml_diff>
--- a/reference_files/Table1-HSMR.xlsx
+++ b/reference_files/Table1-HSMR.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="123">
   <si>
     <t>V217H</t>
   </si>
@@ -396,6 +396,9 @@
   <si>
     <t>S08000032</t>
   </si>
+  <si>
+    <t>SMR</t>
+  </si>
 </sst>
 </file>
 
@@ -639,7 +642,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -749,6 +752,7 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2039,7 +2043,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>smr</c:v>
+                  <c:v>SMR</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3666,13 +3670,13 @@
       <xdr:col>32</xdr:col>
       <xdr:colOff>110377</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>182654</xdr:rowOff>
+      <xdr:rowOff>182653</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>41</xdr:col>
       <xdr:colOff>425824</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>149036</xdr:rowOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>56029</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3681,8 +3685,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7584701" y="720536"/>
-          <a:ext cx="3856505" cy="2902324"/>
+          <a:off x="7495053" y="720535"/>
+          <a:ext cx="3856506" cy="3560112"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4033,7 +4037,110 @@
             </a:rPr>
             <a:t>A single apparently high value of the HSMR is not sufficient evidence on which to conclude that a poor quality or unsafe service is being provided. This is why it is important not to focus solely on 'outliers' when making reliable judgements about the quality of patient care.</a:t>
           </a:r>
-          <a:endParaRPr lang="en-GB" sz="1000" b="1" i="1">
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="1000" b="1" i="1" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>The table below the chart lists the hopsitals as presented left to right on the chart. Outlier are highlighted in </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="1" i="0" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>red</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> (above upper control limit) and </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="1" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>orange</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1000" b="0" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> (above upper warning limit).</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1000" b="0" i="0">
             <a:solidFill>
               <a:schemeClr val="dk1"/>
             </a:solidFill>
@@ -6151,7 +6258,7 @@
   <dimension ref="A1:AK121"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AL29" sqref="AL29"/>
+      <selection activeCell="AS19" sqref="AS19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -6182,6 +6289,22 @@
       <c r="J1" s="67"/>
       <c r="K1" s="67"/>
       <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="67"/>
+      <c r="R1" s="67"/>
+      <c r="S1" s="67"/>
+      <c r="T1" s="67"/>
+      <c r="U1" s="67"/>
+      <c r="V1" s="67"/>
+      <c r="W1" s="67"/>
+      <c r="X1" s="67"/>
+      <c r="Y1" s="67"/>
+      <c r="Z1" s="67"/>
+      <c r="AA1" s="67"/>
+      <c r="AB1" s="67"/>
     </row>
     <row r="2" spans="1:36" s="9" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
@@ -6580,7 +6703,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="34" spans="1:37" s="18" customFormat="1" ht="240.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:37" s="18" customFormat="1" ht="186" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C34" s="20" t="e">
         <f>VLOOKUP(VLOOKUP(C$32,$A$49:$B$80,2,FALSE),hosp_lookup!$A:$B,2,FALSE)</f>
         <v>#N/A</v>
@@ -6810,6 +6933,7 @@
       <c r="I47" s="50">
         <v>9</v>
       </c>
+      <c r="P47" s="18"/>
       <c r="Q47" s="50"/>
       <c r="S47" s="50"/>
       <c r="U47" s="50"/>
@@ -6826,7 +6950,7 @@
         <v>59</v>
       </c>
       <c r="E48" s="51" t="s">
-        <v>53</v>
+        <v>122</v>
       </c>
       <c r="F48" s="51" t="s">
         <v>55</v>
@@ -6849,7 +6973,7 @@
       <c r="L48" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="P48" s="45"/>
+      <c r="P48" s="68"/>
       <c r="Q48" s="51"/>
       <c r="R48" s="51"/>
       <c r="S48" s="51"/>
@@ -6906,7 +7030,7 @@
         <f>IF(J49=2,E49,#N/A)</f>
         <v>#N/A</v>
       </c>
-      <c r="P49" s="45"/>
+      <c r="P49" s="68"/>
       <c r="Q49" s="52"/>
       <c r="R49" s="53"/>
       <c r="S49" s="53"/>
@@ -9837,7 +9961,7 @@
     <row r="121" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:L1"/>
+    <mergeCell ref="B1:AB1"/>
   </mergeCells>
   <conditionalFormatting sqref="C33:AH33">
     <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
change ISD to PHS
</commit_message>
<xml_diff>
--- a/reference_files/Table1-HSMR.xlsx
+++ b/reference_files/Table1-HSMR.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Isdsf00d03\quality_indicators\hsmr\quarter_cycle\Robyn\reference_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\stats\quality_indicators\hsmr\quarter_cycle\Sam2\reference_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -753,9 +753,6 @@
     <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -780,6 +777,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="18" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4538,7 +4538,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AA83"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4552,19 +4554,19 @@
     <row r="1" spans="1:27" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="47"/>
       <c r="B1" s="8"/>
-      <c r="C1" s="65" t="s">
+      <c r="C1" s="75" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="75"/>
     </row>
     <row r="2" spans="1:27" s="9" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="47"/>
@@ -6152,8 +6154,8 @@
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B60" s="30"/>
       <c r="C60" s="1" t="str">
-        <f>"Source: ISD Scotland (SMR01) linked dataset. Reflects the completeness of SMR01 submissions to ISD for individual hospitals as of " &amp; TEXT(funnel_data!L2,"dd mmm yyyy")</f>
-        <v>Source: ISD Scotland (SMR01) linked dataset. Reflects the completeness of SMR01 submissions to ISD for individual hospitals as of 00 Jan 1900</v>
+        <f>"Source: PHS (SMR01) linked dataset. Reflects the completeness of SMR01 submissions to PHS for individual hospitals as of " &amp; TEXT(funnel_data!L2,"dd mmm yyyy")</f>
+        <v>Source: PHS (SMR01) linked dataset. Reflects the completeness of SMR01 submissions to PHS for individual hospitals as of 00 Jan 1900</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -6205,7 +6207,9 @@
   </sheetPr>
   <dimension ref="A1:AK119"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AV34" sqref="AV34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6222,35 +6226,35 @@
   <sheetData>
     <row r="1" spans="1:36" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="75" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
-      <c r="S1" s="65"/>
-      <c r="T1" s="65"/>
-      <c r="U1" s="65"/>
-      <c r="V1" s="65"/>
-      <c r="W1" s="65"/>
-      <c r="X1" s="65"/>
-      <c r="Y1" s="65"/>
-      <c r="Z1" s="65"/>
-      <c r="AA1" s="65"/>
-      <c r="AB1" s="65"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="75"/>
+      <c r="N1" s="75"/>
+      <c r="O1" s="75"/>
+      <c r="P1" s="75"/>
+      <c r="Q1" s="75"/>
+      <c r="R1" s="75"/>
+      <c r="S1" s="75"/>
+      <c r="T1" s="75"/>
+      <c r="U1" s="75"/>
+      <c r="V1" s="75"/>
+      <c r="W1" s="75"/>
+      <c r="X1" s="75"/>
+      <c r="Y1" s="75"/>
+      <c r="Z1" s="75"/>
+      <c r="AA1" s="75"/>
+      <c r="AB1" s="75"/>
     </row>
     <row r="2" spans="1:36" s="9" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
@@ -6780,8 +6784,8 @@
     <row r="36" spans="1:37" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="1" t="str">
-        <f>"Source: ISD Scotland (SMR01) linked dataset. Reflects the completeness of SMR01 submissions to ISD for individual hospitals as of " &amp; TEXT(funnel_data!L2,"dd mmm yyyy")</f>
-        <v>Source: ISD Scotland (SMR01) linked dataset. Reflects the completeness of SMR01 submissions to ISD for individual hospitals as of 00 Jan 1900</v>
+        <f>"Source: PHS Scotland (SMR01) linked dataset. Reflects the completeness of SMR01 submissions to PHS for individual hospitals as of " &amp; TEXT(funnel_data!L2,"dd mmm yyyy")</f>
+        <v>Source: PHS Scotland (SMR01) linked dataset. Reflects the completeness of SMR01 submissions to PHS for individual hospitals as of 00 Jan 1900</v>
       </c>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
@@ -6853,55 +6857,55 @@
       <c r="B47" s="15">
         <v>2</v>
       </c>
-      <c r="C47" s="66">
+      <c r="C47" s="65">
         <v>3</v>
       </c>
       <c r="D47" s="15">
         <v>4</v>
       </c>
-      <c r="E47" s="66">
+      <c r="E47" s="65">
         <v>5</v>
       </c>
       <c r="F47" s="15">
         <v>6</v>
       </c>
-      <c r="G47" s="66">
+      <c r="G47" s="65">
         <v>7</v>
       </c>
       <c r="H47" s="15">
         <v>8</v>
       </c>
-      <c r="I47" s="66">
+      <c r="I47" s="65">
         <v>9</v>
       </c>
-      <c r="Q47" s="66"/>
-      <c r="S47" s="66"/>
-      <c r="U47" s="66"/>
-      <c r="W47" s="66"/>
+      <c r="Q47" s="65"/>
+      <c r="S47" s="65"/>
+      <c r="U47" s="65"/>
+      <c r="W47" s="65"/>
     </row>
     <row r="48" spans="1:37" s="15" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B48" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="C48" s="67" t="s">
+      <c r="C48" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="D48" s="67" t="s">
+      <c r="D48" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="E48" s="67" t="s">
+      <c r="E48" s="66" t="s">
         <v>118</v>
       </c>
-      <c r="F48" s="67" t="s">
+      <c r="F48" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="G48" s="67" t="s">
+      <c r="G48" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="H48" s="67" t="s">
+      <c r="H48" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="I48" s="67" t="s">
+      <c r="I48" s="66" t="s">
         <v>56</v>
       </c>
       <c r="J48" s="15" t="s">
@@ -6914,13 +6918,13 @@
         <v>64</v>
       </c>
       <c r="P48" s="45"/>
-      <c r="Q48" s="67"/>
-      <c r="R48" s="67"/>
-      <c r="S48" s="67"/>
-      <c r="T48" s="67"/>
-      <c r="U48" s="67"/>
-      <c r="V48" s="67"/>
-      <c r="W48" s="67"/>
+      <c r="Q48" s="66"/>
+      <c r="R48" s="66"/>
+      <c r="S48" s="66"/>
+      <c r="T48" s="66"/>
+      <c r="U48" s="66"/>
+      <c r="V48" s="66"/>
+      <c r="W48" s="66"/>
     </row>
     <row r="49" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="15">
@@ -6930,31 +6934,31 @@
         <f t="shared" ref="B49:I58" si="1">VLOOKUP($A49,$A$83:$I$113,B$47,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="C49" s="68" t="e">
+      <c r="C49" s="67" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="D49" s="69" t="e">
+      <c r="D49" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="E49" s="69" t="e">
+      <c r="E49" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="F49" s="69" t="e">
+      <c r="F49" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="G49" s="69" t="e">
+      <c r="G49" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="H49" s="69" t="e">
+      <c r="H49" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="I49" s="69" t="e">
+      <c r="I49" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
@@ -6971,13 +6975,13 @@
         <v>#N/A</v>
       </c>
       <c r="P49" s="45"/>
-      <c r="Q49" s="68"/>
-      <c r="R49" s="69"/>
-      <c r="S49" s="69"/>
-      <c r="T49" s="69"/>
-      <c r="U49" s="69"/>
-      <c r="V49" s="69"/>
-      <c r="W49" s="69"/>
+      <c r="Q49" s="67"/>
+      <c r="R49" s="68"/>
+      <c r="S49" s="68"/>
+      <c r="T49" s="68"/>
+      <c r="U49" s="68"/>
+      <c r="V49" s="68"/>
+      <c r="W49" s="68"/>
     </row>
     <row r="50" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="15">
@@ -6987,31 +6991,31 @@
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="C50" s="68" t="e">
+      <c r="C50" s="67" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="D50" s="69" t="e">
+      <c r="D50" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="E50" s="69" t="e">
+      <c r="E50" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="F50" s="69" t="e">
+      <c r="F50" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="G50" s="69" t="e">
+      <c r="G50" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="H50" s="69" t="e">
+      <c r="H50" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="I50" s="69" t="e">
+      <c r="I50" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
@@ -7028,13 +7032,13 @@
         <v>#N/A</v>
       </c>
       <c r="P50" s="45"/>
-      <c r="Q50" s="68"/>
-      <c r="R50" s="69"/>
-      <c r="S50" s="69"/>
-      <c r="T50" s="69"/>
-      <c r="U50" s="69"/>
-      <c r="V50" s="69"/>
-      <c r="W50" s="69"/>
+      <c r="Q50" s="67"/>
+      <c r="R50" s="68"/>
+      <c r="S50" s="68"/>
+      <c r="T50" s="68"/>
+      <c r="U50" s="68"/>
+      <c r="V50" s="68"/>
+      <c r="W50" s="68"/>
     </row>
     <row r="51" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="15">
@@ -7044,31 +7048,31 @@
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="C51" s="68" t="e">
+      <c r="C51" s="67" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="D51" s="69" t="e">
+      <c r="D51" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="E51" s="69" t="e">
+      <c r="E51" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="F51" s="69" t="e">
+      <c r="F51" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="G51" s="69" t="e">
+      <c r="G51" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="H51" s="69" t="e">
+      <c r="H51" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="I51" s="69" t="e">
+      <c r="I51" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
@@ -7085,13 +7089,13 @@
         <v>#N/A</v>
       </c>
       <c r="P51" s="45"/>
-      <c r="Q51" s="68"/>
-      <c r="R51" s="69"/>
-      <c r="S51" s="69"/>
-      <c r="T51" s="69"/>
-      <c r="U51" s="69"/>
-      <c r="V51" s="69"/>
-      <c r="W51" s="69"/>
+      <c r="Q51" s="67"/>
+      <c r="R51" s="68"/>
+      <c r="S51" s="68"/>
+      <c r="T51" s="68"/>
+      <c r="U51" s="68"/>
+      <c r="V51" s="68"/>
+      <c r="W51" s="68"/>
     </row>
     <row r="52" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="15">
@@ -7101,31 +7105,31 @@
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="C52" s="68" t="e">
+      <c r="C52" s="67" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="D52" s="69" t="e">
+      <c r="D52" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="E52" s="69" t="e">
+      <c r="E52" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="F52" s="69" t="e">
+      <c r="F52" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="G52" s="69" t="e">
+      <c r="G52" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="H52" s="69" t="e">
+      <c r="H52" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="I52" s="69" t="e">
+      <c r="I52" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
@@ -7142,13 +7146,13 @@
         <v>#N/A</v>
       </c>
       <c r="P52" s="45"/>
-      <c r="Q52" s="68"/>
-      <c r="R52" s="69"/>
-      <c r="S52" s="69"/>
-      <c r="T52" s="69"/>
-      <c r="U52" s="69"/>
-      <c r="V52" s="69"/>
-      <c r="W52" s="69"/>
+      <c r="Q52" s="67"/>
+      <c r="R52" s="68"/>
+      <c r="S52" s="68"/>
+      <c r="T52" s="68"/>
+      <c r="U52" s="68"/>
+      <c r="V52" s="68"/>
+      <c r="W52" s="68"/>
     </row>
     <row r="53" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="15">
@@ -7158,31 +7162,31 @@
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="C53" s="68" t="e">
+      <c r="C53" s="67" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="D53" s="69" t="e">
+      <c r="D53" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="E53" s="69" t="e">
+      <c r="E53" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="F53" s="69" t="e">
+      <c r="F53" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="G53" s="69" t="e">
+      <c r="G53" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="H53" s="69" t="e">
+      <c r="H53" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="I53" s="69" t="e">
+      <c r="I53" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
@@ -7199,13 +7203,13 @@
         <v>#N/A</v>
       </c>
       <c r="P53" s="45"/>
-      <c r="Q53" s="68"/>
-      <c r="R53" s="69"/>
-      <c r="S53" s="69"/>
-      <c r="T53" s="69"/>
-      <c r="U53" s="69"/>
-      <c r="V53" s="69"/>
-      <c r="W53" s="69"/>
+      <c r="Q53" s="67"/>
+      <c r="R53" s="68"/>
+      <c r="S53" s="68"/>
+      <c r="T53" s="68"/>
+      <c r="U53" s="68"/>
+      <c r="V53" s="68"/>
+      <c r="W53" s="68"/>
     </row>
     <row r="54" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="15">
@@ -7215,31 +7219,31 @@
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="C54" s="68" t="e">
+      <c r="C54" s="67" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="D54" s="69" t="e">
+      <c r="D54" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="E54" s="69" t="e">
+      <c r="E54" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="F54" s="69" t="e">
+      <c r="F54" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="G54" s="69" t="e">
+      <c r="G54" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="H54" s="69" t="e">
+      <c r="H54" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="I54" s="69" t="e">
+      <c r="I54" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
@@ -7256,13 +7260,13 @@
         <v>#N/A</v>
       </c>
       <c r="P54" s="45"/>
-      <c r="Q54" s="68"/>
-      <c r="R54" s="69"/>
-      <c r="S54" s="69"/>
-      <c r="T54" s="69"/>
-      <c r="U54" s="69"/>
-      <c r="V54" s="69"/>
-      <c r="W54" s="69"/>
+      <c r="Q54" s="67"/>
+      <c r="R54" s="68"/>
+      <c r="S54" s="68"/>
+      <c r="T54" s="68"/>
+      <c r="U54" s="68"/>
+      <c r="V54" s="68"/>
+      <c r="W54" s="68"/>
     </row>
     <row r="55" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="15">
@@ -7272,31 +7276,31 @@
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="C55" s="68" t="e">
+      <c r="C55" s="67" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="D55" s="69" t="e">
+      <c r="D55" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="E55" s="69" t="e">
+      <c r="E55" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="F55" s="69" t="e">
+      <c r="F55" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="G55" s="69" t="e">
+      <c r="G55" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="H55" s="69" t="e">
+      <c r="H55" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="I55" s="69" t="e">
+      <c r="I55" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
@@ -7313,13 +7317,13 @@
         <v>#N/A</v>
       </c>
       <c r="P55" s="45"/>
-      <c r="Q55" s="68"/>
-      <c r="R55" s="69"/>
-      <c r="S55" s="69"/>
-      <c r="T55" s="69"/>
-      <c r="U55" s="69"/>
-      <c r="V55" s="69"/>
-      <c r="W55" s="69"/>
+      <c r="Q55" s="67"/>
+      <c r="R55" s="68"/>
+      <c r="S55" s="68"/>
+      <c r="T55" s="68"/>
+      <c r="U55" s="68"/>
+      <c r="V55" s="68"/>
+      <c r="W55" s="68"/>
     </row>
     <row r="56" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="15">
@@ -7329,31 +7333,31 @@
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="C56" s="68" t="e">
+      <c r="C56" s="67" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="D56" s="69" t="e">
+      <c r="D56" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="E56" s="69" t="e">
+      <c r="E56" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="F56" s="69" t="e">
+      <c r="F56" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="G56" s="69" t="e">
+      <c r="G56" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="H56" s="69" t="e">
+      <c r="H56" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="I56" s="69" t="e">
+      <c r="I56" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
@@ -7370,13 +7374,13 @@
         <v>#N/A</v>
       </c>
       <c r="P56" s="45"/>
-      <c r="Q56" s="68"/>
-      <c r="R56" s="69"/>
-      <c r="S56" s="69"/>
-      <c r="T56" s="69"/>
-      <c r="U56" s="69"/>
-      <c r="V56" s="69"/>
-      <c r="W56" s="69"/>
+      <c r="Q56" s="67"/>
+      <c r="R56" s="68"/>
+      <c r="S56" s="68"/>
+      <c r="T56" s="68"/>
+      <c r="U56" s="68"/>
+      <c r="V56" s="68"/>
+      <c r="W56" s="68"/>
     </row>
     <row r="57" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="15">
@@ -7386,31 +7390,31 @@
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="C57" s="68" t="e">
+      <c r="C57" s="67" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="D57" s="69" t="e">
+      <c r="D57" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="E57" s="69" t="e">
+      <c r="E57" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="F57" s="69" t="e">
+      <c r="F57" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="G57" s="69" t="e">
+      <c r="G57" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="H57" s="69" t="e">
+      <c r="H57" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="I57" s="69" t="e">
+      <c r="I57" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
@@ -7427,13 +7431,13 @@
         <v>#N/A</v>
       </c>
       <c r="P57" s="45"/>
-      <c r="Q57" s="68"/>
-      <c r="R57" s="69"/>
-      <c r="S57" s="69"/>
-      <c r="T57" s="69"/>
-      <c r="U57" s="69"/>
-      <c r="V57" s="69"/>
-      <c r="W57" s="69"/>
+      <c r="Q57" s="67"/>
+      <c r="R57" s="68"/>
+      <c r="S57" s="68"/>
+      <c r="T57" s="68"/>
+      <c r="U57" s="68"/>
+      <c r="V57" s="68"/>
+      <c r="W57" s="68"/>
     </row>
     <row r="58" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="15">
@@ -7443,31 +7447,31 @@
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="C58" s="68" t="e">
+      <c r="C58" s="67" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="D58" s="69" t="e">
+      <c r="D58" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="E58" s="69" t="e">
+      <c r="E58" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="F58" s="69" t="e">
+      <c r="F58" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="G58" s="69" t="e">
+      <c r="G58" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="H58" s="69" t="e">
+      <c r="H58" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="I58" s="69" t="e">
+      <c r="I58" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
@@ -7484,13 +7488,13 @@
         <v>#N/A</v>
       </c>
       <c r="P58" s="45"/>
-      <c r="Q58" s="68"/>
-      <c r="R58" s="69"/>
-      <c r="S58" s="69"/>
-      <c r="T58" s="69"/>
-      <c r="U58" s="69"/>
-      <c r="V58" s="69"/>
-      <c r="W58" s="69"/>
+      <c r="Q58" s="67"/>
+      <c r="R58" s="68"/>
+      <c r="S58" s="68"/>
+      <c r="T58" s="68"/>
+      <c r="U58" s="68"/>
+      <c r="V58" s="68"/>
+      <c r="W58" s="68"/>
     </row>
     <row r="59" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="15">
@@ -7500,31 +7504,31 @@
         <f t="shared" ref="B59:I68" si="5">VLOOKUP($A59,$A$83:$I$113,B$47,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="C59" s="68" t="e">
+      <c r="C59" s="67" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="D59" s="69" t="e">
+      <c r="D59" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="E59" s="69" t="e">
+      <c r="E59" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="F59" s="69" t="e">
+      <c r="F59" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="G59" s="69" t="e">
+      <c r="G59" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="H59" s="69" t="e">
+      <c r="H59" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="I59" s="69" t="e">
+      <c r="I59" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
@@ -7541,13 +7545,13 @@
         <v>#N/A</v>
       </c>
       <c r="P59" s="45"/>
-      <c r="Q59" s="68"/>
-      <c r="R59" s="69"/>
-      <c r="S59" s="69"/>
-      <c r="T59" s="69"/>
-      <c r="U59" s="69"/>
-      <c r="V59" s="69"/>
-      <c r="W59" s="69"/>
+      <c r="Q59" s="67"/>
+      <c r="R59" s="68"/>
+      <c r="S59" s="68"/>
+      <c r="T59" s="68"/>
+      <c r="U59" s="68"/>
+      <c r="V59" s="68"/>
+      <c r="W59" s="68"/>
     </row>
     <row r="60" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="15">
@@ -7557,31 +7561,31 @@
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="C60" s="68" t="e">
+      <c r="C60" s="67" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="D60" s="69" t="e">
+      <c r="D60" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="E60" s="69" t="e">
+      <c r="E60" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="F60" s="69" t="e">
+      <c r="F60" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="G60" s="69" t="e">
+      <c r="G60" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="H60" s="69" t="e">
+      <c r="H60" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="I60" s="69" t="e">
+      <c r="I60" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
@@ -7598,13 +7602,13 @@
         <v>#N/A</v>
       </c>
       <c r="P60" s="45"/>
-      <c r="Q60" s="68"/>
-      <c r="R60" s="69"/>
-      <c r="S60" s="69"/>
-      <c r="T60" s="69"/>
-      <c r="U60" s="69"/>
-      <c r="V60" s="69"/>
-      <c r="W60" s="69"/>
+      <c r="Q60" s="67"/>
+      <c r="R60" s="68"/>
+      <c r="S60" s="68"/>
+      <c r="T60" s="68"/>
+      <c r="U60" s="68"/>
+      <c r="V60" s="68"/>
+      <c r="W60" s="68"/>
     </row>
     <row r="61" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="15">
@@ -7614,31 +7618,31 @@
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="C61" s="68" t="e">
+      <c r="C61" s="67" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="D61" s="69" t="e">
+      <c r="D61" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="E61" s="69" t="e">
+      <c r="E61" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="F61" s="69" t="e">
+      <c r="F61" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="G61" s="69" t="e">
+      <c r="G61" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="H61" s="69" t="e">
+      <c r="H61" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="I61" s="69" t="e">
+      <c r="I61" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
@@ -7655,13 +7659,13 @@
         <v>#N/A</v>
       </c>
       <c r="P61" s="45"/>
-      <c r="Q61" s="68"/>
-      <c r="R61" s="69"/>
-      <c r="S61" s="69"/>
-      <c r="T61" s="69"/>
-      <c r="U61" s="69"/>
-      <c r="V61" s="69"/>
-      <c r="W61" s="69"/>
+      <c r="Q61" s="67"/>
+      <c r="R61" s="68"/>
+      <c r="S61" s="68"/>
+      <c r="T61" s="68"/>
+      <c r="U61" s="68"/>
+      <c r="V61" s="68"/>
+      <c r="W61" s="68"/>
     </row>
     <row r="62" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="15">
@@ -7671,31 +7675,31 @@
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="C62" s="68" t="e">
+      <c r="C62" s="67" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="D62" s="69" t="e">
+      <c r="D62" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="E62" s="69" t="e">
+      <c r="E62" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="F62" s="69" t="e">
+      <c r="F62" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="G62" s="69" t="e">
+      <c r="G62" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="H62" s="69" t="e">
+      <c r="H62" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="I62" s="69" t="e">
+      <c r="I62" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
@@ -7712,13 +7716,13 @@
         <v>#N/A</v>
       </c>
       <c r="P62" s="45"/>
-      <c r="Q62" s="68"/>
-      <c r="R62" s="69"/>
-      <c r="S62" s="69"/>
-      <c r="T62" s="69"/>
-      <c r="U62" s="69"/>
-      <c r="V62" s="69"/>
-      <c r="W62" s="69"/>
+      <c r="Q62" s="67"/>
+      <c r="R62" s="68"/>
+      <c r="S62" s="68"/>
+      <c r="T62" s="68"/>
+      <c r="U62" s="68"/>
+      <c r="V62" s="68"/>
+      <c r="W62" s="68"/>
     </row>
     <row r="63" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="15">
@@ -7728,31 +7732,31 @@
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="C63" s="68" t="e">
+      <c r="C63" s="67" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="D63" s="69" t="e">
+      <c r="D63" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="E63" s="69" t="e">
+      <c r="E63" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="F63" s="69" t="e">
+      <c r="F63" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="G63" s="69" t="e">
+      <c r="G63" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="H63" s="69" t="e">
+      <c r="H63" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="I63" s="69" t="e">
+      <c r="I63" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
@@ -7769,13 +7773,13 @@
         <v>#N/A</v>
       </c>
       <c r="P63" s="45"/>
-      <c r="Q63" s="68"/>
-      <c r="R63" s="69"/>
-      <c r="S63" s="69"/>
-      <c r="T63" s="69"/>
-      <c r="U63" s="69"/>
-      <c r="V63" s="69"/>
-      <c r="W63" s="69"/>
+      <c r="Q63" s="67"/>
+      <c r="R63" s="68"/>
+      <c r="S63" s="68"/>
+      <c r="T63" s="68"/>
+      <c r="U63" s="68"/>
+      <c r="V63" s="68"/>
+      <c r="W63" s="68"/>
     </row>
     <row r="64" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="15">
@@ -7785,31 +7789,31 @@
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="C64" s="68" t="e">
+      <c r="C64" s="67" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="D64" s="69" t="e">
+      <c r="D64" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="E64" s="69" t="e">
+      <c r="E64" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="F64" s="69" t="e">
+      <c r="F64" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="G64" s="69" t="e">
+      <c r="G64" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="H64" s="69" t="e">
+      <c r="H64" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="I64" s="69" t="e">
+      <c r="I64" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
@@ -7834,31 +7838,31 @@
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="C65" s="68" t="e">
+      <c r="C65" s="67" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="D65" s="69" t="e">
+      <c r="D65" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="E65" s="69" t="e">
+      <c r="E65" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="F65" s="69" t="e">
+      <c r="F65" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="G65" s="69" t="e">
+      <c r="G65" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="H65" s="69" t="e">
+      <c r="H65" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="I65" s="69" t="e">
+      <c r="I65" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
@@ -7883,31 +7887,31 @@
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="C66" s="68" t="e">
+      <c r="C66" s="67" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="D66" s="69" t="e">
+      <c r="D66" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="E66" s="69" t="e">
+      <c r="E66" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="F66" s="69" t="e">
+      <c r="F66" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="G66" s="69" t="e">
+      <c r="G66" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="H66" s="69" t="e">
+      <c r="H66" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="I66" s="69" t="e">
+      <c r="I66" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
@@ -7932,31 +7936,31 @@
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="C67" s="68" t="e">
+      <c r="C67" s="67" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="D67" s="69" t="e">
+      <c r="D67" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="E67" s="69" t="e">
+      <c r="E67" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="F67" s="69" t="e">
+      <c r="F67" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="G67" s="69" t="e">
+      <c r="G67" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="H67" s="69" t="e">
+      <c r="H67" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="I67" s="69" t="e">
+      <c r="I67" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
@@ -7981,31 +7985,31 @@
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="C68" s="68" t="e">
+      <c r="C68" s="67" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="D68" s="69" t="e">
+      <c r="D68" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="E68" s="69" t="e">
+      <c r="E68" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="F68" s="69" t="e">
+      <c r="F68" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="G68" s="69" t="e">
+      <c r="G68" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="H68" s="69" t="e">
+      <c r="H68" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="I68" s="69" t="e">
+      <c r="I68" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
@@ -8030,31 +8034,31 @@
         <f t="shared" ref="B69:I79" si="6">VLOOKUP($A69,$A$83:$I$113,B$47,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="C69" s="68" t="e">
+      <c r="C69" s="67" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="D69" s="69" t="e">
+      <c r="D69" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="E69" s="69" t="e">
+      <c r="E69" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="F69" s="69" t="e">
+      <c r="F69" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="G69" s="69" t="e">
+      <c r="G69" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="H69" s="69" t="e">
+      <c r="H69" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="I69" s="69" t="e">
+      <c r="I69" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
@@ -8079,31 +8083,31 @@
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="C70" s="68" t="e">
+      <c r="C70" s="67" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="D70" s="69" t="e">
+      <c r="D70" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="E70" s="69" t="e">
+      <c r="E70" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="F70" s="69" t="e">
+      <c r="F70" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="G70" s="69" t="e">
+      <c r="G70" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="H70" s="69" t="e">
+      <c r="H70" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="I70" s="69" t="e">
+      <c r="I70" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
@@ -8128,31 +8132,31 @@
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="C71" s="68" t="e">
+      <c r="C71" s="67" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="D71" s="69" t="e">
+      <c r="D71" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="E71" s="69" t="e">
+      <c r="E71" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="F71" s="69" t="e">
+      <c r="F71" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="G71" s="69" t="e">
+      <c r="G71" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="H71" s="69" t="e">
+      <c r="H71" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="I71" s="69" t="e">
+      <c r="I71" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
@@ -8177,31 +8181,31 @@
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="C72" s="68" t="e">
+      <c r="C72" s="67" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="D72" s="69" t="e">
+      <c r="D72" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="E72" s="69" t="e">
+      <c r="E72" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="F72" s="69" t="e">
+      <c r="F72" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="G72" s="69" t="e">
+      <c r="G72" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="H72" s="69" t="e">
+      <c r="H72" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="I72" s="69" t="e">
+      <c r="I72" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
@@ -8226,31 +8230,31 @@
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="C73" s="68" t="e">
+      <c r="C73" s="67" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="D73" s="69" t="e">
+      <c r="D73" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="E73" s="69" t="e">
+      <c r="E73" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="F73" s="69" t="e">
+      <c r="F73" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="G73" s="69" t="e">
+      <c r="G73" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="H73" s="69" t="e">
+      <c r="H73" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="I73" s="69" t="e">
+      <c r="I73" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
@@ -8275,31 +8279,31 @@
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="C74" s="68" t="e">
+      <c r="C74" s="67" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="D74" s="69" t="e">
+      <c r="D74" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="E74" s="69" t="e">
+      <c r="E74" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="F74" s="69" t="e">
+      <c r="F74" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="G74" s="69" t="e">
+      <c r="G74" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="H74" s="69" t="e">
+      <c r="H74" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="I74" s="69" t="e">
+      <c r="I74" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
@@ -8324,31 +8328,31 @@
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="C75" s="68" t="e">
+      <c r="C75" s="67" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="D75" s="69" t="e">
+      <c r="D75" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="E75" s="69" t="e">
+      <c r="E75" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="F75" s="69" t="e">
+      <c r="F75" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="G75" s="69" t="e">
+      <c r="G75" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="H75" s="69" t="e">
+      <c r="H75" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="I75" s="69" t="e">
+      <c r="I75" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
@@ -8373,31 +8377,31 @@
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="C76" s="68" t="e">
+      <c r="C76" s="67" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="D76" s="69" t="e">
+      <c r="D76" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="E76" s="69" t="e">
+      <c r="E76" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="F76" s="69" t="e">
+      <c r="F76" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="G76" s="69" t="e">
+      <c r="G76" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="H76" s="69" t="e">
+      <c r="H76" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="I76" s="69" t="e">
+      <c r="I76" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
@@ -8422,31 +8426,31 @@
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="C77" s="68" t="e">
+      <c r="C77" s="67" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="D77" s="69" t="e">
+      <c r="D77" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="E77" s="69" t="e">
+      <c r="E77" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="F77" s="69" t="e">
+      <c r="F77" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="G77" s="69" t="e">
+      <c r="G77" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="H77" s="69" t="e">
+      <c r="H77" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="I77" s="69" t="e">
+      <c r="I77" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
@@ -8471,31 +8475,31 @@
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="C78" s="68" t="e">
+      <c r="C78" s="67" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="D78" s="69" t="e">
+      <c r="D78" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="E78" s="69" t="e">
+      <c r="E78" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="F78" s="69" t="e">
+      <c r="F78" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="G78" s="69" t="e">
+      <c r="G78" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="H78" s="69" t="e">
+      <c r="H78" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="I78" s="69" t="e">
+      <c r="I78" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
@@ -8520,31 +8524,31 @@
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="C79" s="68" t="e">
+      <c r="C79" s="67" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="D79" s="69" t="e">
+      <c r="D79" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="E79" s="69" t="e">
+      <c r="E79" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="F79" s="69" t="e">
+      <c r="F79" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="G79" s="69" t="e">
+      <c r="G79" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="H79" s="69" t="e">
+      <c r="H79" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="I79" s="69" t="e">
+      <c r="I79" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
@@ -8563,80 +8567,80 @@
     </row>
     <row r="80" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B80" s="45"/>
-      <c r="C80" s="70"/>
-      <c r="D80" s="70"/>
-      <c r="E80" s="70"/>
-      <c r="F80" s="70"/>
-      <c r="G80" s="70"/>
-      <c r="H80" s="70"/>
-      <c r="I80" s="70"/>
+      <c r="C80" s="69"/>
+      <c r="D80" s="69"/>
+      <c r="E80" s="69"/>
+      <c r="F80" s="69"/>
+      <c r="G80" s="69"/>
+      <c r="H80" s="69"/>
+      <c r="I80" s="69"/>
     </row>
     <row r="81" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B81" s="15">
         <v>1</v>
       </c>
-      <c r="C81" s="71">
+      <c r="C81" s="70">
         <v>4</v>
       </c>
-      <c r="D81" s="71">
+      <c r="D81" s="70">
         <v>10</v>
       </c>
-      <c r="E81" s="71">
+      <c r="E81" s="70">
         <v>6</v>
       </c>
-      <c r="F81" s="71">
+      <c r="F81" s="70">
         <v>19</v>
       </c>
-      <c r="G81" s="71">
+      <c r="G81" s="70">
         <v>21</v>
       </c>
-      <c r="H81" s="71">
+      <c r="H81" s="70">
         <v>18</v>
       </c>
-      <c r="I81" s="72">
+      <c r="I81" s="71">
         <v>20</v>
       </c>
-      <c r="Q81" s="66"/>
-      <c r="R81" s="66"/>
-      <c r="S81" s="66"/>
-      <c r="T81" s="66"/>
-      <c r="U81" s="66"/>
-      <c r="V81" s="66"/>
-      <c r="W81" s="73"/>
+      <c r="Q81" s="65"/>
+      <c r="R81" s="65"/>
+      <c r="S81" s="65"/>
+      <c r="T81" s="65"/>
+      <c r="U81" s="65"/>
+      <c r="V81" s="65"/>
+      <c r="W81" s="72"/>
     </row>
     <row r="82" spans="1:23" s="15" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B82" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="C82" s="67" t="s">
+      <c r="C82" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="D82" s="67" t="s">
+      <c r="D82" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="E82" s="67" t="s">
+      <c r="E82" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="F82" s="67" t="s">
+      <c r="F82" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="G82" s="67" t="s">
+      <c r="G82" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="H82" s="67" t="s">
+      <c r="H82" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="I82" s="67" t="s">
+      <c r="I82" s="66" t="s">
         <v>56</v>
       </c>
       <c r="P82" s="45"/>
-      <c r="Q82" s="67"/>
-      <c r="R82" s="67"/>
-      <c r="S82" s="67"/>
-      <c r="T82" s="67"/>
-      <c r="U82" s="67"/>
-      <c r="V82" s="67"/>
-      <c r="W82" s="67"/>
+      <c r="Q82" s="66"/>
+      <c r="R82" s="66"/>
+      <c r="S82" s="66"/>
+      <c r="T82" s="66"/>
+      <c r="U82" s="66"/>
+      <c r="V82" s="66"/>
+      <c r="W82" s="66"/>
     </row>
     <row r="83" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="15" t="e">
@@ -8646,35 +8650,35 @@
       <c r="B83" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C83" s="74" t="e">
+      <c r="C83" s="73" t="e">
         <f>VLOOKUP($B83&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D83" s="74">
+      <c r="D83" s="73">
         <v>1</v>
       </c>
-      <c r="E83" s="74" t="e">
+      <c r="E83" s="73" t="e">
         <f>VLOOKUP($B83&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F83" s="74" t="e">
+      <c r="F83" s="73" t="e">
         <f>VLOOKUP($B83&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G83" s="74" t="e">
+      <c r="G83" s="73" t="e">
         <f>VLOOKUP($B83&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H83" s="74" t="e">
+      <c r="H83" s="73" t="e">
         <f>VLOOKUP($B83&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I83" s="74" t="e">
+      <c r="I83" s="73" t="e">
         <f>VLOOKUP($B83&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M83" s="75"/>
-      <c r="N83" s="75"/>
+      <c r="M83" s="74"/>
+      <c r="N83" s="74"/>
     </row>
     <row r="84" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="15" t="e">
@@ -8684,35 +8688,35 @@
       <c r="B84" s="45" t="s">
         <v>107</v>
       </c>
-      <c r="C84" s="74" t="e">
+      <c r="C84" s="73" t="e">
         <f>VLOOKUP($B84&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D84" s="74">
+      <c r="D84" s="73">
         <v>1</v>
       </c>
-      <c r="E84" s="74" t="e">
+      <c r="E84" s="73" t="e">
         <f>VLOOKUP($B84&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F84" s="74" t="e">
+      <c r="F84" s="73" t="e">
         <f>VLOOKUP($B84&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G84" s="74" t="e">
+      <c r="G84" s="73" t="e">
         <f>VLOOKUP($B84&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H84" s="74" t="e">
+      <c r="H84" s="73" t="e">
         <f>VLOOKUP($B84&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I84" s="74" t="e">
+      <c r="I84" s="73" t="e">
         <f>VLOOKUP($B84&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M84" s="75"/>
-      <c r="N84" s="75"/>
+      <c r="M84" s="74"/>
+      <c r="N84" s="74"/>
     </row>
     <row r="85" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="15" t="e">
@@ -8722,35 +8726,35 @@
       <c r="B85" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="C85" s="74" t="e">
+      <c r="C85" s="73" t="e">
         <f>VLOOKUP($B85&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D85" s="74">
+      <c r="D85" s="73">
         <v>1</v>
       </c>
-      <c r="E85" s="74" t="e">
+      <c r="E85" s="73" t="e">
         <f>VLOOKUP($B85&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F85" s="74" t="e">
+      <c r="F85" s="73" t="e">
         <f>VLOOKUP($B85&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G85" s="74" t="e">
+      <c r="G85" s="73" t="e">
         <f>VLOOKUP($B85&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H85" s="74" t="e">
+      <c r="H85" s="73" t="e">
         <f>VLOOKUP($B85&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I85" s="74" t="e">
+      <c r="I85" s="73" t="e">
         <f>VLOOKUP($B85&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M85" s="75"/>
-      <c r="N85" s="75"/>
+      <c r="M85" s="74"/>
+      <c r="N85" s="74"/>
     </row>
     <row r="86" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="15" t="e">
@@ -8760,35 +8764,35 @@
       <c r="B86" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="C86" s="74" t="e">
+      <c r="C86" s="73" t="e">
         <f>VLOOKUP($B86&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D86" s="74">
+      <c r="D86" s="73">
         <v>1</v>
       </c>
-      <c r="E86" s="74" t="e">
+      <c r="E86" s="73" t="e">
         <f>VLOOKUP($B86&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F86" s="74" t="e">
+      <c r="F86" s="73" t="e">
         <f>VLOOKUP($B86&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G86" s="74" t="e">
+      <c r="G86" s="73" t="e">
         <f>VLOOKUP($B86&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H86" s="74" t="e">
+      <c r="H86" s="73" t="e">
         <f>VLOOKUP($B86&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I86" s="74" t="e">
+      <c r="I86" s="73" t="e">
         <f>VLOOKUP($B86&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M86" s="75"/>
-      <c r="N86" s="75"/>
+      <c r="M86" s="74"/>
+      <c r="N86" s="74"/>
     </row>
     <row r="87" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="15" t="e">
@@ -8798,35 +8802,35 @@
       <c r="B87" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="C87" s="74" t="e">
+      <c r="C87" s="73" t="e">
         <f>VLOOKUP($B87&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D87" s="74">
+      <c r="D87" s="73">
         <v>1</v>
       </c>
-      <c r="E87" s="74" t="e">
+      <c r="E87" s="73" t="e">
         <f>VLOOKUP($B87&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F87" s="74" t="e">
+      <c r="F87" s="73" t="e">
         <f>VLOOKUP($B87&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G87" s="74" t="e">
+      <c r="G87" s="73" t="e">
         <f>VLOOKUP($B87&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H87" s="74" t="e">
+      <c r="H87" s="73" t="e">
         <f>VLOOKUP($B87&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I87" s="74" t="e">
+      <c r="I87" s="73" t="e">
         <f>VLOOKUP($B87&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M87" s="75"/>
-      <c r="N87" s="75"/>
+      <c r="M87" s="74"/>
+      <c r="N87" s="74"/>
     </row>
     <row r="88" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="15" t="e">
@@ -8836,35 +8840,35 @@
       <c r="B88" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="C88" s="74" t="e">
+      <c r="C88" s="73" t="e">
         <f>VLOOKUP($B88&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D88" s="74">
+      <c r="D88" s="73">
         <v>1</v>
       </c>
-      <c r="E88" s="74" t="e">
+      <c r="E88" s="73" t="e">
         <f>VLOOKUP($B88&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F88" s="74" t="e">
+      <c r="F88" s="73" t="e">
         <f>VLOOKUP($B88&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G88" s="74" t="e">
+      <c r="G88" s="73" t="e">
         <f>VLOOKUP($B88&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H88" s="74" t="e">
+      <c r="H88" s="73" t="e">
         <f>VLOOKUP($B88&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I88" s="74" t="e">
+      <c r="I88" s="73" t="e">
         <f>VLOOKUP($B88&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M88" s="75"/>
-      <c r="N88" s="75"/>
+      <c r="M88" s="74"/>
+      <c r="N88" s="74"/>
     </row>
     <row r="89" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="15" t="e">
@@ -8874,35 +8878,35 @@
       <c r="B89" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="C89" s="74" t="e">
+      <c r="C89" s="73" t="e">
         <f>VLOOKUP($B89&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D89" s="74">
+      <c r="D89" s="73">
         <v>1</v>
       </c>
-      <c r="E89" s="74" t="e">
+      <c r="E89" s="73" t="e">
         <f>VLOOKUP($B89&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F89" s="74" t="e">
+      <c r="F89" s="73" t="e">
         <f>VLOOKUP($B89&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G89" s="74" t="e">
+      <c r="G89" s="73" t="e">
         <f>VLOOKUP($B89&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H89" s="74" t="e">
+      <c r="H89" s="73" t="e">
         <f>VLOOKUP($B89&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I89" s="74" t="e">
+      <c r="I89" s="73" t="e">
         <f>VLOOKUP($B89&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M89" s="75"/>
-      <c r="N89" s="75"/>
+      <c r="M89" s="74"/>
+      <c r="N89" s="74"/>
     </row>
     <row r="90" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="15" t="e">
@@ -8912,35 +8916,35 @@
       <c r="B90" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="C90" s="74" t="e">
+      <c r="C90" s="73" t="e">
         <f>VLOOKUP($B90&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D90" s="74">
+      <c r="D90" s="73">
         <v>1</v>
       </c>
-      <c r="E90" s="74" t="e">
+      <c r="E90" s="73" t="e">
         <f>VLOOKUP($B90&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F90" s="74" t="e">
+      <c r="F90" s="73" t="e">
         <f>VLOOKUP($B90&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G90" s="74" t="e">
+      <c r="G90" s="73" t="e">
         <f>VLOOKUP($B90&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H90" s="74" t="e">
+      <c r="H90" s="73" t="e">
         <f>VLOOKUP($B90&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I90" s="74" t="e">
+      <c r="I90" s="73" t="e">
         <f>VLOOKUP($B90&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M90" s="75"/>
-      <c r="N90" s="75"/>
+      <c r="M90" s="74"/>
+      <c r="N90" s="74"/>
     </row>
     <row r="91" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="15" t="e">
@@ -8950,35 +8954,35 @@
       <c r="B91" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C91" s="74" t="e">
+      <c r="C91" s="73" t="e">
         <f>VLOOKUP($B91&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D91" s="74">
+      <c r="D91" s="73">
         <v>1</v>
       </c>
-      <c r="E91" s="74" t="e">
+      <c r="E91" s="73" t="e">
         <f>VLOOKUP($B91&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F91" s="74" t="e">
+      <c r="F91" s="73" t="e">
         <f>VLOOKUP($B91&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G91" s="74" t="e">
+      <c r="G91" s="73" t="e">
         <f>VLOOKUP($B91&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H91" s="74" t="e">
+      <c r="H91" s="73" t="e">
         <f>VLOOKUP($B91&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I91" s="74" t="e">
+      <c r="I91" s="73" t="e">
         <f>VLOOKUP($B91&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M91" s="75"/>
-      <c r="N91" s="75"/>
+      <c r="M91" s="74"/>
+      <c r="N91" s="74"/>
     </row>
     <row r="92" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="15" t="e">
@@ -8988,35 +8992,35 @@
       <c r="B92" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="C92" s="74" t="e">
+      <c r="C92" s="73" t="e">
         <f>VLOOKUP($B92&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D92" s="74">
+      <c r="D92" s="73">
         <v>1</v>
       </c>
-      <c r="E92" s="74" t="e">
+      <c r="E92" s="73" t="e">
         <f>VLOOKUP($B92&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F92" s="74" t="e">
+      <c r="F92" s="73" t="e">
         <f>VLOOKUP($B92&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G92" s="74" t="e">
+      <c r="G92" s="73" t="e">
         <f>VLOOKUP($B92&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H92" s="74" t="e">
+      <c r="H92" s="73" t="e">
         <f>VLOOKUP($B92&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I92" s="74" t="e">
+      <c r="I92" s="73" t="e">
         <f>VLOOKUP($B92&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M92" s="75"/>
-      <c r="N92" s="75"/>
+      <c r="M92" s="74"/>
+      <c r="N92" s="74"/>
     </row>
     <row r="93" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="15" t="e">
@@ -9026,35 +9030,35 @@
       <c r="B93" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="C93" s="74" t="e">
+      <c r="C93" s="73" t="e">
         <f>VLOOKUP($B93&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D93" s="74">
+      <c r="D93" s="73">
         <v>1</v>
       </c>
-      <c r="E93" s="74" t="e">
+      <c r="E93" s="73" t="e">
         <f>VLOOKUP($B93&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F93" s="74" t="e">
+      <c r="F93" s="73" t="e">
         <f>VLOOKUP($B93&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G93" s="74" t="e">
+      <c r="G93" s="73" t="e">
         <f>VLOOKUP($B93&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H93" s="74" t="e">
+      <c r="H93" s="73" t="e">
         <f>VLOOKUP($B93&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I93" s="74" t="e">
+      <c r="I93" s="73" t="e">
         <f>VLOOKUP($B93&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M93" s="75"/>
-      <c r="N93" s="75"/>
+      <c r="M93" s="74"/>
+      <c r="N93" s="74"/>
     </row>
     <row r="94" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="15" t="e">
@@ -9064,35 +9068,35 @@
       <c r="B94" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="C94" s="74" t="e">
+      <c r="C94" s="73" t="e">
         <f>VLOOKUP($B94&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D94" s="74">
+      <c r="D94" s="73">
         <v>1</v>
       </c>
-      <c r="E94" s="74" t="e">
+      <c r="E94" s="73" t="e">
         <f>VLOOKUP($B94&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F94" s="74" t="e">
+      <c r="F94" s="73" t="e">
         <f>VLOOKUP($B94&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G94" s="74" t="e">
+      <c r="G94" s="73" t="e">
         <f>VLOOKUP($B94&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H94" s="74" t="e">
+      <c r="H94" s="73" t="e">
         <f>VLOOKUP($B94&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I94" s="74" t="e">
+      <c r="I94" s="73" t="e">
         <f>VLOOKUP($B94&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M94" s="75"/>
-      <c r="N94" s="75"/>
+      <c r="M94" s="74"/>
+      <c r="N94" s="74"/>
     </row>
     <row r="95" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="15" t="e">
@@ -9102,35 +9106,35 @@
       <c r="B95" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="C95" s="74" t="e">
+      <c r="C95" s="73" t="e">
         <f>VLOOKUP($B95&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D95" s="74">
+      <c r="D95" s="73">
         <v>1</v>
       </c>
-      <c r="E95" s="74" t="e">
+      <c r="E95" s="73" t="e">
         <f>VLOOKUP($B95&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F95" s="74" t="e">
+      <c r="F95" s="73" t="e">
         <f>VLOOKUP($B95&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G95" s="74" t="e">
+      <c r="G95" s="73" t="e">
         <f>VLOOKUP($B95&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H95" s="74" t="e">
+      <c r="H95" s="73" t="e">
         <f>VLOOKUP($B95&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I95" s="74" t="e">
+      <c r="I95" s="73" t="e">
         <f>VLOOKUP($B95&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M95" s="75"/>
-      <c r="N95" s="75"/>
+      <c r="M95" s="74"/>
+      <c r="N95" s="74"/>
     </row>
     <row r="96" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="15" t="e">
@@ -9140,35 +9144,35 @@
       <c r="B96" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="C96" s="74" t="e">
+      <c r="C96" s="73" t="e">
         <f>VLOOKUP($B96&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D96" s="74">
+      <c r="D96" s="73">
         <v>1</v>
       </c>
-      <c r="E96" s="74" t="e">
+      <c r="E96" s="73" t="e">
         <f>VLOOKUP($B96&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F96" s="74" t="e">
+      <c r="F96" s="73" t="e">
         <f>VLOOKUP($B96&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G96" s="74" t="e">
+      <c r="G96" s="73" t="e">
         <f>VLOOKUP($B96&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H96" s="74" t="e">
+      <c r="H96" s="73" t="e">
         <f>VLOOKUP($B96&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I96" s="74" t="e">
+      <c r="I96" s="73" t="e">
         <f>VLOOKUP($B96&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M96" s="75"/>
-      <c r="N96" s="75"/>
+      <c r="M96" s="74"/>
+      <c r="N96" s="74"/>
     </row>
     <row r="97" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="15" t="e">
@@ -9178,35 +9182,35 @@
       <c r="B97" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="C97" s="74" t="e">
+      <c r="C97" s="73" t="e">
         <f>VLOOKUP($B97&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D97" s="74">
+      <c r="D97" s="73">
         <v>1</v>
       </c>
-      <c r="E97" s="74" t="e">
+      <c r="E97" s="73" t="e">
         <f>VLOOKUP($B97&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F97" s="74" t="e">
+      <c r="F97" s="73" t="e">
         <f>VLOOKUP($B97&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G97" s="74" t="e">
+      <c r="G97" s="73" t="e">
         <f>VLOOKUP($B97&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H97" s="74" t="e">
+      <c r="H97" s="73" t="e">
         <f>VLOOKUP($B97&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I97" s="74" t="e">
+      <c r="I97" s="73" t="e">
         <f>VLOOKUP($B97&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M97" s="75"/>
-      <c r="N97" s="75"/>
+      <c r="M97" s="74"/>
+      <c r="N97" s="74"/>
     </row>
     <row r="98" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="15" t="e">
@@ -9216,35 +9220,35 @@
       <c r="B98" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="C98" s="74" t="e">
+      <c r="C98" s="73" t="e">
         <f>VLOOKUP($B98&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D98" s="74">
+      <c r="D98" s="73">
         <v>1</v>
       </c>
-      <c r="E98" s="74" t="e">
+      <c r="E98" s="73" t="e">
         <f>VLOOKUP($B98&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F98" s="74" t="e">
+      <c r="F98" s="73" t="e">
         <f>VLOOKUP($B98&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G98" s="74" t="e">
+      <c r="G98" s="73" t="e">
         <f>VLOOKUP($B98&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H98" s="74" t="e">
+      <c r="H98" s="73" t="e">
         <f>VLOOKUP($B98&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I98" s="74" t="e">
+      <c r="I98" s="73" t="e">
         <f>VLOOKUP($B98&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M98" s="75"/>
-      <c r="N98" s="75"/>
+      <c r="M98" s="74"/>
+      <c r="N98" s="74"/>
     </row>
     <row r="99" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="15" t="e">
@@ -9254,35 +9258,35 @@
       <c r="B99" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="C99" s="74" t="e">
+      <c r="C99" s="73" t="e">
         <f>VLOOKUP($B99&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D99" s="74">
+      <c r="D99" s="73">
         <v>1</v>
       </c>
-      <c r="E99" s="74" t="e">
+      <c r="E99" s="73" t="e">
         <f>VLOOKUP($B99&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F99" s="74" t="e">
+      <c r="F99" s="73" t="e">
         <f>VLOOKUP($B99&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G99" s="74" t="e">
+      <c r="G99" s="73" t="e">
         <f>VLOOKUP($B99&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H99" s="74" t="e">
+      <c r="H99" s="73" t="e">
         <f>VLOOKUP($B99&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I99" s="74" t="e">
+      <c r="I99" s="73" t="e">
         <f>VLOOKUP($B99&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M99" s="75"/>
-      <c r="N99" s="75"/>
+      <c r="M99" s="74"/>
+      <c r="N99" s="74"/>
     </row>
     <row r="100" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="15" t="e">
@@ -9292,35 +9296,35 @@
       <c r="B100" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="C100" s="74" t="e">
+      <c r="C100" s="73" t="e">
         <f>VLOOKUP($B100&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D100" s="74">
+      <c r="D100" s="73">
         <v>1</v>
       </c>
-      <c r="E100" s="74" t="e">
+      <c r="E100" s="73" t="e">
         <f>VLOOKUP($B100&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F100" s="74" t="e">
+      <c r="F100" s="73" t="e">
         <f>VLOOKUP($B100&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G100" s="74" t="e">
+      <c r="G100" s="73" t="e">
         <f>VLOOKUP($B100&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H100" s="74" t="e">
+      <c r="H100" s="73" t="e">
         <f>VLOOKUP($B100&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I100" s="74" t="e">
+      <c r="I100" s="73" t="e">
         <f>VLOOKUP($B100&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M100" s="75"/>
-      <c r="N100" s="75"/>
+      <c r="M100" s="74"/>
+      <c r="N100" s="74"/>
     </row>
     <row r="101" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A101" s="15" t="e">
@@ -9330,35 +9334,35 @@
       <c r="B101" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="C101" s="74" t="e">
+      <c r="C101" s="73" t="e">
         <f>VLOOKUP($B101&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D101" s="74">
+      <c r="D101" s="73">
         <v>1</v>
       </c>
-      <c r="E101" s="74" t="e">
+      <c r="E101" s="73" t="e">
         <f>VLOOKUP($B101&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F101" s="74" t="e">
+      <c r="F101" s="73" t="e">
         <f>VLOOKUP($B101&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G101" s="74" t="e">
+      <c r="G101" s="73" t="e">
         <f>VLOOKUP($B101&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H101" s="74" t="e">
+      <c r="H101" s="73" t="e">
         <f>VLOOKUP($B101&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I101" s="74" t="e">
+      <c r="I101" s="73" t="e">
         <f>VLOOKUP($B101&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M101" s="75"/>
-      <c r="N101" s="75"/>
+      <c r="M101" s="74"/>
+      <c r="N101" s="74"/>
     </row>
     <row r="102" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="15" t="e">
@@ -9368,35 +9372,35 @@
       <c r="B102" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="C102" s="74" t="e">
+      <c r="C102" s="73" t="e">
         <f>VLOOKUP($B102&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D102" s="74">
+      <c r="D102" s="73">
         <v>1</v>
       </c>
-      <c r="E102" s="74" t="e">
+      <c r="E102" s="73" t="e">
         <f>VLOOKUP($B102&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F102" s="74" t="e">
+      <c r="F102" s="73" t="e">
         <f>VLOOKUP($B102&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G102" s="74" t="e">
+      <c r="G102" s="73" t="e">
         <f>VLOOKUP($B102&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H102" s="74" t="e">
+      <c r="H102" s="73" t="e">
         <f>VLOOKUP($B102&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I102" s="74" t="e">
+      <c r="I102" s="73" t="e">
         <f>VLOOKUP($B102&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M102" s="75"/>
-      <c r="N102" s="75"/>
+      <c r="M102" s="74"/>
+      <c r="N102" s="74"/>
     </row>
     <row r="103" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" s="15" t="e">
@@ -9406,35 +9410,35 @@
       <c r="B103" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="C103" s="74" t="e">
+      <c r="C103" s="73" t="e">
         <f>VLOOKUP($B103&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D103" s="74">
+      <c r="D103" s="73">
         <v>1</v>
       </c>
-      <c r="E103" s="74" t="e">
+      <c r="E103" s="73" t="e">
         <f>VLOOKUP($B103&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F103" s="74" t="e">
+      <c r="F103" s="73" t="e">
         <f>VLOOKUP($B103&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G103" s="74" t="e">
+      <c r="G103" s="73" t="e">
         <f>VLOOKUP($B103&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H103" s="74" t="e">
+      <c r="H103" s="73" t="e">
         <f>VLOOKUP($B103&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I103" s="74" t="e">
+      <c r="I103" s="73" t="e">
         <f>VLOOKUP($B103&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M103" s="75"/>
-      <c r="N103" s="75"/>
+      <c r="M103" s="74"/>
+      <c r="N103" s="74"/>
     </row>
     <row r="104" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A104" s="15" t="e">
@@ -9444,35 +9448,35 @@
       <c r="B104" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="C104" s="74" t="e">
+      <c r="C104" s="73" t="e">
         <f>VLOOKUP($B104&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D104" s="74">
+      <c r="D104" s="73">
         <v>1</v>
       </c>
-      <c r="E104" s="74" t="e">
+      <c r="E104" s="73" t="e">
         <f>VLOOKUP($B104&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F104" s="74" t="e">
+      <c r="F104" s="73" t="e">
         <f>VLOOKUP($B104&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G104" s="74" t="e">
+      <c r="G104" s="73" t="e">
         <f>VLOOKUP($B104&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H104" s="74" t="e">
+      <c r="H104" s="73" t="e">
         <f>VLOOKUP($B104&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I104" s="74" t="e">
+      <c r="I104" s="73" t="e">
         <f>VLOOKUP($B104&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M104" s="75"/>
-      <c r="N104" s="75"/>
+      <c r="M104" s="74"/>
+      <c r="N104" s="74"/>
     </row>
     <row r="105" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A105" s="15" t="e">
@@ -9482,35 +9486,35 @@
       <c r="B105" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="C105" s="74" t="e">
+      <c r="C105" s="73" t="e">
         <f>VLOOKUP($B105&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D105" s="74">
+      <c r="D105" s="73">
         <v>1</v>
       </c>
-      <c r="E105" s="74" t="e">
+      <c r="E105" s="73" t="e">
         <f>VLOOKUP($B105&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F105" s="74" t="e">
+      <c r="F105" s="73" t="e">
         <f>VLOOKUP($B105&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G105" s="74" t="e">
+      <c r="G105" s="73" t="e">
         <f>VLOOKUP($B105&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H105" s="74" t="e">
+      <c r="H105" s="73" t="e">
         <f>VLOOKUP($B105&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I105" s="74" t="e">
+      <c r="I105" s="73" t="e">
         <f>VLOOKUP($B105&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M105" s="75"/>
-      <c r="N105" s="75"/>
+      <c r="M105" s="74"/>
+      <c r="N105" s="74"/>
     </row>
     <row r="106" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A106" s="15" t="e">
@@ -9520,35 +9524,35 @@
       <c r="B106" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="C106" s="74" t="e">
+      <c r="C106" s="73" t="e">
         <f>VLOOKUP($B106&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D106" s="74">
+      <c r="D106" s="73">
         <v>1</v>
       </c>
-      <c r="E106" s="74" t="e">
+      <c r="E106" s="73" t="e">
         <f>VLOOKUP($B106&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F106" s="74" t="e">
+      <c r="F106" s="73" t="e">
         <f>VLOOKUP($B106&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G106" s="74" t="e">
+      <c r="G106" s="73" t="e">
         <f>VLOOKUP($B106&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H106" s="74" t="e">
+      <c r="H106" s="73" t="e">
         <f>VLOOKUP($B106&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I106" s="74" t="e">
+      <c r="I106" s="73" t="e">
         <f>VLOOKUP($B106&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M106" s="75"/>
-      <c r="N106" s="75"/>
+      <c r="M106" s="74"/>
+      <c r="N106" s="74"/>
     </row>
     <row r="107" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A107" s="15" t="e">
@@ -9558,35 +9562,35 @@
       <c r="B107" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C107" s="74" t="e">
+      <c r="C107" s="73" t="e">
         <f>VLOOKUP($B107&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D107" s="74">
+      <c r="D107" s="73">
         <v>1</v>
       </c>
-      <c r="E107" s="74" t="e">
+      <c r="E107" s="73" t="e">
         <f>VLOOKUP($B107&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F107" s="74" t="e">
+      <c r="F107" s="73" t="e">
         <f>VLOOKUP($B107&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G107" s="74" t="e">
+      <c r="G107" s="73" t="e">
         <f>VLOOKUP($B107&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H107" s="74" t="e">
+      <c r="H107" s="73" t="e">
         <f>VLOOKUP($B107&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I107" s="74" t="e">
+      <c r="I107" s="73" t="e">
         <f>VLOOKUP($B107&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M107" s="75"/>
-      <c r="N107" s="75"/>
+      <c r="M107" s="74"/>
+      <c r="N107" s="74"/>
     </row>
     <row r="108" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A108" s="15" t="e">
@@ -9596,35 +9600,35 @@
       <c r="B108" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="C108" s="74" t="e">
+      <c r="C108" s="73" t="e">
         <f>VLOOKUP($B108&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D108" s="74">
+      <c r="D108" s="73">
         <v>1</v>
       </c>
-      <c r="E108" s="74" t="e">
+      <c r="E108" s="73" t="e">
         <f>VLOOKUP($B108&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F108" s="74" t="e">
+      <c r="F108" s="73" t="e">
         <f>VLOOKUP($B108&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G108" s="74" t="e">
+      <c r="G108" s="73" t="e">
         <f>VLOOKUP($B108&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H108" s="74" t="e">
+      <c r="H108" s="73" t="e">
         <f>VLOOKUP($B108&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I108" s="74" t="e">
+      <c r="I108" s="73" t="e">
         <f>VLOOKUP($B108&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M108" s="75"/>
-      <c r="N108" s="75"/>
+      <c r="M108" s="74"/>
+      <c r="N108" s="74"/>
     </row>
     <row r="109" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A109" s="15" t="e">
@@ -9634,30 +9638,30 @@
       <c r="B109" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="C109" s="74" t="e">
+      <c r="C109" s="73" t="e">
         <f>VLOOKUP($B109&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D109" s="74">
+      <c r="D109" s="73">
         <v>1</v>
       </c>
-      <c r="E109" s="74" t="e">
+      <c r="E109" s="73" t="e">
         <f>VLOOKUP($B109&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F109" s="74" t="e">
+      <c r="F109" s="73" t="e">
         <f>VLOOKUP($B109&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G109" s="74" t="e">
+      <c r="G109" s="73" t="e">
         <f>VLOOKUP($B109&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H109" s="74" t="e">
+      <c r="H109" s="73" t="e">
         <f>VLOOKUP($B109&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I109" s="74" t="e">
+      <c r="I109" s="73" t="e">
         <f>VLOOKUP($B109&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
@@ -9670,30 +9674,30 @@
       <c r="B110" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="C110" s="74" t="e">
+      <c r="C110" s="73" t="e">
         <f>VLOOKUP($B110&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D110" s="74">
+      <c r="D110" s="73">
         <v>1</v>
       </c>
-      <c r="E110" s="74" t="e">
+      <c r="E110" s="73" t="e">
         <f>VLOOKUP($B110&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F110" s="74" t="e">
+      <c r="F110" s="73" t="e">
         <f>VLOOKUP($B110&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G110" s="74" t="e">
+      <c r="G110" s="73" t="e">
         <f>VLOOKUP($B110&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H110" s="74" t="e">
+      <c r="H110" s="73" t="e">
         <f>VLOOKUP($B110&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I110" s="74" t="e">
+      <c r="I110" s="73" t="e">
         <f>VLOOKUP($B110&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
@@ -9706,30 +9710,30 @@
       <c r="B111" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C111" s="74" t="e">
+      <c r="C111" s="73" t="e">
         <f>VLOOKUP($B111&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D111" s="74">
+      <c r="D111" s="73">
         <v>1</v>
       </c>
-      <c r="E111" s="74" t="e">
+      <c r="E111" s="73" t="e">
         <f>VLOOKUP($B111&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F111" s="74" t="e">
+      <c r="F111" s="73" t="e">
         <f>VLOOKUP($B111&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G111" s="74" t="e">
+      <c r="G111" s="73" t="e">
         <f>VLOOKUP($B111&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H111" s="74" t="e">
+      <c r="H111" s="73" t="e">
         <f>VLOOKUP($B111&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I111" s="74" t="e">
+      <c r="I111" s="73" t="e">
         <f>VLOOKUP($B111&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
@@ -9742,30 +9746,30 @@
       <c r="B112" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C112" s="74" t="e">
+      <c r="C112" s="73" t="e">
         <f>VLOOKUP($B112&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D112" s="74">
+      <c r="D112" s="73">
         <v>1</v>
       </c>
-      <c r="E112" s="74" t="e">
+      <c r="E112" s="73" t="e">
         <f>VLOOKUP($B112&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F112" s="74" t="e">
+      <c r="F112" s="73" t="e">
         <f>VLOOKUP($B112&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G112" s="74" t="e">
+      <c r="G112" s="73" t="e">
         <f>VLOOKUP($B112&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H112" s="74" t="e">
+      <c r="H112" s="73" t="e">
         <f>VLOOKUP($B112&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I112" s="74" t="e">
+      <c r="I112" s="73" t="e">
         <f>VLOOKUP($B112&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
@@ -9778,30 +9782,30 @@
       <c r="B113" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C113" s="74" t="e">
+      <c r="C113" s="73" t="e">
         <f>VLOOKUP($B113&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D113" s="74">
+      <c r="D113" s="73">
         <v>1</v>
       </c>
-      <c r="E113" s="74" t="e">
+      <c r="E113" s="73" t="e">
         <f>VLOOKUP($B113&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F113" s="74" t="e">
+      <c r="F113" s="73" t="e">
         <f>VLOOKUP($B113&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G113" s="74" t="e">
+      <c r="G113" s="73" t="e">
         <f>VLOOKUP($B113&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H113" s="74" t="e">
+      <c r="H113" s="73" t="e">
         <f>VLOOKUP($B113&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I113" s="74" t="e">
+      <c r="I113" s="73" t="e">
         <f>VLOOKUP($B113&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>

</xml_diff>

<commit_message>
Update excel template files
Replace ISD with PHS
Correct "%" to "per 1,000 population" for population data
Rename Table 3 and 4 to Table 3a and 3b
</commit_message>
<xml_diff>
--- a/reference_files/Table1-HSMR.xlsx
+++ b/reference_files/Table1-HSMR.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Isdsf00d03\quality_indicators\hsmr\quarter_cycle\Robyn\reference_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Isdsf00d03\quality_indicators\hsmr\quarter_cycle\Analyst folders\Scott\Updates\hsmr-pra\reference_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -753,9 +753,6 @@
     <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -780,6 +777,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="18" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4538,7 +4538,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AA83"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4552,19 +4554,19 @@
     <row r="1" spans="1:27" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="47"/>
       <c r="B1" s="8"/>
-      <c r="C1" s="65" t="s">
+      <c r="C1" s="75" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="75"/>
     </row>
     <row r="2" spans="1:27" s="9" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="47"/>
@@ -6152,8 +6154,8 @@
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B60" s="30"/>
       <c r="C60" s="1" t="str">
-        <f>"Source: ISD Scotland (SMR01) linked dataset. Reflects the completeness of SMR01 submissions to ISD for individual hospitals as of " &amp; TEXT(funnel_data!L2,"dd mmm yyyy")</f>
-        <v>Source: ISD Scotland (SMR01) linked dataset. Reflects the completeness of SMR01 submissions to ISD for individual hospitals as of 00 Jan 1900</v>
+        <f>"Source: Public Health Scotland (SMR01) linked dataset. Reflects the completeness of SMR01 submissions to PHS for individual hospitals as of " &amp; TEXT(funnel_data!L2,"dd mmm yyyy")</f>
+        <v>Source: Public Health Scotland (SMR01) linked dataset. Reflects the completeness of SMR01 submissions to PHS for individual hospitals as of 00 Jan 1900</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -6205,7 +6207,9 @@
   </sheetPr>
   <dimension ref="A1:AK119"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6222,35 +6226,35 @@
   <sheetData>
     <row r="1" spans="1:36" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="75" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
-      <c r="S1" s="65"/>
-      <c r="T1" s="65"/>
-      <c r="U1" s="65"/>
-      <c r="V1" s="65"/>
-      <c r="W1" s="65"/>
-      <c r="X1" s="65"/>
-      <c r="Y1" s="65"/>
-      <c r="Z1" s="65"/>
-      <c r="AA1" s="65"/>
-      <c r="AB1" s="65"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="75"/>
+      <c r="N1" s="75"/>
+      <c r="O1" s="75"/>
+      <c r="P1" s="75"/>
+      <c r="Q1" s="75"/>
+      <c r="R1" s="75"/>
+      <c r="S1" s="75"/>
+      <c r="T1" s="75"/>
+      <c r="U1" s="75"/>
+      <c r="V1" s="75"/>
+      <c r="W1" s="75"/>
+      <c r="X1" s="75"/>
+      <c r="Y1" s="75"/>
+      <c r="Z1" s="75"/>
+      <c r="AA1" s="75"/>
+      <c r="AB1" s="75"/>
     </row>
     <row r="2" spans="1:36" s="9" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
@@ -6780,8 +6784,8 @@
     <row r="36" spans="1:37" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="1" t="str">
-        <f>"Source: ISD Scotland (SMR01) linked dataset. Reflects the completeness of SMR01 submissions to ISD for individual hospitals as of " &amp; TEXT(funnel_data!L2,"dd mmm yyyy")</f>
-        <v>Source: ISD Scotland (SMR01) linked dataset. Reflects the completeness of SMR01 submissions to ISD for individual hospitals as of 00 Jan 1900</v>
+        <f>"Source: Public Health Scotland (SMR01) linked dataset. Reflects the completeness of SMR01 submissions to PHS for individual hospitals as of " &amp; TEXT(funnel_data!L2,"dd mmm yyyy")</f>
+        <v>Source: Public Health Scotland (SMR01) linked dataset. Reflects the completeness of SMR01 submissions to PHS for individual hospitals as of 00 Jan 1900</v>
       </c>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
@@ -6853,55 +6857,55 @@
       <c r="B47" s="15">
         <v>2</v>
       </c>
-      <c r="C47" s="66">
+      <c r="C47" s="65">
         <v>3</v>
       </c>
       <c r="D47" s="15">
         <v>4</v>
       </c>
-      <c r="E47" s="66">
+      <c r="E47" s="65">
         <v>5</v>
       </c>
       <c r="F47" s="15">
         <v>6</v>
       </c>
-      <c r="G47" s="66">
+      <c r="G47" s="65">
         <v>7</v>
       </c>
       <c r="H47" s="15">
         <v>8</v>
       </c>
-      <c r="I47" s="66">
+      <c r="I47" s="65">
         <v>9</v>
       </c>
-      <c r="Q47" s="66"/>
-      <c r="S47" s="66"/>
-      <c r="U47" s="66"/>
-      <c r="W47" s="66"/>
+      <c r="Q47" s="65"/>
+      <c r="S47" s="65"/>
+      <c r="U47" s="65"/>
+      <c r="W47" s="65"/>
     </row>
     <row r="48" spans="1:37" s="15" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B48" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="C48" s="67" t="s">
+      <c r="C48" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="D48" s="67" t="s">
+      <c r="D48" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="E48" s="67" t="s">
+      <c r="E48" s="66" t="s">
         <v>118</v>
       </c>
-      <c r="F48" s="67" t="s">
+      <c r="F48" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="G48" s="67" t="s">
+      <c r="G48" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="H48" s="67" t="s">
+      <c r="H48" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="I48" s="67" t="s">
+      <c r="I48" s="66" t="s">
         <v>56</v>
       </c>
       <c r="J48" s="15" t="s">
@@ -6914,13 +6918,13 @@
         <v>64</v>
       </c>
       <c r="P48" s="45"/>
-      <c r="Q48" s="67"/>
-      <c r="R48" s="67"/>
-      <c r="S48" s="67"/>
-      <c r="T48" s="67"/>
-      <c r="U48" s="67"/>
-      <c r="V48" s="67"/>
-      <c r="W48" s="67"/>
+      <c r="Q48" s="66"/>
+      <c r="R48" s="66"/>
+      <c r="S48" s="66"/>
+      <c r="T48" s="66"/>
+      <c r="U48" s="66"/>
+      <c r="V48" s="66"/>
+      <c r="W48" s="66"/>
     </row>
     <row r="49" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="15">
@@ -6930,31 +6934,31 @@
         <f t="shared" ref="B49:I58" si="1">VLOOKUP($A49,$A$83:$I$113,B$47,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="C49" s="68" t="e">
+      <c r="C49" s="67" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="D49" s="69" t="e">
+      <c r="D49" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="E49" s="69" t="e">
+      <c r="E49" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="F49" s="69" t="e">
+      <c r="F49" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="G49" s="69" t="e">
+      <c r="G49" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="H49" s="69" t="e">
+      <c r="H49" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="I49" s="69" t="e">
+      <c r="I49" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
@@ -6971,13 +6975,13 @@
         <v>#N/A</v>
       </c>
       <c r="P49" s="45"/>
-      <c r="Q49" s="68"/>
-      <c r="R49" s="69"/>
-      <c r="S49" s="69"/>
-      <c r="T49" s="69"/>
-      <c r="U49" s="69"/>
-      <c r="V49" s="69"/>
-      <c r="W49" s="69"/>
+      <c r="Q49" s="67"/>
+      <c r="R49" s="68"/>
+      <c r="S49" s="68"/>
+      <c r="T49" s="68"/>
+      <c r="U49" s="68"/>
+      <c r="V49" s="68"/>
+      <c r="W49" s="68"/>
     </row>
     <row r="50" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="15">
@@ -6987,31 +6991,31 @@
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="C50" s="68" t="e">
+      <c r="C50" s="67" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="D50" s="69" t="e">
+      <c r="D50" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="E50" s="69" t="e">
+      <c r="E50" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="F50" s="69" t="e">
+      <c r="F50" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="G50" s="69" t="e">
+      <c r="G50" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="H50" s="69" t="e">
+      <c r="H50" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="I50" s="69" t="e">
+      <c r="I50" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
@@ -7028,13 +7032,13 @@
         <v>#N/A</v>
       </c>
       <c r="P50" s="45"/>
-      <c r="Q50" s="68"/>
-      <c r="R50" s="69"/>
-      <c r="S50" s="69"/>
-      <c r="T50" s="69"/>
-      <c r="U50" s="69"/>
-      <c r="V50" s="69"/>
-      <c r="W50" s="69"/>
+      <c r="Q50" s="67"/>
+      <c r="R50" s="68"/>
+      <c r="S50" s="68"/>
+      <c r="T50" s="68"/>
+      <c r="U50" s="68"/>
+      <c r="V50" s="68"/>
+      <c r="W50" s="68"/>
     </row>
     <row r="51" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="15">
@@ -7044,31 +7048,31 @@
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="C51" s="68" t="e">
+      <c r="C51" s="67" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="D51" s="69" t="e">
+      <c r="D51" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="E51" s="69" t="e">
+      <c r="E51" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="F51" s="69" t="e">
+      <c r="F51" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="G51" s="69" t="e">
+      <c r="G51" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="H51" s="69" t="e">
+      <c r="H51" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="I51" s="69" t="e">
+      <c r="I51" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
@@ -7085,13 +7089,13 @@
         <v>#N/A</v>
       </c>
       <c r="P51" s="45"/>
-      <c r="Q51" s="68"/>
-      <c r="R51" s="69"/>
-      <c r="S51" s="69"/>
-      <c r="T51" s="69"/>
-      <c r="U51" s="69"/>
-      <c r="V51" s="69"/>
-      <c r="W51" s="69"/>
+      <c r="Q51" s="67"/>
+      <c r="R51" s="68"/>
+      <c r="S51" s="68"/>
+      <c r="T51" s="68"/>
+      <c r="U51" s="68"/>
+      <c r="V51" s="68"/>
+      <c r="W51" s="68"/>
     </row>
     <row r="52" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="15">
@@ -7101,31 +7105,31 @@
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="C52" s="68" t="e">
+      <c r="C52" s="67" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="D52" s="69" t="e">
+      <c r="D52" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="E52" s="69" t="e">
+      <c r="E52" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="F52" s="69" t="e">
+      <c r="F52" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="G52" s="69" t="e">
+      <c r="G52" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="H52" s="69" t="e">
+      <c r="H52" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="I52" s="69" t="e">
+      <c r="I52" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
@@ -7142,13 +7146,13 @@
         <v>#N/A</v>
       </c>
       <c r="P52" s="45"/>
-      <c r="Q52" s="68"/>
-      <c r="R52" s="69"/>
-      <c r="S52" s="69"/>
-      <c r="T52" s="69"/>
-      <c r="U52" s="69"/>
-      <c r="V52" s="69"/>
-      <c r="W52" s="69"/>
+      <c r="Q52" s="67"/>
+      <c r="R52" s="68"/>
+      <c r="S52" s="68"/>
+      <c r="T52" s="68"/>
+      <c r="U52" s="68"/>
+      <c r="V52" s="68"/>
+      <c r="W52" s="68"/>
     </row>
     <row r="53" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="15">
@@ -7158,31 +7162,31 @@
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="C53" s="68" t="e">
+      <c r="C53" s="67" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="D53" s="69" t="e">
+      <c r="D53" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="E53" s="69" t="e">
+      <c r="E53" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="F53" s="69" t="e">
+      <c r="F53" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="G53" s="69" t="e">
+      <c r="G53" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="H53" s="69" t="e">
+      <c r="H53" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="I53" s="69" t="e">
+      <c r="I53" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
@@ -7199,13 +7203,13 @@
         <v>#N/A</v>
       </c>
       <c r="P53" s="45"/>
-      <c r="Q53" s="68"/>
-      <c r="R53" s="69"/>
-      <c r="S53" s="69"/>
-      <c r="T53" s="69"/>
-      <c r="U53" s="69"/>
-      <c r="V53" s="69"/>
-      <c r="W53" s="69"/>
+      <c r="Q53" s="67"/>
+      <c r="R53" s="68"/>
+      <c r="S53" s="68"/>
+      <c r="T53" s="68"/>
+      <c r="U53" s="68"/>
+      <c r="V53" s="68"/>
+      <c r="W53" s="68"/>
     </row>
     <row r="54" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="15">
@@ -7215,31 +7219,31 @@
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="C54" s="68" t="e">
+      <c r="C54" s="67" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="D54" s="69" t="e">
+      <c r="D54" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="E54" s="69" t="e">
+      <c r="E54" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="F54" s="69" t="e">
+      <c r="F54" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="G54" s="69" t="e">
+      <c r="G54" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="H54" s="69" t="e">
+      <c r="H54" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="I54" s="69" t="e">
+      <c r="I54" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
@@ -7256,13 +7260,13 @@
         <v>#N/A</v>
       </c>
       <c r="P54" s="45"/>
-      <c r="Q54" s="68"/>
-      <c r="R54" s="69"/>
-      <c r="S54" s="69"/>
-      <c r="T54" s="69"/>
-      <c r="U54" s="69"/>
-      <c r="V54" s="69"/>
-      <c r="W54" s="69"/>
+      <c r="Q54" s="67"/>
+      <c r="R54" s="68"/>
+      <c r="S54" s="68"/>
+      <c r="T54" s="68"/>
+      <c r="U54" s="68"/>
+      <c r="V54" s="68"/>
+      <c r="W54" s="68"/>
     </row>
     <row r="55" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="15">
@@ -7272,31 +7276,31 @@
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="C55" s="68" t="e">
+      <c r="C55" s="67" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="D55" s="69" t="e">
+      <c r="D55" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="E55" s="69" t="e">
+      <c r="E55" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="F55" s="69" t="e">
+      <c r="F55" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="G55" s="69" t="e">
+      <c r="G55" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="H55" s="69" t="e">
+      <c r="H55" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="I55" s="69" t="e">
+      <c r="I55" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
@@ -7313,13 +7317,13 @@
         <v>#N/A</v>
       </c>
       <c r="P55" s="45"/>
-      <c r="Q55" s="68"/>
-      <c r="R55" s="69"/>
-      <c r="S55" s="69"/>
-      <c r="T55" s="69"/>
-      <c r="U55" s="69"/>
-      <c r="V55" s="69"/>
-      <c r="W55" s="69"/>
+      <c r="Q55" s="67"/>
+      <c r="R55" s="68"/>
+      <c r="S55" s="68"/>
+      <c r="T55" s="68"/>
+      <c r="U55" s="68"/>
+      <c r="V55" s="68"/>
+      <c r="W55" s="68"/>
     </row>
     <row r="56" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="15">
@@ -7329,31 +7333,31 @@
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="C56" s="68" t="e">
+      <c r="C56" s="67" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="D56" s="69" t="e">
+      <c r="D56" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="E56" s="69" t="e">
+      <c r="E56" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="F56" s="69" t="e">
+      <c r="F56" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="G56" s="69" t="e">
+      <c r="G56" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="H56" s="69" t="e">
+      <c r="H56" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="I56" s="69" t="e">
+      <c r="I56" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
@@ -7370,13 +7374,13 @@
         <v>#N/A</v>
       </c>
       <c r="P56" s="45"/>
-      <c r="Q56" s="68"/>
-      <c r="R56" s="69"/>
-      <c r="S56" s="69"/>
-      <c r="T56" s="69"/>
-      <c r="U56" s="69"/>
-      <c r="V56" s="69"/>
-      <c r="W56" s="69"/>
+      <c r="Q56" s="67"/>
+      <c r="R56" s="68"/>
+      <c r="S56" s="68"/>
+      <c r="T56" s="68"/>
+      <c r="U56" s="68"/>
+      <c r="V56" s="68"/>
+      <c r="W56" s="68"/>
     </row>
     <row r="57" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="15">
@@ -7386,31 +7390,31 @@
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="C57" s="68" t="e">
+      <c r="C57" s="67" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="D57" s="69" t="e">
+      <c r="D57" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="E57" s="69" t="e">
+      <c r="E57" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="F57" s="69" t="e">
+      <c r="F57" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="G57" s="69" t="e">
+      <c r="G57" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="H57" s="69" t="e">
+      <c r="H57" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="I57" s="69" t="e">
+      <c r="I57" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
@@ -7427,13 +7431,13 @@
         <v>#N/A</v>
       </c>
       <c r="P57" s="45"/>
-      <c r="Q57" s="68"/>
-      <c r="R57" s="69"/>
-      <c r="S57" s="69"/>
-      <c r="T57" s="69"/>
-      <c r="U57" s="69"/>
-      <c r="V57" s="69"/>
-      <c r="W57" s="69"/>
+      <c r="Q57" s="67"/>
+      <c r="R57" s="68"/>
+      <c r="S57" s="68"/>
+      <c r="T57" s="68"/>
+      <c r="U57" s="68"/>
+      <c r="V57" s="68"/>
+      <c r="W57" s="68"/>
     </row>
     <row r="58" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="15">
@@ -7443,31 +7447,31 @@
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="C58" s="68" t="e">
+      <c r="C58" s="67" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="D58" s="69" t="e">
+      <c r="D58" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="E58" s="69" t="e">
+      <c r="E58" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="F58" s="69" t="e">
+      <c r="F58" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="G58" s="69" t="e">
+      <c r="G58" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="H58" s="69" t="e">
+      <c r="H58" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="I58" s="69" t="e">
+      <c r="I58" s="68" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
@@ -7484,13 +7488,13 @@
         <v>#N/A</v>
       </c>
       <c r="P58" s="45"/>
-      <c r="Q58" s="68"/>
-      <c r="R58" s="69"/>
-      <c r="S58" s="69"/>
-      <c r="T58" s="69"/>
-      <c r="U58" s="69"/>
-      <c r="V58" s="69"/>
-      <c r="W58" s="69"/>
+      <c r="Q58" s="67"/>
+      <c r="R58" s="68"/>
+      <c r="S58" s="68"/>
+      <c r="T58" s="68"/>
+      <c r="U58" s="68"/>
+      <c r="V58" s="68"/>
+      <c r="W58" s="68"/>
     </row>
     <row r="59" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="15">
@@ -7500,31 +7504,31 @@
         <f t="shared" ref="B59:I68" si="5">VLOOKUP($A59,$A$83:$I$113,B$47,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="C59" s="68" t="e">
+      <c r="C59" s="67" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="D59" s="69" t="e">
+      <c r="D59" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="E59" s="69" t="e">
+      <c r="E59" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="F59" s="69" t="e">
+      <c r="F59" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="G59" s="69" t="e">
+      <c r="G59" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="H59" s="69" t="e">
+      <c r="H59" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="I59" s="69" t="e">
+      <c r="I59" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
@@ -7541,13 +7545,13 @@
         <v>#N/A</v>
       </c>
       <c r="P59" s="45"/>
-      <c r="Q59" s="68"/>
-      <c r="R59" s="69"/>
-      <c r="S59" s="69"/>
-      <c r="T59" s="69"/>
-      <c r="U59" s="69"/>
-      <c r="V59" s="69"/>
-      <c r="W59" s="69"/>
+      <c r="Q59" s="67"/>
+      <c r="R59" s="68"/>
+      <c r="S59" s="68"/>
+      <c r="T59" s="68"/>
+      <c r="U59" s="68"/>
+      <c r="V59" s="68"/>
+      <c r="W59" s="68"/>
     </row>
     <row r="60" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="15">
@@ -7557,31 +7561,31 @@
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="C60" s="68" t="e">
+      <c r="C60" s="67" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="D60" s="69" t="e">
+      <c r="D60" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="E60" s="69" t="e">
+      <c r="E60" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="F60" s="69" t="e">
+      <c r="F60" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="G60" s="69" t="e">
+      <c r="G60" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="H60" s="69" t="e">
+      <c r="H60" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="I60" s="69" t="e">
+      <c r="I60" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
@@ -7598,13 +7602,13 @@
         <v>#N/A</v>
       </c>
       <c r="P60" s="45"/>
-      <c r="Q60" s="68"/>
-      <c r="R60" s="69"/>
-      <c r="S60" s="69"/>
-      <c r="T60" s="69"/>
-      <c r="U60" s="69"/>
-      <c r="V60" s="69"/>
-      <c r="W60" s="69"/>
+      <c r="Q60" s="67"/>
+      <c r="R60" s="68"/>
+      <c r="S60" s="68"/>
+      <c r="T60" s="68"/>
+      <c r="U60" s="68"/>
+      <c r="V60" s="68"/>
+      <c r="W60" s="68"/>
     </row>
     <row r="61" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="15">
@@ -7614,31 +7618,31 @@
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="C61" s="68" t="e">
+      <c r="C61" s="67" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="D61" s="69" t="e">
+      <c r="D61" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="E61" s="69" t="e">
+      <c r="E61" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="F61" s="69" t="e">
+      <c r="F61" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="G61" s="69" t="e">
+      <c r="G61" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="H61" s="69" t="e">
+      <c r="H61" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="I61" s="69" t="e">
+      <c r="I61" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
@@ -7655,13 +7659,13 @@
         <v>#N/A</v>
       </c>
       <c r="P61" s="45"/>
-      <c r="Q61" s="68"/>
-      <c r="R61" s="69"/>
-      <c r="S61" s="69"/>
-      <c r="T61" s="69"/>
-      <c r="U61" s="69"/>
-      <c r="V61" s="69"/>
-      <c r="W61" s="69"/>
+      <c r="Q61" s="67"/>
+      <c r="R61" s="68"/>
+      <c r="S61" s="68"/>
+      <c r="T61" s="68"/>
+      <c r="U61" s="68"/>
+      <c r="V61" s="68"/>
+      <c r="W61" s="68"/>
     </row>
     <row r="62" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="15">
@@ -7671,31 +7675,31 @@
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="C62" s="68" t="e">
+      <c r="C62" s="67" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="D62" s="69" t="e">
+      <c r="D62" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="E62" s="69" t="e">
+      <c r="E62" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="F62" s="69" t="e">
+      <c r="F62" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="G62" s="69" t="e">
+      <c r="G62" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="H62" s="69" t="e">
+      <c r="H62" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="I62" s="69" t="e">
+      <c r="I62" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
@@ -7712,13 +7716,13 @@
         <v>#N/A</v>
       </c>
       <c r="P62" s="45"/>
-      <c r="Q62" s="68"/>
-      <c r="R62" s="69"/>
-      <c r="S62" s="69"/>
-      <c r="T62" s="69"/>
-      <c r="U62" s="69"/>
-      <c r="V62" s="69"/>
-      <c r="W62" s="69"/>
+      <c r="Q62" s="67"/>
+      <c r="R62" s="68"/>
+      <c r="S62" s="68"/>
+      <c r="T62" s="68"/>
+      <c r="U62" s="68"/>
+      <c r="V62" s="68"/>
+      <c r="W62" s="68"/>
     </row>
     <row r="63" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="15">
@@ -7728,31 +7732,31 @@
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="C63" s="68" t="e">
+      <c r="C63" s="67" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="D63" s="69" t="e">
+      <c r="D63" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="E63" s="69" t="e">
+      <c r="E63" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="F63" s="69" t="e">
+      <c r="F63" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="G63" s="69" t="e">
+      <c r="G63" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="H63" s="69" t="e">
+      <c r="H63" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="I63" s="69" t="e">
+      <c r="I63" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
@@ -7769,13 +7773,13 @@
         <v>#N/A</v>
       </c>
       <c r="P63" s="45"/>
-      <c r="Q63" s="68"/>
-      <c r="R63" s="69"/>
-      <c r="S63" s="69"/>
-      <c r="T63" s="69"/>
-      <c r="U63" s="69"/>
-      <c r="V63" s="69"/>
-      <c r="W63" s="69"/>
+      <c r="Q63" s="67"/>
+      <c r="R63" s="68"/>
+      <c r="S63" s="68"/>
+      <c r="T63" s="68"/>
+      <c r="U63" s="68"/>
+      <c r="V63" s="68"/>
+      <c r="W63" s="68"/>
     </row>
     <row r="64" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="15">
@@ -7785,31 +7789,31 @@
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="C64" s="68" t="e">
+      <c r="C64" s="67" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="D64" s="69" t="e">
+      <c r="D64" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="E64" s="69" t="e">
+      <c r="E64" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="F64" s="69" t="e">
+      <c r="F64" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="G64" s="69" t="e">
+      <c r="G64" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="H64" s="69" t="e">
+      <c r="H64" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="I64" s="69" t="e">
+      <c r="I64" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
@@ -7834,31 +7838,31 @@
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="C65" s="68" t="e">
+      <c r="C65" s="67" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="D65" s="69" t="e">
+      <c r="D65" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="E65" s="69" t="e">
+      <c r="E65" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="F65" s="69" t="e">
+      <c r="F65" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="G65" s="69" t="e">
+      <c r="G65" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="H65" s="69" t="e">
+      <c r="H65" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="I65" s="69" t="e">
+      <c r="I65" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
@@ -7883,31 +7887,31 @@
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="C66" s="68" t="e">
+      <c r="C66" s="67" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="D66" s="69" t="e">
+      <c r="D66" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="E66" s="69" t="e">
+      <c r="E66" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="F66" s="69" t="e">
+      <c r="F66" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="G66" s="69" t="e">
+      <c r="G66" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="H66" s="69" t="e">
+      <c r="H66" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="I66" s="69" t="e">
+      <c r="I66" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
@@ -7932,31 +7936,31 @@
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="C67" s="68" t="e">
+      <c r="C67" s="67" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="D67" s="69" t="e">
+      <c r="D67" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="E67" s="69" t="e">
+      <c r="E67" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="F67" s="69" t="e">
+      <c r="F67" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="G67" s="69" t="e">
+      <c r="G67" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="H67" s="69" t="e">
+      <c r="H67" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="I67" s="69" t="e">
+      <c r="I67" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
@@ -7981,31 +7985,31 @@
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="C68" s="68" t="e">
+      <c r="C68" s="67" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="D68" s="69" t="e">
+      <c r="D68" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="E68" s="69" t="e">
+      <c r="E68" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="F68" s="69" t="e">
+      <c r="F68" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="G68" s="69" t="e">
+      <c r="G68" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="H68" s="69" t="e">
+      <c r="H68" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-      <c r="I68" s="69" t="e">
+      <c r="I68" s="68" t="e">
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
@@ -8030,31 +8034,31 @@
         <f t="shared" ref="B69:I79" si="6">VLOOKUP($A69,$A$83:$I$113,B$47,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="C69" s="68" t="e">
+      <c r="C69" s="67" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="D69" s="69" t="e">
+      <c r="D69" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="E69" s="69" t="e">
+      <c r="E69" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="F69" s="69" t="e">
+      <c r="F69" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="G69" s="69" t="e">
+      <c r="G69" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="H69" s="69" t="e">
+      <c r="H69" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="I69" s="69" t="e">
+      <c r="I69" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
@@ -8079,31 +8083,31 @@
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="C70" s="68" t="e">
+      <c r="C70" s="67" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="D70" s="69" t="e">
+      <c r="D70" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="E70" s="69" t="e">
+      <c r="E70" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="F70" s="69" t="e">
+      <c r="F70" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="G70" s="69" t="e">
+      <c r="G70" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="H70" s="69" t="e">
+      <c r="H70" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="I70" s="69" t="e">
+      <c r="I70" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
@@ -8128,31 +8132,31 @@
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="C71" s="68" t="e">
+      <c r="C71" s="67" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="D71" s="69" t="e">
+      <c r="D71" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="E71" s="69" t="e">
+      <c r="E71" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="F71" s="69" t="e">
+      <c r="F71" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="G71" s="69" t="e">
+      <c r="G71" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="H71" s="69" t="e">
+      <c r="H71" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="I71" s="69" t="e">
+      <c r="I71" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
@@ -8177,31 +8181,31 @@
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="C72" s="68" t="e">
+      <c r="C72" s="67" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="D72" s="69" t="e">
+      <c r="D72" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="E72" s="69" t="e">
+      <c r="E72" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="F72" s="69" t="e">
+      <c r="F72" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="G72" s="69" t="e">
+      <c r="G72" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="H72" s="69" t="e">
+      <c r="H72" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="I72" s="69" t="e">
+      <c r="I72" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
@@ -8226,31 +8230,31 @@
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="C73" s="68" t="e">
+      <c r="C73" s="67" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="D73" s="69" t="e">
+      <c r="D73" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="E73" s="69" t="e">
+      <c r="E73" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="F73" s="69" t="e">
+      <c r="F73" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="G73" s="69" t="e">
+      <c r="G73" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="H73" s="69" t="e">
+      <c r="H73" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="I73" s="69" t="e">
+      <c r="I73" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
@@ -8275,31 +8279,31 @@
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="C74" s="68" t="e">
+      <c r="C74" s="67" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="D74" s="69" t="e">
+      <c r="D74" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="E74" s="69" t="e">
+      <c r="E74" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="F74" s="69" t="e">
+      <c r="F74" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="G74" s="69" t="e">
+      <c r="G74" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="H74" s="69" t="e">
+      <c r="H74" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="I74" s="69" t="e">
+      <c r="I74" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
@@ -8324,31 +8328,31 @@
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="C75" s="68" t="e">
+      <c r="C75" s="67" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="D75" s="69" t="e">
+      <c r="D75" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="E75" s="69" t="e">
+      <c r="E75" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="F75" s="69" t="e">
+      <c r="F75" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="G75" s="69" t="e">
+      <c r="G75" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="H75" s="69" t="e">
+      <c r="H75" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="I75" s="69" t="e">
+      <c r="I75" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
@@ -8373,31 +8377,31 @@
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="C76" s="68" t="e">
+      <c r="C76" s="67" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="D76" s="69" t="e">
+      <c r="D76" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="E76" s="69" t="e">
+      <c r="E76" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="F76" s="69" t="e">
+      <c r="F76" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="G76" s="69" t="e">
+      <c r="G76" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="H76" s="69" t="e">
+      <c r="H76" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="I76" s="69" t="e">
+      <c r="I76" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
@@ -8422,31 +8426,31 @@
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="C77" s="68" t="e">
+      <c r="C77" s="67" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="D77" s="69" t="e">
+      <c r="D77" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="E77" s="69" t="e">
+      <c r="E77" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="F77" s="69" t="e">
+      <c r="F77" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="G77" s="69" t="e">
+      <c r="G77" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="H77" s="69" t="e">
+      <c r="H77" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="I77" s="69" t="e">
+      <c r="I77" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
@@ -8471,31 +8475,31 @@
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="C78" s="68" t="e">
+      <c r="C78" s="67" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="D78" s="69" t="e">
+      <c r="D78" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="E78" s="69" t="e">
+      <c r="E78" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="F78" s="69" t="e">
+      <c r="F78" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="G78" s="69" t="e">
+      <c r="G78" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="H78" s="69" t="e">
+      <c r="H78" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="I78" s="69" t="e">
+      <c r="I78" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
@@ -8520,31 +8524,31 @@
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="C79" s="68" t="e">
+      <c r="C79" s="67" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="D79" s="69" t="e">
+      <c r="D79" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="E79" s="69" t="e">
+      <c r="E79" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="F79" s="69" t="e">
+      <c r="F79" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="G79" s="69" t="e">
+      <c r="G79" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="H79" s="69" t="e">
+      <c r="H79" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
-      <c r="I79" s="69" t="e">
+      <c r="I79" s="68" t="e">
         <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
@@ -8563,80 +8567,80 @@
     </row>
     <row r="80" spans="1:12" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B80" s="45"/>
-      <c r="C80" s="70"/>
-      <c r="D80" s="70"/>
-      <c r="E80" s="70"/>
-      <c r="F80" s="70"/>
-      <c r="G80" s="70"/>
-      <c r="H80" s="70"/>
-      <c r="I80" s="70"/>
+      <c r="C80" s="69"/>
+      <c r="D80" s="69"/>
+      <c r="E80" s="69"/>
+      <c r="F80" s="69"/>
+      <c r="G80" s="69"/>
+      <c r="H80" s="69"/>
+      <c r="I80" s="69"/>
     </row>
     <row r="81" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B81" s="15">
         <v>1</v>
       </c>
-      <c r="C81" s="71">
+      <c r="C81" s="70">
         <v>4</v>
       </c>
-      <c r="D81" s="71">
+      <c r="D81" s="70">
         <v>10</v>
       </c>
-      <c r="E81" s="71">
+      <c r="E81" s="70">
         <v>6</v>
       </c>
-      <c r="F81" s="71">
+      <c r="F81" s="70">
         <v>19</v>
       </c>
-      <c r="G81" s="71">
+      <c r="G81" s="70">
         <v>21</v>
       </c>
-      <c r="H81" s="71">
+      <c r="H81" s="70">
         <v>18</v>
       </c>
-      <c r="I81" s="72">
+      <c r="I81" s="71">
         <v>20</v>
       </c>
-      <c r="Q81" s="66"/>
-      <c r="R81" s="66"/>
-      <c r="S81" s="66"/>
-      <c r="T81" s="66"/>
-      <c r="U81" s="66"/>
-      <c r="V81" s="66"/>
-      <c r="W81" s="73"/>
+      <c r="Q81" s="65"/>
+      <c r="R81" s="65"/>
+      <c r="S81" s="65"/>
+      <c r="T81" s="65"/>
+      <c r="U81" s="65"/>
+      <c r="V81" s="65"/>
+      <c r="W81" s="72"/>
     </row>
     <row r="82" spans="1:23" s="15" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B82" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="C82" s="67" t="s">
+      <c r="C82" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="D82" s="67" t="s">
+      <c r="D82" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="E82" s="67" t="s">
+      <c r="E82" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="F82" s="67" t="s">
+      <c r="F82" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="G82" s="67" t="s">
+      <c r="G82" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="H82" s="67" t="s">
+      <c r="H82" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="I82" s="67" t="s">
+      <c r="I82" s="66" t="s">
         <v>56</v>
       </c>
       <c r="P82" s="45"/>
-      <c r="Q82" s="67"/>
-      <c r="R82" s="67"/>
-      <c r="S82" s="67"/>
-      <c r="T82" s="67"/>
-      <c r="U82" s="67"/>
-      <c r="V82" s="67"/>
-      <c r="W82" s="67"/>
+      <c r="Q82" s="66"/>
+      <c r="R82" s="66"/>
+      <c r="S82" s="66"/>
+      <c r="T82" s="66"/>
+      <c r="U82" s="66"/>
+      <c r="V82" s="66"/>
+      <c r="W82" s="66"/>
     </row>
     <row r="83" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="15" t="e">
@@ -8646,35 +8650,35 @@
       <c r="B83" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C83" s="74" t="e">
+      <c r="C83" s="73" t="e">
         <f>VLOOKUP($B83&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D83" s="74">
+      <c r="D83" s="73">
         <v>1</v>
       </c>
-      <c r="E83" s="74" t="e">
+      <c r="E83" s="73" t="e">
         <f>VLOOKUP($B83&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F83" s="74" t="e">
+      <c r="F83" s="73" t="e">
         <f>VLOOKUP($B83&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G83" s="74" t="e">
+      <c r="G83" s="73" t="e">
         <f>VLOOKUP($B83&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H83" s="74" t="e">
+      <c r="H83" s="73" t="e">
         <f>VLOOKUP($B83&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I83" s="74" t="e">
+      <c r="I83" s="73" t="e">
         <f>VLOOKUP($B83&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M83" s="75"/>
-      <c r="N83" s="75"/>
+      <c r="M83" s="74"/>
+      <c r="N83" s="74"/>
     </row>
     <row r="84" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="15" t="e">
@@ -8684,35 +8688,35 @@
       <c r="B84" s="45" t="s">
         <v>107</v>
       </c>
-      <c r="C84" s="74" t="e">
+      <c r="C84" s="73" t="e">
         <f>VLOOKUP($B84&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D84" s="74">
+      <c r="D84" s="73">
         <v>1</v>
       </c>
-      <c r="E84" s="74" t="e">
+      <c r="E84" s="73" t="e">
         <f>VLOOKUP($B84&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F84" s="74" t="e">
+      <c r="F84" s="73" t="e">
         <f>VLOOKUP($B84&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G84" s="74" t="e">
+      <c r="G84" s="73" t="e">
         <f>VLOOKUP($B84&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H84" s="74" t="e">
+      <c r="H84" s="73" t="e">
         <f>VLOOKUP($B84&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I84" s="74" t="e">
+      <c r="I84" s="73" t="e">
         <f>VLOOKUP($B84&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M84" s="75"/>
-      <c r="N84" s="75"/>
+      <c r="M84" s="74"/>
+      <c r="N84" s="74"/>
     </row>
     <row r="85" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="15" t="e">
@@ -8722,35 +8726,35 @@
       <c r="B85" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="C85" s="74" t="e">
+      <c r="C85" s="73" t="e">
         <f>VLOOKUP($B85&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D85" s="74">
+      <c r="D85" s="73">
         <v>1</v>
       </c>
-      <c r="E85" s="74" t="e">
+      <c r="E85" s="73" t="e">
         <f>VLOOKUP($B85&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F85" s="74" t="e">
+      <c r="F85" s="73" t="e">
         <f>VLOOKUP($B85&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G85" s="74" t="e">
+      <c r="G85" s="73" t="e">
         <f>VLOOKUP($B85&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H85" s="74" t="e">
+      <c r="H85" s="73" t="e">
         <f>VLOOKUP($B85&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I85" s="74" t="e">
+      <c r="I85" s="73" t="e">
         <f>VLOOKUP($B85&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M85" s="75"/>
-      <c r="N85" s="75"/>
+      <c r="M85" s="74"/>
+      <c r="N85" s="74"/>
     </row>
     <row r="86" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="15" t="e">
@@ -8760,35 +8764,35 @@
       <c r="B86" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="C86" s="74" t="e">
+      <c r="C86" s="73" t="e">
         <f>VLOOKUP($B86&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D86" s="74">
+      <c r="D86" s="73">
         <v>1</v>
       </c>
-      <c r="E86" s="74" t="e">
+      <c r="E86" s="73" t="e">
         <f>VLOOKUP($B86&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F86" s="74" t="e">
+      <c r="F86" s="73" t="e">
         <f>VLOOKUP($B86&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G86" s="74" t="e">
+      <c r="G86" s="73" t="e">
         <f>VLOOKUP($B86&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H86" s="74" t="e">
+      <c r="H86" s="73" t="e">
         <f>VLOOKUP($B86&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I86" s="74" t="e">
+      <c r="I86" s="73" t="e">
         <f>VLOOKUP($B86&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M86" s="75"/>
-      <c r="N86" s="75"/>
+      <c r="M86" s="74"/>
+      <c r="N86" s="74"/>
     </row>
     <row r="87" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="15" t="e">
@@ -8798,35 +8802,35 @@
       <c r="B87" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="C87" s="74" t="e">
+      <c r="C87" s="73" t="e">
         <f>VLOOKUP($B87&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D87" s="74">
+      <c r="D87" s="73">
         <v>1</v>
       </c>
-      <c r="E87" s="74" t="e">
+      <c r="E87" s="73" t="e">
         <f>VLOOKUP($B87&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F87" s="74" t="e">
+      <c r="F87" s="73" t="e">
         <f>VLOOKUP($B87&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G87" s="74" t="e">
+      <c r="G87" s="73" t="e">
         <f>VLOOKUP($B87&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H87" s="74" t="e">
+      <c r="H87" s="73" t="e">
         <f>VLOOKUP($B87&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I87" s="74" t="e">
+      <c r="I87" s="73" t="e">
         <f>VLOOKUP($B87&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M87" s="75"/>
-      <c r="N87" s="75"/>
+      <c r="M87" s="74"/>
+      <c r="N87" s="74"/>
     </row>
     <row r="88" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="15" t="e">
@@ -8836,35 +8840,35 @@
       <c r="B88" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="C88" s="74" t="e">
+      <c r="C88" s="73" t="e">
         <f>VLOOKUP($B88&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D88" s="74">
+      <c r="D88" s="73">
         <v>1</v>
       </c>
-      <c r="E88" s="74" t="e">
+      <c r="E88" s="73" t="e">
         <f>VLOOKUP($B88&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F88" s="74" t="e">
+      <c r="F88" s="73" t="e">
         <f>VLOOKUP($B88&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G88" s="74" t="e">
+      <c r="G88" s="73" t="e">
         <f>VLOOKUP($B88&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H88" s="74" t="e">
+      <c r="H88" s="73" t="e">
         <f>VLOOKUP($B88&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I88" s="74" t="e">
+      <c r="I88" s="73" t="e">
         <f>VLOOKUP($B88&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M88" s="75"/>
-      <c r="N88" s="75"/>
+      <c r="M88" s="74"/>
+      <c r="N88" s="74"/>
     </row>
     <row r="89" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="15" t="e">
@@ -8874,35 +8878,35 @@
       <c r="B89" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="C89" s="74" t="e">
+      <c r="C89" s="73" t="e">
         <f>VLOOKUP($B89&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D89" s="74">
+      <c r="D89" s="73">
         <v>1</v>
       </c>
-      <c r="E89" s="74" t="e">
+      <c r="E89" s="73" t="e">
         <f>VLOOKUP($B89&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F89" s="74" t="e">
+      <c r="F89" s="73" t="e">
         <f>VLOOKUP($B89&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G89" s="74" t="e">
+      <c r="G89" s="73" t="e">
         <f>VLOOKUP($B89&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H89" s="74" t="e">
+      <c r="H89" s="73" t="e">
         <f>VLOOKUP($B89&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I89" s="74" t="e">
+      <c r="I89" s="73" t="e">
         <f>VLOOKUP($B89&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M89" s="75"/>
-      <c r="N89" s="75"/>
+      <c r="M89" s="74"/>
+      <c r="N89" s="74"/>
     </row>
     <row r="90" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="15" t="e">
@@ -8912,35 +8916,35 @@
       <c r="B90" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="C90" s="74" t="e">
+      <c r="C90" s="73" t="e">
         <f>VLOOKUP($B90&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D90" s="74">
+      <c r="D90" s="73">
         <v>1</v>
       </c>
-      <c r="E90" s="74" t="e">
+      <c r="E90" s="73" t="e">
         <f>VLOOKUP($B90&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F90" s="74" t="e">
+      <c r="F90" s="73" t="e">
         <f>VLOOKUP($B90&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G90" s="74" t="e">
+      <c r="G90" s="73" t="e">
         <f>VLOOKUP($B90&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H90" s="74" t="e">
+      <c r="H90" s="73" t="e">
         <f>VLOOKUP($B90&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I90" s="74" t="e">
+      <c r="I90" s="73" t="e">
         <f>VLOOKUP($B90&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M90" s="75"/>
-      <c r="N90" s="75"/>
+      <c r="M90" s="74"/>
+      <c r="N90" s="74"/>
     </row>
     <row r="91" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="15" t="e">
@@ -8950,35 +8954,35 @@
       <c r="B91" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C91" s="74" t="e">
+      <c r="C91" s="73" t="e">
         <f>VLOOKUP($B91&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D91" s="74">
+      <c r="D91" s="73">
         <v>1</v>
       </c>
-      <c r="E91" s="74" t="e">
+      <c r="E91" s="73" t="e">
         <f>VLOOKUP($B91&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F91" s="74" t="e">
+      <c r="F91" s="73" t="e">
         <f>VLOOKUP($B91&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G91" s="74" t="e">
+      <c r="G91" s="73" t="e">
         <f>VLOOKUP($B91&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H91" s="74" t="e">
+      <c r="H91" s="73" t="e">
         <f>VLOOKUP($B91&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I91" s="74" t="e">
+      <c r="I91" s="73" t="e">
         <f>VLOOKUP($B91&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M91" s="75"/>
-      <c r="N91" s="75"/>
+      <c r="M91" s="74"/>
+      <c r="N91" s="74"/>
     </row>
     <row r="92" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="15" t="e">
@@ -8988,35 +8992,35 @@
       <c r="B92" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="C92" s="74" t="e">
+      <c r="C92" s="73" t="e">
         <f>VLOOKUP($B92&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D92" s="74">
+      <c r="D92" s="73">
         <v>1</v>
       </c>
-      <c r="E92" s="74" t="e">
+      <c r="E92" s="73" t="e">
         <f>VLOOKUP($B92&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F92" s="74" t="e">
+      <c r="F92" s="73" t="e">
         <f>VLOOKUP($B92&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G92" s="74" t="e">
+      <c r="G92" s="73" t="e">
         <f>VLOOKUP($B92&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H92" s="74" t="e">
+      <c r="H92" s="73" t="e">
         <f>VLOOKUP($B92&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I92" s="74" t="e">
+      <c r="I92" s="73" t="e">
         <f>VLOOKUP($B92&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M92" s="75"/>
-      <c r="N92" s="75"/>
+      <c r="M92" s="74"/>
+      <c r="N92" s="74"/>
     </row>
     <row r="93" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="15" t="e">
@@ -9026,35 +9030,35 @@
       <c r="B93" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="C93" s="74" t="e">
+      <c r="C93" s="73" t="e">
         <f>VLOOKUP($B93&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D93" s="74">
+      <c r="D93" s="73">
         <v>1</v>
       </c>
-      <c r="E93" s="74" t="e">
+      <c r="E93" s="73" t="e">
         <f>VLOOKUP($B93&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F93" s="74" t="e">
+      <c r="F93" s="73" t="e">
         <f>VLOOKUP($B93&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G93" s="74" t="e">
+      <c r="G93" s="73" t="e">
         <f>VLOOKUP($B93&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H93" s="74" t="e">
+      <c r="H93" s="73" t="e">
         <f>VLOOKUP($B93&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I93" s="74" t="e">
+      <c r="I93" s="73" t="e">
         <f>VLOOKUP($B93&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M93" s="75"/>
-      <c r="N93" s="75"/>
+      <c r="M93" s="74"/>
+      <c r="N93" s="74"/>
     </row>
     <row r="94" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="15" t="e">
@@ -9064,35 +9068,35 @@
       <c r="B94" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="C94" s="74" t="e">
+      <c r="C94" s="73" t="e">
         <f>VLOOKUP($B94&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D94" s="74">
+      <c r="D94" s="73">
         <v>1</v>
       </c>
-      <c r="E94" s="74" t="e">
+      <c r="E94" s="73" t="e">
         <f>VLOOKUP($B94&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F94" s="74" t="e">
+      <c r="F94" s="73" t="e">
         <f>VLOOKUP($B94&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G94" s="74" t="e">
+      <c r="G94" s="73" t="e">
         <f>VLOOKUP($B94&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H94" s="74" t="e">
+      <c r="H94" s="73" t="e">
         <f>VLOOKUP($B94&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I94" s="74" t="e">
+      <c r="I94" s="73" t="e">
         <f>VLOOKUP($B94&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M94" s="75"/>
-      <c r="N94" s="75"/>
+      <c r="M94" s="74"/>
+      <c r="N94" s="74"/>
     </row>
     <row r="95" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="15" t="e">
@@ -9102,35 +9106,35 @@
       <c r="B95" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="C95" s="74" t="e">
+      <c r="C95" s="73" t="e">
         <f>VLOOKUP($B95&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D95" s="74">
+      <c r="D95" s="73">
         <v>1</v>
       </c>
-      <c r="E95" s="74" t="e">
+      <c r="E95" s="73" t="e">
         <f>VLOOKUP($B95&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F95" s="74" t="e">
+      <c r="F95" s="73" t="e">
         <f>VLOOKUP($B95&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G95" s="74" t="e">
+      <c r="G95" s="73" t="e">
         <f>VLOOKUP($B95&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H95" s="74" t="e">
+      <c r="H95" s="73" t="e">
         <f>VLOOKUP($B95&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I95" s="74" t="e">
+      <c r="I95" s="73" t="e">
         <f>VLOOKUP($B95&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M95" s="75"/>
-      <c r="N95" s="75"/>
+      <c r="M95" s="74"/>
+      <c r="N95" s="74"/>
     </row>
     <row r="96" spans="1:23" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="15" t="e">
@@ -9140,35 +9144,35 @@
       <c r="B96" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="C96" s="74" t="e">
+      <c r="C96" s="73" t="e">
         <f>VLOOKUP($B96&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D96" s="74">
+      <c r="D96" s="73">
         <v>1</v>
       </c>
-      <c r="E96" s="74" t="e">
+      <c r="E96" s="73" t="e">
         <f>VLOOKUP($B96&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F96" s="74" t="e">
+      <c r="F96" s="73" t="e">
         <f>VLOOKUP($B96&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G96" s="74" t="e">
+      <c r="G96" s="73" t="e">
         <f>VLOOKUP($B96&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H96" s="74" t="e">
+      <c r="H96" s="73" t="e">
         <f>VLOOKUP($B96&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I96" s="74" t="e">
+      <c r="I96" s="73" t="e">
         <f>VLOOKUP($B96&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M96" s="75"/>
-      <c r="N96" s="75"/>
+      <c r="M96" s="74"/>
+      <c r="N96" s="74"/>
     </row>
     <row r="97" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="15" t="e">
@@ -9178,35 +9182,35 @@
       <c r="B97" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="C97" s="74" t="e">
+      <c r="C97" s="73" t="e">
         <f>VLOOKUP($B97&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D97" s="74">
+      <c r="D97" s="73">
         <v>1</v>
       </c>
-      <c r="E97" s="74" t="e">
+      <c r="E97" s="73" t="e">
         <f>VLOOKUP($B97&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F97" s="74" t="e">
+      <c r="F97" s="73" t="e">
         <f>VLOOKUP($B97&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G97" s="74" t="e">
+      <c r="G97" s="73" t="e">
         <f>VLOOKUP($B97&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H97" s="74" t="e">
+      <c r="H97" s="73" t="e">
         <f>VLOOKUP($B97&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I97" s="74" t="e">
+      <c r="I97" s="73" t="e">
         <f>VLOOKUP($B97&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M97" s="75"/>
-      <c r="N97" s="75"/>
+      <c r="M97" s="74"/>
+      <c r="N97" s="74"/>
     </row>
     <row r="98" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="15" t="e">
@@ -9216,35 +9220,35 @@
       <c r="B98" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="C98" s="74" t="e">
+      <c r="C98" s="73" t="e">
         <f>VLOOKUP($B98&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D98" s="74">
+      <c r="D98" s="73">
         <v>1</v>
       </c>
-      <c r="E98" s="74" t="e">
+      <c r="E98" s="73" t="e">
         <f>VLOOKUP($B98&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F98" s="74" t="e">
+      <c r="F98" s="73" t="e">
         <f>VLOOKUP($B98&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G98" s="74" t="e">
+      <c r="G98" s="73" t="e">
         <f>VLOOKUP($B98&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H98" s="74" t="e">
+      <c r="H98" s="73" t="e">
         <f>VLOOKUP($B98&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I98" s="74" t="e">
+      <c r="I98" s="73" t="e">
         <f>VLOOKUP($B98&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M98" s="75"/>
-      <c r="N98" s="75"/>
+      <c r="M98" s="74"/>
+      <c r="N98" s="74"/>
     </row>
     <row r="99" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="15" t="e">
@@ -9254,35 +9258,35 @@
       <c r="B99" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="C99" s="74" t="e">
+      <c r="C99" s="73" t="e">
         <f>VLOOKUP($B99&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D99" s="74">
+      <c r="D99" s="73">
         <v>1</v>
       </c>
-      <c r="E99" s="74" t="e">
+      <c r="E99" s="73" t="e">
         <f>VLOOKUP($B99&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F99" s="74" t="e">
+      <c r="F99" s="73" t="e">
         <f>VLOOKUP($B99&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G99" s="74" t="e">
+      <c r="G99" s="73" t="e">
         <f>VLOOKUP($B99&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H99" s="74" t="e">
+      <c r="H99" s="73" t="e">
         <f>VLOOKUP($B99&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I99" s="74" t="e">
+      <c r="I99" s="73" t="e">
         <f>VLOOKUP($B99&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M99" s="75"/>
-      <c r="N99" s="75"/>
+      <c r="M99" s="74"/>
+      <c r="N99" s="74"/>
     </row>
     <row r="100" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="15" t="e">
@@ -9292,35 +9296,35 @@
       <c r="B100" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="C100" s="74" t="e">
+      <c r="C100" s="73" t="e">
         <f>VLOOKUP($B100&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D100" s="74">
+      <c r="D100" s="73">
         <v>1</v>
       </c>
-      <c r="E100" s="74" t="e">
+      <c r="E100" s="73" t="e">
         <f>VLOOKUP($B100&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F100" s="74" t="e">
+      <c r="F100" s="73" t="e">
         <f>VLOOKUP($B100&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G100" s="74" t="e">
+      <c r="G100" s="73" t="e">
         <f>VLOOKUP($B100&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H100" s="74" t="e">
+      <c r="H100" s="73" t="e">
         <f>VLOOKUP($B100&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I100" s="74" t="e">
+      <c r="I100" s="73" t="e">
         <f>VLOOKUP($B100&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M100" s="75"/>
-      <c r="N100" s="75"/>
+      <c r="M100" s="74"/>
+      <c r="N100" s="74"/>
     </row>
     <row r="101" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A101" s="15" t="e">
@@ -9330,35 +9334,35 @@
       <c r="B101" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="C101" s="74" t="e">
+      <c r="C101" s="73" t="e">
         <f>VLOOKUP($B101&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D101" s="74">
+      <c r="D101" s="73">
         <v>1</v>
       </c>
-      <c r="E101" s="74" t="e">
+      <c r="E101" s="73" t="e">
         <f>VLOOKUP($B101&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F101" s="74" t="e">
+      <c r="F101" s="73" t="e">
         <f>VLOOKUP($B101&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G101" s="74" t="e">
+      <c r="G101" s="73" t="e">
         <f>VLOOKUP($B101&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H101" s="74" t="e">
+      <c r="H101" s="73" t="e">
         <f>VLOOKUP($B101&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I101" s="74" t="e">
+      <c r="I101" s="73" t="e">
         <f>VLOOKUP($B101&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M101" s="75"/>
-      <c r="N101" s="75"/>
+      <c r="M101" s="74"/>
+      <c r="N101" s="74"/>
     </row>
     <row r="102" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="15" t="e">
@@ -9368,35 +9372,35 @@
       <c r="B102" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="C102" s="74" t="e">
+      <c r="C102" s="73" t="e">
         <f>VLOOKUP($B102&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D102" s="74">
+      <c r="D102" s="73">
         <v>1</v>
       </c>
-      <c r="E102" s="74" t="e">
+      <c r="E102" s="73" t="e">
         <f>VLOOKUP($B102&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F102" s="74" t="e">
+      <c r="F102" s="73" t="e">
         <f>VLOOKUP($B102&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G102" s="74" t="e">
+      <c r="G102" s="73" t="e">
         <f>VLOOKUP($B102&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H102" s="74" t="e">
+      <c r="H102" s="73" t="e">
         <f>VLOOKUP($B102&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I102" s="74" t="e">
+      <c r="I102" s="73" t="e">
         <f>VLOOKUP($B102&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M102" s="75"/>
-      <c r="N102" s="75"/>
+      <c r="M102" s="74"/>
+      <c r="N102" s="74"/>
     </row>
     <row r="103" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" s="15" t="e">
@@ -9406,35 +9410,35 @@
       <c r="B103" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="C103" s="74" t="e">
+      <c r="C103" s="73" t="e">
         <f>VLOOKUP($B103&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D103" s="74">
+      <c r="D103" s="73">
         <v>1</v>
       </c>
-      <c r="E103" s="74" t="e">
+      <c r="E103" s="73" t="e">
         <f>VLOOKUP($B103&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F103" s="74" t="e">
+      <c r="F103" s="73" t="e">
         <f>VLOOKUP($B103&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G103" s="74" t="e">
+      <c r="G103" s="73" t="e">
         <f>VLOOKUP($B103&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H103" s="74" t="e">
+      <c r="H103" s="73" t="e">
         <f>VLOOKUP($B103&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I103" s="74" t="e">
+      <c r="I103" s="73" t="e">
         <f>VLOOKUP($B103&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M103" s="75"/>
-      <c r="N103" s="75"/>
+      <c r="M103" s="74"/>
+      <c r="N103" s="74"/>
     </row>
     <row r="104" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A104" s="15" t="e">
@@ -9444,35 +9448,35 @@
       <c r="B104" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="C104" s="74" t="e">
+      <c r="C104" s="73" t="e">
         <f>VLOOKUP($B104&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D104" s="74">
+      <c r="D104" s="73">
         <v>1</v>
       </c>
-      <c r="E104" s="74" t="e">
+      <c r="E104" s="73" t="e">
         <f>VLOOKUP($B104&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F104" s="74" t="e">
+      <c r="F104" s="73" t="e">
         <f>VLOOKUP($B104&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G104" s="74" t="e">
+      <c r="G104" s="73" t="e">
         <f>VLOOKUP($B104&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H104" s="74" t="e">
+      <c r="H104" s="73" t="e">
         <f>VLOOKUP($B104&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I104" s="74" t="e">
+      <c r="I104" s="73" t="e">
         <f>VLOOKUP($B104&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M104" s="75"/>
-      <c r="N104" s="75"/>
+      <c r="M104" s="74"/>
+      <c r="N104" s="74"/>
     </row>
     <row r="105" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A105" s="15" t="e">
@@ -9482,35 +9486,35 @@
       <c r="B105" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="C105" s="74" t="e">
+      <c r="C105" s="73" t="e">
         <f>VLOOKUP($B105&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D105" s="74">
+      <c r="D105" s="73">
         <v>1</v>
       </c>
-      <c r="E105" s="74" t="e">
+      <c r="E105" s="73" t="e">
         <f>VLOOKUP($B105&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F105" s="74" t="e">
+      <c r="F105" s="73" t="e">
         <f>VLOOKUP($B105&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G105" s="74" t="e">
+      <c r="G105" s="73" t="e">
         <f>VLOOKUP($B105&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H105" s="74" t="e">
+      <c r="H105" s="73" t="e">
         <f>VLOOKUP($B105&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I105" s="74" t="e">
+      <c r="I105" s="73" t="e">
         <f>VLOOKUP($B105&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M105" s="75"/>
-      <c r="N105" s="75"/>
+      <c r="M105" s="74"/>
+      <c r="N105" s="74"/>
     </row>
     <row r="106" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A106" s="15" t="e">
@@ -9520,35 +9524,35 @@
       <c r="B106" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="C106" s="74" t="e">
+      <c r="C106" s="73" t="e">
         <f>VLOOKUP($B106&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D106" s="74">
+      <c r="D106" s="73">
         <v>1</v>
       </c>
-      <c r="E106" s="74" t="e">
+      <c r="E106" s="73" t="e">
         <f>VLOOKUP($B106&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F106" s="74" t="e">
+      <c r="F106" s="73" t="e">
         <f>VLOOKUP($B106&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G106" s="74" t="e">
+      <c r="G106" s="73" t="e">
         <f>VLOOKUP($B106&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H106" s="74" t="e">
+      <c r="H106" s="73" t="e">
         <f>VLOOKUP($B106&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I106" s="74" t="e">
+      <c r="I106" s="73" t="e">
         <f>VLOOKUP($B106&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M106" s="75"/>
-      <c r="N106" s="75"/>
+      <c r="M106" s="74"/>
+      <c r="N106" s="74"/>
     </row>
     <row r="107" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A107" s="15" t="e">
@@ -9558,35 +9562,35 @@
       <c r="B107" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C107" s="74" t="e">
+      <c r="C107" s="73" t="e">
         <f>VLOOKUP($B107&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D107" s="74">
+      <c r="D107" s="73">
         <v>1</v>
       </c>
-      <c r="E107" s="74" t="e">
+      <c r="E107" s="73" t="e">
         <f>VLOOKUP($B107&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F107" s="74" t="e">
+      <c r="F107" s="73" t="e">
         <f>VLOOKUP($B107&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G107" s="74" t="e">
+      <c r="G107" s="73" t="e">
         <f>VLOOKUP($B107&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H107" s="74" t="e">
+      <c r="H107" s="73" t="e">
         <f>VLOOKUP($B107&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I107" s="74" t="e">
+      <c r="I107" s="73" t="e">
         <f>VLOOKUP($B107&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M107" s="75"/>
-      <c r="N107" s="75"/>
+      <c r="M107" s="74"/>
+      <c r="N107" s="74"/>
     </row>
     <row r="108" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A108" s="15" t="e">
@@ -9596,35 +9600,35 @@
       <c r="B108" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="C108" s="74" t="e">
+      <c r="C108" s="73" t="e">
         <f>VLOOKUP($B108&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D108" s="74">
+      <c r="D108" s="73">
         <v>1</v>
       </c>
-      <c r="E108" s="74" t="e">
+      <c r="E108" s="73" t="e">
         <f>VLOOKUP($B108&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F108" s="74" t="e">
+      <c r="F108" s="73" t="e">
         <f>VLOOKUP($B108&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G108" s="74" t="e">
+      <c r="G108" s="73" t="e">
         <f>VLOOKUP($B108&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H108" s="74" t="e">
+      <c r="H108" s="73" t="e">
         <f>VLOOKUP($B108&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I108" s="74" t="e">
+      <c r="I108" s="73" t="e">
         <f>VLOOKUP($B108&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="M108" s="75"/>
-      <c r="N108" s="75"/>
+      <c r="M108" s="74"/>
+      <c r="N108" s="74"/>
     </row>
     <row r="109" spans="1:14" s="15" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A109" s="15" t="e">
@@ -9634,30 +9638,30 @@
       <c r="B109" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="C109" s="74" t="e">
+      <c r="C109" s="73" t="e">
         <f>VLOOKUP($B109&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D109" s="74">
+      <c r="D109" s="73">
         <v>1</v>
       </c>
-      <c r="E109" s="74" t="e">
+      <c r="E109" s="73" t="e">
         <f>VLOOKUP($B109&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F109" s="74" t="e">
+      <c r="F109" s="73" t="e">
         <f>VLOOKUP($B109&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G109" s="74" t="e">
+      <c r="G109" s="73" t="e">
         <f>VLOOKUP($B109&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H109" s="74" t="e">
+      <c r="H109" s="73" t="e">
         <f>VLOOKUP($B109&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I109" s="74" t="e">
+      <c r="I109" s="73" t="e">
         <f>VLOOKUP($B109&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
@@ -9670,30 +9674,30 @@
       <c r="B110" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="C110" s="74" t="e">
+      <c r="C110" s="73" t="e">
         <f>VLOOKUP($B110&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D110" s="74">
+      <c r="D110" s="73">
         <v>1</v>
       </c>
-      <c r="E110" s="74" t="e">
+      <c r="E110" s="73" t="e">
         <f>VLOOKUP($B110&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F110" s="74" t="e">
+      <c r="F110" s="73" t="e">
         <f>VLOOKUP($B110&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G110" s="74" t="e">
+      <c r="G110" s="73" t="e">
         <f>VLOOKUP($B110&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H110" s="74" t="e">
+      <c r="H110" s="73" t="e">
         <f>VLOOKUP($B110&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I110" s="74" t="e">
+      <c r="I110" s="73" t="e">
         <f>VLOOKUP($B110&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
@@ -9706,30 +9710,30 @@
       <c r="B111" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C111" s="74" t="e">
+      <c r="C111" s="73" t="e">
         <f>VLOOKUP($B111&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D111" s="74">
+      <c r="D111" s="73">
         <v>1</v>
       </c>
-      <c r="E111" s="74" t="e">
+      <c r="E111" s="73" t="e">
         <f>VLOOKUP($B111&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F111" s="74" t="e">
+      <c r="F111" s="73" t="e">
         <f>VLOOKUP($B111&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G111" s="74" t="e">
+      <c r="G111" s="73" t="e">
         <f>VLOOKUP($B111&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H111" s="74" t="e">
+      <c r="H111" s="73" t="e">
         <f>VLOOKUP($B111&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I111" s="74" t="e">
+      <c r="I111" s="73" t="e">
         <f>VLOOKUP($B111&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
@@ -9742,30 +9746,30 @@
       <c r="B112" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C112" s="74" t="e">
+      <c r="C112" s="73" t="e">
         <f>VLOOKUP($B112&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D112" s="74">
+      <c r="D112" s="73">
         <v>1</v>
       </c>
-      <c r="E112" s="74" t="e">
+      <c r="E112" s="73" t="e">
         <f>VLOOKUP($B112&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F112" s="74" t="e">
+      <c r="F112" s="73" t="e">
         <f>VLOOKUP($B112&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G112" s="74" t="e">
+      <c r="G112" s="73" t="e">
         <f>VLOOKUP($B112&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H112" s="74" t="e">
+      <c r="H112" s="73" t="e">
         <f>VLOOKUP($B112&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I112" s="74" t="e">
+      <c r="I112" s="73" t="e">
         <f>VLOOKUP($B112&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>
@@ -9778,30 +9782,30 @@
       <c r="B113" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C113" s="74" t="e">
+      <c r="C113" s="73" t="e">
         <f>VLOOKUP($B113&amp;"3",funnel_data!$A:$X,C$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="D113" s="74">
+      <c r="D113" s="73">
         <v>1</v>
       </c>
-      <c r="E113" s="74" t="e">
+      <c r="E113" s="73" t="e">
         <f>VLOOKUP($B113&amp;"3",funnel_data!$A:$X,E$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F113" s="74" t="e">
+      <c r="F113" s="73" t="e">
         <f>VLOOKUP($B113&amp;"3",funnel_data!$A:$X,F$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="G113" s="74" t="e">
+      <c r="G113" s="73" t="e">
         <f>VLOOKUP($B113&amp;"3",funnel_data!$A:$X,G$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="H113" s="74" t="e">
+      <c r="H113" s="73" t="e">
         <f>VLOOKUP($B113&amp;"3",funnel_data!$A:$X,H$81,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="I113" s="74" t="e">
+      <c r="I113" s="73" t="e">
         <f>VLOOKUP($B113&amp;"3",funnel_data!$A:$X,I$81,FALSE)</f>
         <v>#N/A</v>
       </c>

</xml_diff>

<commit_message>
Update Table 1 template
Match chart formatting in report more closely
Use HSMR instead of SMR in table
</commit_message>
<xml_diff>
--- a/reference_files/Table1-HSMR.xlsx
+++ b/reference_files/Table1-HSMR.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Isdsf00d03\quality_indicators\hsmr\quarter_cycle\Analyst folders\Scott\Updates\hsmr-pra\reference_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Isdsf00d03\quality_indicators\hsmr\quarter_cycle\Analyst folders\Scott\hsmr-pra\reference_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="123">
   <si>
     <t>V217H</t>
   </si>
@@ -377,9 +377,6 @@
     <t>S08000032</t>
   </si>
   <si>
-    <t>SMR</t>
-  </si>
-  <si>
     <t>R103H</t>
   </si>
   <si>
@@ -392,7 +389,16 @@
     <t>Crude mortality rate (%)</t>
   </si>
   <si>
-    <t>Standardised mortality ratio (SMR)</t>
+    <t>Upper/Lower Control Limit</t>
+  </si>
+  <si>
+    <t>Upper/Lower Warning Limit</t>
+  </si>
+  <si>
+    <t>Hospital</t>
+  </si>
+  <si>
+    <t>Hospital standardised mortality ratio</t>
   </si>
 </sst>
 </file>
@@ -847,7 +853,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.18065674656856839"/>
+          <c:y val="7.4569108553029867E-2"/>
+          <c:w val="0.79497565542219628"/>
+          <c:h val="0.80981947066552462"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
@@ -855,7 +871,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Scotland SMR</c:v>
+            <c:v>Scotland</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -1089,7 +1105,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>UCL</c:v>
+                  <c:v>Upper/Lower Control Limit</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1563,7 +1579,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>UWL</c:v>
+                  <c:v>Upper/Lower Warning Limit</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2041,7 +2057,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>SMR</c:v>
+                  <c:v>Hospital</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2826,6 +2842,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.4529003753714495"/>
+              <c:y val="0.9483877585797118"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2911,7 +2935,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -2935,11 +2959,34 @@
                     <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:rPr>
-                  <a:t>Standardised mortality ratio</a:t>
+                  <a:t>Hospital Standardised Mortality</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>Ratio</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0"/>
+              <c:y val="0.38168338587514622"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2949,7 +2996,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -3016,7 +3063,15 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="t"/>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="4"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
       <c:legendEntry>
         <c:idx val="6"/>
         <c:delete val="1"/>
@@ -3025,6 +3080,16 @@
         <c:idx val="7"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.18100474955153228"/>
+          <c:y val="0"/>
+          <c:w val="0.807629521338878"/>
+          <c:h val="5.6771783925344287E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4535,9 +4600,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AA83"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4552,7 +4615,7 @@
       <c r="A1" s="47"/>
       <c r="B1" s="8"/>
       <c r="C1" s="75" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D1" s="75"/>
       <c r="E1" s="75"/>
@@ -4615,8 +4678,8 @@
       <c r="A4" s="47"/>
       <c r="B4" s="8"/>
       <c r="C4" s="14" t="str">
-        <f>"Hospital standardised mortality ratio (funnel plot) "&amp;B5</f>
-        <v xml:space="preserve">Hospital standardised mortality ratio (funnel plot) </v>
+        <f>"Hospital standardised mortality ratio "&amp;B5</f>
+        <v xml:space="preserve">Hospital standardised mortality ratio </v>
       </c>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
@@ -4669,13 +4732,13 @@
         <v>101</v>
       </c>
       <c r="F10" s="43" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="G10" s="43" t="s">
         <v>102</v>
       </c>
       <c r="H10" s="43" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
@@ -5809,10 +5872,10 @@
         <v>58</v>
       </c>
       <c r="B48" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="C48" s="33" t="s">
         <v>116</v>
-      </c>
-      <c r="C48" s="33" t="s">
-        <v>117</v>
       </c>
       <c r="D48" s="40" t="e">
         <f>VLOOKUP($B48&amp;$A$5,'Raw Data'!$A:$X,3,FALSE)</f>
@@ -6204,9 +6267,7 @@
   </sheetPr>
   <dimension ref="A1:AK119"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AL30" sqref="AL30"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6224,7 +6285,7 @@
     <row r="1" spans="1:36" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
       <c r="B1" s="75" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C1" s="75"/>
       <c r="D1" s="75"/>
@@ -6300,8 +6361,8 @@
     <row r="4" spans="1:36" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="14" t="str">
-        <f>"Hospital standardised mortality ratio (funnel plot): " &amp; period_lookup!A1</f>
-        <v>Hospital standardised mortality ratio (funnel plot): 0</v>
+        <f>"Hospital standardised mortality ratio: " &amp; period_lookup!A1</f>
+        <v>Hospital standardised mortality ratio: 0</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
@@ -14269,9 +14330,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AM80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:AM80"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -14592,16 +14651,16 @@
         <v>57</v>
       </c>
       <c r="E8" s="66" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="F8" s="66" t="s">
-        <v>53</v>
+        <v>119</v>
       </c>
       <c r="G8" s="66" t="s">
         <v>54</v>
       </c>
       <c r="H8" s="66" t="s">
-        <v>55</v>
+        <v>120</v>
       </c>
       <c r="I8" s="66" t="s">
         <v>56</v>
@@ -17292,7 +17351,7 @@
         <v>#N/A</v>
       </c>
       <c r="B45" s="45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C45" s="73" t="e">
         <f>VLOOKUP($B45&amp;"3",'Raw Data'!$A:$X,C$41,FALSE)</f>
@@ -19531,10 +19590,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>116</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>117</v>
       </c>
       <c r="G4" s="5"/>
     </row>

</xml_diff>

<commit_message>
Updated funnel plot to highlight below LWL and LCL
</commit_message>
<xml_diff>
--- a/reference_files/Table1-HSMR.xlsx
+++ b/reference_files/Table1-HSMR.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Isdsf00d03\quality_indicators\hsmr\quarter_cycle\Analyst folders\Scott\hsmr-pra\reference_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\stats\ScotPHO\1.Analysts_space\Catherine\hsmr-pra\reference_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4226CB51-B668-44B3-B938-07D51D6ACD50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="4350" windowWidth="15600" windowHeight="4395" tabRatio="837"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="837" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="49" r:id="rId1"/>
@@ -25,12 +26,23 @@
     <definedName name="SPSS" localSheetId="1">#REF!</definedName>
     <definedName name="SPSS">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="129">
   <si>
     <t>V217H</t>
   </si>
@@ -400,17 +412,35 @@
   <si>
     <t>Hospital standardised mortality ratio</t>
   </si>
+  <si>
+    <t>outliers4</t>
+  </si>
+  <si>
+    <t>outliers5</t>
+  </si>
+  <si>
+    <t>ucl</t>
+  </si>
+  <si>
+    <t>uwl</t>
+  </si>
+  <si>
+    <t>lwl</t>
+  </si>
+  <si>
+    <t>lcl</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#.00"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -572,6 +602,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -748,7 +785,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="23" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="3" borderId="4" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
@@ -760,10 +796,11 @@
     <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="14" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -790,15 +827,35 @@
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 3" xfId="2"/>
-    <cellStyle name="Normal 4" xfId="3"/>
-    <cellStyle name="Normal 5" xfId="4"/>
-    <cellStyle name="Normal 6" xfId="5"/>
-    <cellStyle name="Normal_Book1" xfId="6"/>
-    <cellStyle name="Percent 2" xfId="7"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 4" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 5" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 6" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal_Book1" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Percent 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFC00000"/>
@@ -816,11 +873,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFFFC000"/>
+        <color theme="9"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2316,13 +2373,15 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="C00000"/>
               </a:solidFill>
               <a:ln w="9525">
-                <a:noFill/>
+                <a:solidFill>
+                  <a:srgbClr val="C00000"/>
+                </a:solidFill>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -2561,15 +2620,15 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln w="9525">
-                <a:noFill/>
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -2782,6 +2841,502 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-EFA1-4C28-B48F-8742FE2712E8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>funnel_lookup!$M$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>outliers4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>funnel_lookup!$C$9:$C$39</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>funnel_lookup!$M$9:$M$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E410-43DF-BEAB-DEF044A089A3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>funnel_lookup!$N$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>outliers5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="C00000">
+                    <a:alpha val="94000"/>
+                  </a:srgbClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>funnel_lookup!$C$9:$C$39</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>funnel_lookup!$N$9:$N$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E410-43DF-BEAB-DEF044A089A3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3080,13 +3635,21 @@
         <c:idx val="7"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="8"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="9"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.18100474955153228"/>
           <c:y val="0"/>
-          <c:w val="0.807629521338878"/>
+          <c:w val="0.8166525892899773"/>
           <c:h val="5.6771783925344287E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -3721,7 +4284,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -4207,17 +4776,6 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="1">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t/>
-          </a:r>
           <a:br>
             <a:rPr lang="en-GB" sz="1000" b="1">
               <a:solidFill>
@@ -4238,17 +4796,6 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="1">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t/>
-          </a:r>
           <a:br>
             <a:rPr lang="en-GB" sz="1000" b="1">
               <a:solidFill>
@@ -4292,7 +4839,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4386,6 +4939,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -4421,6 +4991,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4596,7 +5183,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AA83"/>
   <sheetViews>
@@ -6261,13 +6848,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet21">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AK119"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AZ22" sqref="AZ22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6482,7 +7071,7 @@
     </row>
     <row r="31" spans="3:37" x14ac:dyDescent="0.2">
       <c r="M31" s="17"/>
-      <c r="AH31" s="63"/>
+      <c r="AH31" s="62"/>
     </row>
     <row r="32" spans="3:37" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C32" s="15">
@@ -6578,134 +7167,134 @@
       <c r="AG32" s="15">
         <v>31</v>
       </c>
-      <c r="AH32" s="64"/>
+      <c r="AH32" s="63"/>
     </row>
     <row r="33" spans="1:37" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C33" s="19" t="e">
-        <f>VLOOKUP(C$32,funnel_lookup!$A$9:$J$39,10)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D33" s="19" t="e">
-        <f>VLOOKUP(D$32,funnel_lookup!$A$9:$J$39,10)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E33" s="19" t="e">
-        <f>VLOOKUP(E$32,funnel_lookup!$A$9:$J$39,10)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F33" s="19" t="e">
-        <f>VLOOKUP(F$32,funnel_lookup!$A$9:$J$39,10)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G33" s="19" t="e">
-        <f>VLOOKUP(G$32,funnel_lookup!$A$9:$J$39,10)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H33" s="19" t="e">
-        <f>VLOOKUP(H$32,funnel_lookup!$A$9:$J$39,10)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I33" s="19" t="e">
-        <f>VLOOKUP(I$32,funnel_lookup!$A$9:$J$39,10)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J33" s="19" t="e">
-        <f>VLOOKUP(J$32,funnel_lookup!$A$9:$J$39,10)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K33" s="19" t="e">
-        <f>VLOOKUP(K$32,funnel_lookup!$A$9:$J$39,10)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L33" s="19" t="e">
-        <f>VLOOKUP(L$32,funnel_lookup!$A$9:$J$39,10)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M33" s="19" t="e">
-        <f>VLOOKUP(M$32,funnel_lookup!$A$9:$J$39,10)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N33" s="19" t="e">
-        <f>VLOOKUP(N$32,funnel_lookup!$A$9:$J$39,10)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O33" s="19" t="e">
-        <f>VLOOKUP(O$32,funnel_lookup!$A$9:$J$39,10)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P33" s="19" t="e">
-        <f>VLOOKUP(P$32,funnel_lookup!$A$9:$J$39,10)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q33" s="19" t="e">
-        <f>VLOOKUP(Q$32,funnel_lookup!$A$9:$J$39,10)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R33" s="19" t="e">
-        <f>VLOOKUP(R$32,funnel_lookup!$A$9:$J$39,10)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S33" s="19" t="e">
-        <f>VLOOKUP(S$32,funnel_lookup!$A$9:$J$39,10)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="T33" s="19" t="e">
-        <f>VLOOKUP(T$32,funnel_lookup!$A$9:$J$39,10)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="U33" s="19" t="e">
-        <f>VLOOKUP(U$32,funnel_lookup!$A$9:$J$39,10)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="V33" s="19" t="e">
-        <f>VLOOKUP(V$32,funnel_lookup!$A$9:$J$39,10)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="W33" s="19" t="e">
-        <f>VLOOKUP(W$32,funnel_lookup!$A$9:$J$39,10)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X33" s="19" t="e">
-        <f>VLOOKUP(X$32,funnel_lookup!$A$9:$J$39,10)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Y33" s="19" t="e">
-        <f>VLOOKUP(Y$32,funnel_lookup!$A$9:$J$39,10)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Z33" s="19" t="e">
-        <f>VLOOKUP(Z$32,funnel_lookup!$A$9:$J$39,10)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AA33" s="19" t="e">
-        <f>VLOOKUP(AA$32,funnel_lookup!$A$9:$J$39,10)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AB33" s="19" t="e">
-        <f>VLOOKUP(AB$32,funnel_lookup!$A$9:$J$39,10)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AC33" s="19" t="e">
-        <f>VLOOKUP(AC$32,funnel_lookup!$A$9:$J$39,10)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AD33" s="19" t="e">
-        <f>VLOOKUP(AD$32,funnel_lookup!$A$9:$J$39,10)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AE33" s="19" t="e">
-        <f>VLOOKUP(AE$32,funnel_lookup!$A$9:$J$39,10)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AF33" s="19" t="e">
-        <f>VLOOKUP(AF$32,funnel_lookup!$A$9:$J$39,10)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AG33" s="57" t="e">
-        <f>VLOOKUP(AG$32,funnel_lookup!$A$9:$J$39,10)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AH33" s="59"/>
+      <c r="C33" s="19">
+        <f>IFERROR(VLOOKUP(C$32,funnel_lookup!$A$9:$J$39,10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="D33" s="19">
+        <f>IFERROR(VLOOKUP(D$32,funnel_lookup!$A$9:$J$39,10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E33" s="19">
+        <f>IFERROR(VLOOKUP(E$32,funnel_lookup!$A$9:$J$39,10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="F33" s="19">
+        <f>IFERROR(VLOOKUP(F$32,funnel_lookup!$A$9:$J$39,10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G33" s="19">
+        <f>IFERROR(VLOOKUP(G$32,funnel_lookup!$A$9:$J$39,10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H33" s="19">
+        <f>IFERROR(VLOOKUP(H$32,funnel_lookup!$A$9:$J$39,10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I33" s="19">
+        <f>IFERROR(VLOOKUP(I$32,funnel_lookup!$A$9:$J$39,10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J33" s="19">
+        <f>IFERROR(VLOOKUP(J$32,funnel_lookup!$A$9:$J$39,10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K33" s="19">
+        <f>IFERROR(VLOOKUP(K$32,funnel_lookup!$A$9:$J$39,10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L33" s="19">
+        <f>IFERROR(VLOOKUP(L$32,funnel_lookup!$A$9:$J$39,10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M33" s="19">
+        <f>IFERROR(VLOOKUP(M$32,funnel_lookup!$A$9:$J$39,10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N33" s="19">
+        <f>IFERROR(VLOOKUP(N$32,funnel_lookup!$A$9:$J$39,10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O33" s="19">
+        <f>IFERROR(VLOOKUP(O$32,funnel_lookup!$A$9:$J$39,10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="P33" s="19">
+        <f>IFERROR(VLOOKUP(P$32,funnel_lookup!$A$9:$J$39,10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q33" s="19">
+        <f>IFERROR(VLOOKUP(Q$32,funnel_lookup!$A$9:$J$39,10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="R33" s="19">
+        <f>IFERROR(VLOOKUP(R$32,funnel_lookup!$A$9:$J$39,10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="S33" s="19">
+        <f>IFERROR(VLOOKUP(S$32,funnel_lookup!$A$9:$J$39,10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T33" s="19">
+        <f>IFERROR(VLOOKUP(T$32,funnel_lookup!$A$9:$J$39,10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="U33" s="19">
+        <f>IFERROR(VLOOKUP(U$32,funnel_lookup!$A$9:$J$39,10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="V33" s="19">
+        <f>IFERROR(VLOOKUP(V$32,funnel_lookup!$A$9:$J$39,10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="W33" s="19">
+        <f>IFERROR(VLOOKUP(W$32,funnel_lookup!$A$9:$J$39,10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="X33" s="19">
+        <f>IFERROR(VLOOKUP(X$32,funnel_lookup!$A$9:$J$39,10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y33" s="19">
+        <f>IFERROR(VLOOKUP(Y$32,funnel_lookup!$A$9:$J$39,10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z33" s="19">
+        <f>IFERROR(VLOOKUP(Z$32,funnel_lookup!$A$9:$J$39,10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA33" s="19">
+        <f>IFERROR(VLOOKUP(AA$32,funnel_lookup!$A$9:$J$39,10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AB33" s="19">
+        <f>IFERROR(VLOOKUP(AB$32,funnel_lookup!$A$9:$J$39,10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC33" s="19">
+        <f>IFERROR(VLOOKUP(AC$32,funnel_lookup!$A$9:$J$39,10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD33" s="19">
+        <f>IFERROR(VLOOKUP(AD$32,funnel_lookup!$A$9:$J$39,10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AE33" s="19">
+        <f>IFERROR(VLOOKUP(AE$32,funnel_lookup!$A$9:$J$39,10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AF33" s="19">
+        <f>IFERROR(VLOOKUP(AF$32,funnel_lookup!$A$9:$J$39,10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AG33" s="19">
+        <f>IFERROR(VLOOKUP(AG$32,funnel_lookup!$A$9:$J$39,10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AH33" s="58"/>
     </row>
     <row r="34" spans="1:37" s="18" customFormat="1" ht="186" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C34" s="20" t="e">
@@ -6828,14 +7417,14 @@
         <f>VLOOKUP(VLOOKUP(AF$32,funnel_lookup!$A$9:$B$39,2,FALSE),hosp_lookup!$A:$B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="AG34" s="58" t="e">
+      <c r="AG34" s="57" t="e">
         <f>VLOOKUP(VLOOKUP(AG$32,funnel_lookup!$A$9:$B$39,2,FALSE),hosp_lookup!$A:$B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="AH34" s="60"/>
+      <c r="AH34" s="59"/>
     </row>
     <row r="35" spans="1:37" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="AH35" s="62"/>
+      <c r="AH35" s="61"/>
       <c r="AJ35" s="15"/>
       <c r="AK35" s="15"/>
     </row>
@@ -6863,7 +7452,7 @@
       <c r="W36" s="21"/>
       <c r="X36" s="21"/>
       <c r="Y36" s="21"/>
-      <c r="AH36" s="61"/>
+      <c r="AH36" s="60"/>
       <c r="AJ36" s="18"/>
       <c r="AK36" s="18"/>
     </row>
@@ -6985,14 +7574,22 @@
     <mergeCell ref="B1:AB1"/>
   </mergeCells>
   <conditionalFormatting sqref="C33:AH33">
-    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" stopIfTrue="1" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
       <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C33:AG33">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+      <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -7005,7 +7602,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:R1022"/>
   <sheetViews>
@@ -14320,142 +14917,145 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:S1022"/>
+  <autoFilter ref="A1:S1022" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AM80"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="64"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A1" s="18"/>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18"/>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="18"/>
-      <c r="AD1" s="18"/>
-      <c r="AE1" s="18"/>
-      <c r="AF1" s="18"/>
-      <c r="AG1" s="18"/>
-      <c r="AH1" s="18"/>
-      <c r="AI1" s="18"/>
-      <c r="AJ1" s="18"/>
-      <c r="AK1" s="18"/>
-      <c r="AL1" s="18"/>
-      <c r="AM1" s="18"/>
+      <c r="A1" s="15"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="15"/>
+      <c r="AB1" s="15"/>
+      <c r="AC1" s="15"/>
+      <c r="AD1" s="15"/>
+      <c r="AE1" s="15"/>
+      <c r="AF1" s="15"/>
+      <c r="AG1" s="15"/>
+      <c r="AH1" s="15"/>
+      <c r="AI1" s="15"/>
+      <c r="AJ1" s="15"/>
+      <c r="AK1" s="15"/>
+      <c r="AL1" s="15"/>
+      <c r="AM1" s="15"/>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="18"/>
-      <c r="U2" s="18"/>
-      <c r="V2" s="18"/>
-      <c r="W2" s="18"/>
-      <c r="X2" s="18"/>
-      <c r="Y2" s="18"/>
-      <c r="Z2" s="18"/>
-      <c r="AA2" s="18"/>
-      <c r="AB2" s="18"/>
-      <c r="AC2" s="18"/>
-      <c r="AD2" s="18"/>
-      <c r="AE2" s="18"/>
-      <c r="AF2" s="18"/>
-      <c r="AG2" s="18"/>
-      <c r="AH2" s="18"/>
-      <c r="AI2" s="18"/>
-      <c r="AJ2" s="18"/>
-      <c r="AK2" s="18"/>
-      <c r="AL2" s="18"/>
-      <c r="AM2" s="18"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="15"/>
+      <c r="X2" s="15"/>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="15"/>
+      <c r="AA2" s="15"/>
+      <c r="AB2" s="15"/>
+      <c r="AC2" s="15"/>
+      <c r="AD2" s="15"/>
+      <c r="AE2" s="15"/>
+      <c r="AF2" s="15"/>
+      <c r="AG2" s="15"/>
+      <c r="AH2" s="15"/>
+      <c r="AI2" s="15"/>
+      <c r="AJ2" s="15"/>
+      <c r="AK2" s="15"/>
+      <c r="AL2" s="15"/>
+      <c r="AM2" s="15"/>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="18"/>
-      <c r="R3" s="18"/>
-      <c r="S3" s="18"/>
-      <c r="T3" s="18"/>
-      <c r="U3" s="18"/>
-      <c r="V3" s="18"/>
-      <c r="W3" s="18"/>
-      <c r="X3" s="18"/>
-      <c r="Y3" s="18"/>
-      <c r="Z3" s="18"/>
-      <c r="AA3" s="18"/>
-      <c r="AB3" s="18"/>
-      <c r="AC3" s="18"/>
-      <c r="AD3" s="18"/>
-      <c r="AE3" s="18"/>
-      <c r="AF3" s="18"/>
-      <c r="AG3" s="18"/>
-      <c r="AH3" s="18"/>
-      <c r="AI3" s="18"/>
-      <c r="AJ3" s="18"/>
-      <c r="AK3" s="18"/>
-      <c r="AL3" s="18"/>
-      <c r="AM3" s="18"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="15"/>
+      <c r="V3" s="15"/>
+      <c r="W3" s="15"/>
+      <c r="X3" s="15"/>
+      <c r="Y3" s="15"/>
+      <c r="Z3" s="15"/>
+      <c r="AA3" s="15"/>
+      <c r="AB3" s="15"/>
+      <c r="AC3" s="15"/>
+      <c r="AD3" s="15"/>
+      <c r="AE3" s="15"/>
+      <c r="AF3" s="15"/>
+      <c r="AG3" s="15"/>
+      <c r="AH3" s="15"/>
+      <c r="AI3" s="15"/>
+      <c r="AJ3" s="15"/>
+      <c r="AK3" s="15"/>
+      <c r="AL3" s="15"/>
+      <c r="AM3" s="15"/>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" s="15"/>
@@ -14609,10 +15209,18 @@
         <v>9</v>
       </c>
       <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
+      <c r="K7" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="L7" s="38" t="s">
+        <v>126</v>
+      </c>
+      <c r="M7" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="N7" s="38" t="s">
+        <v>128</v>
+      </c>
       <c r="O7" s="15"/>
       <c r="P7" s="15"/>
       <c r="Q7" s="65"/>
@@ -14674,8 +15282,12 @@
       <c r="L8" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
+      <c r="M8" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="N8" s="15" t="s">
+        <v>124</v>
+      </c>
       <c r="O8" s="15"/>
       <c r="P8" s="45"/>
       <c r="Q8" s="66"/>
@@ -14739,19 +15351,25 @@
         <v>#N/A</v>
       </c>
       <c r="J9" s="15" t="e">
-        <f t="shared" ref="J9:J39" si="1">IF(E9&gt;F9,3,IF(E9&gt;H9,2,0))</f>
+        <f>IF(E9&gt;F9,3,IF(AND(E9&gt;H9, E9 &lt;=F9),2, IF(E9 &lt;G9,5, IF(AND(E9&lt;I9, E9 &gt;=G9), 4,0))))</f>
         <v>#N/A</v>
       </c>
       <c r="K9" s="15" t="e">
-        <f t="shared" ref="K9:K39" si="2">IF(J9=3,E9,#N/A)</f>
+        <f>IF(J9=3,E9,NA())</f>
         <v>#N/A</v>
       </c>
       <c r="L9" s="15" t="e">
-        <f t="shared" ref="L9:L39" si="3">IF(J9=2,E9,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
+        <f>IF(J9=2,E9,NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M9" s="15" t="e">
+        <f>IF(J9=4,E9,NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N9" s="15" t="e">
+        <f>IF(J9=5,E9,NA())</f>
+        <v>#N/A</v>
+      </c>
       <c r="O9" s="15"/>
       <c r="P9" s="45"/>
       <c r="Q9" s="67"/>
@@ -14815,19 +15433,25 @@
         <v>#N/A</v>
       </c>
       <c r="J10" s="15" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="J10:J39" si="1">IF(E10&gt;F10,3,IF(AND(E10&gt;H10, E10 &lt;=F10),2, IF(E10 &lt;G10,5, IF(AND(E10&lt;I10, E10 &gt;=G10), 4,0))))</f>
         <v>#N/A</v>
       </c>
       <c r="K10" s="15" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="K10:K39" si="2">IF(J10=3,E10,NA())</f>
         <v>#N/A</v>
       </c>
       <c r="L10" s="15" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
+        <f t="shared" ref="L10:L39" si="3">IF(J10=2,E10,NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M10" s="15" t="e">
+        <f t="shared" ref="M10:M39" si="4">IF(J10=4,E10,NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N10" s="15" t="e">
+        <f t="shared" ref="N10:N39" si="5">IF(J10=5,E10,NA())</f>
+        <v>#N/A</v>
+      </c>
       <c r="O10" s="15"/>
       <c r="P10" s="45"/>
       <c r="Q10" s="67"/>
@@ -14902,8 +15526,14 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
+      <c r="M11" s="15" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N11" s="15" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
       <c r="O11" s="15"/>
       <c r="P11" s="45"/>
       <c r="Q11" s="67"/>
@@ -14978,8 +15608,14 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
+      <c r="M12" s="15" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N12" s="15" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
       <c r="O12" s="15"/>
       <c r="P12" s="45"/>
       <c r="Q12" s="67"/>
@@ -15054,8 +15690,14 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
+      <c r="M13" s="15" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N13" s="15" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
       <c r="O13" s="15"/>
       <c r="P13" s="45"/>
       <c r="Q13" s="67"/>
@@ -15130,8 +15772,14 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
+      <c r="M14" s="15" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N14" s="15" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
       <c r="O14" s="15"/>
       <c r="P14" s="45"/>
       <c r="Q14" s="67"/>
@@ -15206,8 +15854,14 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
+      <c r="M15" s="15" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N15" s="15" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
       <c r="O15" s="15"/>
       <c r="P15" s="45"/>
       <c r="Q15" s="67"/>
@@ -15282,8 +15936,14 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
+      <c r="M16" s="15" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N16" s="15" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
       <c r="O16" s="15"/>
       <c r="P16" s="45"/>
       <c r="Q16" s="67"/>
@@ -15358,8 +16018,14 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
+      <c r="M17" s="15" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N17" s="15" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
       <c r="O17" s="15"/>
       <c r="P17" s="45"/>
       <c r="Q17" s="67"/>
@@ -15434,8 +16100,14 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
+      <c r="M18" s="15" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N18" s="15" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
       <c r="O18" s="15"/>
       <c r="P18" s="45"/>
       <c r="Q18" s="67"/>
@@ -15467,35 +16139,35 @@
         <v>11</v>
       </c>
       <c r="B19" s="45" t="e">
-        <f t="shared" ref="B19:I28" si="4">VLOOKUP($A19,$A$43:$I$73,B$7,FALSE)</f>
+        <f t="shared" ref="B19:I28" si="6">VLOOKUP($A19,$A$43:$I$73,B$7,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="C19" s="67" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="D19" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="E19" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="F19" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="G19" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="H19" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="I19" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="J19" s="15" t="e">
@@ -15510,8 +16182,14 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="M19" s="15"/>
-      <c r="N19" s="15"/>
+      <c r="M19" s="15" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N19" s="15" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
       <c r="O19" s="15"/>
       <c r="P19" s="45"/>
       <c r="Q19" s="67"/>
@@ -15543,35 +16221,35 @@
         <v>12</v>
       </c>
       <c r="B20" s="45" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="C20" s="67" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="D20" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="E20" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="F20" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="G20" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="H20" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="I20" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="J20" s="15" t="e">
@@ -15586,8 +16264,14 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
+      <c r="M20" s="15" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N20" s="15" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
       <c r="O20" s="15"/>
       <c r="P20" s="45"/>
       <c r="Q20" s="67"/>
@@ -15619,35 +16303,35 @@
         <v>13</v>
       </c>
       <c r="B21" s="45" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="C21" s="67" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="D21" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="E21" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="F21" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="G21" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="H21" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="I21" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="J21" s="15" t="e">
@@ -15662,8 +16346,14 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
+      <c r="M21" s="15" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N21" s="15" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
       <c r="O21" s="15"/>
       <c r="P21" s="45"/>
       <c r="Q21" s="67"/>
@@ -15695,35 +16385,35 @@
         <v>14</v>
       </c>
       <c r="B22" s="45" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="C22" s="67" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="D22" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="E22" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="F22" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="G22" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="H22" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="I22" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="J22" s="15" t="e">
@@ -15738,8 +16428,14 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
+      <c r="M22" s="15" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N22" s="15" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
       <c r="O22" s="15"/>
       <c r="P22" s="45"/>
       <c r="Q22" s="67"/>
@@ -15771,35 +16467,35 @@
         <v>15</v>
       </c>
       <c r="B23" s="45" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="C23" s="67" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="D23" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="E23" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="F23" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="G23" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="H23" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="I23" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="J23" s="15" t="e">
@@ -15814,8 +16510,14 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
+      <c r="M23" s="15" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N23" s="15" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
       <c r="O23" s="15"/>
       <c r="P23" s="45"/>
       <c r="Q23" s="67"/>
@@ -15847,35 +16549,35 @@
         <v>16</v>
       </c>
       <c r="B24" s="45" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="C24" s="67" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="D24" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="E24" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="F24" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="G24" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="H24" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="I24" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="J24" s="15" t="e">
@@ -15890,8 +16592,14 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
+      <c r="M24" s="15" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N24" s="15" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
       <c r="O24" s="15"/>
       <c r="P24" s="15"/>
       <c r="Q24" s="15"/>
@@ -15923,35 +16631,35 @@
         <v>17</v>
       </c>
       <c r="B25" s="45" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="C25" s="67" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="D25" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="E25" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="F25" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="G25" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="H25" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="I25" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="J25" s="15" t="e">
@@ -15966,8 +16674,14 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
+      <c r="M25" s="15" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N25" s="15" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
       <c r="O25" s="15"/>
       <c r="P25" s="15"/>
       <c r="Q25" s="15"/>
@@ -15999,35 +16713,35 @@
         <v>18</v>
       </c>
       <c r="B26" s="45" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="C26" s="67" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="D26" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="E26" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="F26" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="G26" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="H26" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="I26" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="J26" s="15" t="e">
@@ -16042,8 +16756,14 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
+      <c r="M26" s="15" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N26" s="15" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
       <c r="O26" s="15"/>
       <c r="P26" s="15"/>
       <c r="Q26" s="15"/>
@@ -16075,35 +16795,35 @@
         <v>19</v>
       </c>
       <c r="B27" s="45" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="C27" s="67" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="D27" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="E27" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="F27" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="G27" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="H27" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="I27" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="J27" s="15" t="e">
@@ -16118,8 +16838,14 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="M27" s="15"/>
-      <c r="N27" s="15"/>
+      <c r="M27" s="15" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N27" s="15" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
       <c r="O27" s="15"/>
       <c r="P27" s="15"/>
       <c r="Q27" s="15"/>
@@ -16151,35 +16877,35 @@
         <v>20</v>
       </c>
       <c r="B28" s="45" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="C28" s="67" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="D28" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="E28" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="F28" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="G28" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="H28" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="I28" s="68" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="J28" s="15" t="e">
@@ -16194,8 +16920,14 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="M28" s="15"/>
-      <c r="N28" s="15"/>
+      <c r="M28" s="15" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N28" s="15" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
       <c r="O28" s="15"/>
       <c r="P28" s="15"/>
       <c r="Q28" s="15"/>
@@ -16227,35 +16959,35 @@
         <v>21</v>
       </c>
       <c r="B29" s="45" t="e">
-        <f t="shared" ref="B29:I39" si="5">VLOOKUP($A29,$A$43:$I$73,B$7,FALSE)</f>
+        <f t="shared" ref="B29:I39" si="7">VLOOKUP($A29,$A$43:$I$73,B$7,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="C29" s="67" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="D29" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="E29" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="F29" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="G29" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="H29" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="I29" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="J29" s="15" t="e">
@@ -16270,8 +17002,14 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="M29" s="15"/>
-      <c r="N29" s="15"/>
+      <c r="M29" s="15" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N29" s="15" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
       <c r="O29" s="15"/>
       <c r="P29" s="15"/>
       <c r="Q29" s="15"/>
@@ -16303,35 +17041,35 @@
         <v>22</v>
       </c>
       <c r="B30" s="45" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="C30" s="67" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="D30" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="E30" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="F30" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="G30" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="H30" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="I30" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="J30" s="15" t="e">
@@ -16346,8 +17084,14 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="M30" s="15"/>
-      <c r="N30" s="15"/>
+      <c r="M30" s="15" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N30" s="15" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
       <c r="O30" s="15"/>
       <c r="P30" s="15"/>
       <c r="Q30" s="15"/>
@@ -16379,35 +17123,35 @@
         <v>23</v>
       </c>
       <c r="B31" s="45" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="C31" s="67" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="D31" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="E31" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="F31" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="G31" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="H31" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="I31" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="J31" s="15" t="e">
@@ -16422,8 +17166,14 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="M31" s="15"/>
-      <c r="N31" s="15"/>
+      <c r="M31" s="15" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N31" s="15" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
       <c r="O31" s="15"/>
       <c r="P31" s="15"/>
       <c r="Q31" s="15"/>
@@ -16455,35 +17205,35 @@
         <v>24</v>
       </c>
       <c r="B32" s="45" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="C32" s="67" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="D32" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="E32" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="F32" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="G32" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="H32" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="I32" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="J32" s="15" t="e">
@@ -16498,8 +17248,14 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="M32" s="15"/>
-      <c r="N32" s="15"/>
+      <c r="M32" s="15" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N32" s="15" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
       <c r="O32" s="15"/>
       <c r="P32" s="15"/>
       <c r="Q32" s="15"/>
@@ -16531,35 +17287,35 @@
         <v>25</v>
       </c>
       <c r="B33" s="45" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="C33" s="67" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="D33" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="E33" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="F33" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="G33" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="H33" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="I33" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="J33" s="15" t="e">
@@ -16574,8 +17330,14 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="M33" s="15"/>
-      <c r="N33" s="15"/>
+      <c r="M33" s="15" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N33" s="15" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
       <c r="O33" s="15"/>
       <c r="P33" s="15"/>
       <c r="Q33" s="15"/>
@@ -16607,35 +17369,35 @@
         <v>26</v>
       </c>
       <c r="B34" s="45" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="C34" s="67" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="D34" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="E34" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="F34" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="G34" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="H34" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="I34" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="J34" s="15" t="e">
@@ -16650,8 +17412,14 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="M34" s="15"/>
-      <c r="N34" s="15"/>
+      <c r="M34" s="15" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N34" s="15" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
       <c r="O34" s="15"/>
       <c r="P34" s="15"/>
       <c r="Q34" s="15"/>
@@ -16683,35 +17451,35 @@
         <v>27</v>
       </c>
       <c r="B35" s="45" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="C35" s="67" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="D35" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="E35" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="F35" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="G35" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="H35" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="I35" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="J35" s="15" t="e">
@@ -16726,8 +17494,14 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="M35" s="15"/>
-      <c r="N35" s="15"/>
+      <c r="M35" s="15" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N35" s="15" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
       <c r="O35" s="15"/>
       <c r="P35" s="15"/>
       <c r="Q35" s="15"/>
@@ -16759,35 +17533,35 @@
         <v>28</v>
       </c>
       <c r="B36" s="45" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="C36" s="67" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="D36" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="E36" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="F36" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="G36" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="H36" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="I36" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="J36" s="15" t="e">
@@ -16802,8 +17576,14 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="M36" s="15"/>
-      <c r="N36" s="15"/>
+      <c r="M36" s="15" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N36" s="15" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
       <c r="O36" s="15"/>
       <c r="P36" s="15"/>
       <c r="Q36" s="15"/>
@@ -16835,35 +17615,35 @@
         <v>29</v>
       </c>
       <c r="B37" s="45" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="C37" s="67" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="D37" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="E37" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="F37" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="G37" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="H37" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="I37" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="J37" s="15" t="e">
@@ -16878,8 +17658,14 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="M37" s="15"/>
-      <c r="N37" s="15"/>
+      <c r="M37" s="15" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N37" s="15" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
       <c r="O37" s="15"/>
       <c r="P37" s="15"/>
       <c r="Q37" s="15"/>
@@ -16911,35 +17697,35 @@
         <v>30</v>
       </c>
       <c r="B38" s="45" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="C38" s="67" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="D38" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="E38" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="F38" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="G38" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="H38" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="I38" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="J38" s="15" t="e">
@@ -16954,8 +17740,14 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="M38" s="15"/>
-      <c r="N38" s="15"/>
+      <c r="M38" s="15" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N38" s="15" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
       <c r="O38" s="15"/>
       <c r="P38" s="15"/>
       <c r="Q38" s="15"/>
@@ -16987,35 +17779,35 @@
         <v>31</v>
       </c>
       <c r="B39" s="45" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="C39" s="67" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="D39" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="E39" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="F39" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="G39" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="H39" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="I39" s="68" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="J39" s="15" t="e">
@@ -17030,8 +17822,14 @@
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="M39" s="15"/>
-      <c r="N39" s="15"/>
+      <c r="M39" s="15" t="e">
+        <f t="shared" si="4"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N39" s="15" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
       <c r="O39" s="15"/>
       <c r="P39" s="15"/>
       <c r="Q39" s="15"/>
@@ -17215,7 +18013,7 @@
     </row>
     <row r="43" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="e">
-        <f t="shared" ref="A43:A73" si="6">RANK(C43,$C$43:$C$73,1)</f>
+        <f t="shared" ref="A43:A73" si="8">RANK(C43,$C$43:$C$73,1)</f>
         <v>#N/A</v>
       </c>
       <c r="B43" s="45" t="s">
@@ -17233,19 +18031,19 @@
         <v>#N/A</v>
       </c>
       <c r="F43" s="73" t="e">
-        <f>VLOOKUP($B43&amp;"3",'Raw Data'!$A:$X,F$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B43&amp;"3",'Raw Data'!$A:$X,F$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="G43" s="73" t="e">
-        <f>VLOOKUP($B43&amp;"3",'Raw Data'!$A:$X,G$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B43&amp;"3",'Raw Data'!$A:$X,G$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="H43" s="73" t="e">
-        <f>VLOOKUP($B43&amp;"3",'Raw Data'!$A:$X,H$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B43&amp;"3",'Raw Data'!$A:$X,H$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="I43" s="73" t="e">
-        <f>VLOOKUP($B43&amp;"3",'Raw Data'!$A:$X,I$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B43&amp;"3",'Raw Data'!$A:$X,I$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="J43" s="15"/>
@@ -17281,7 +18079,7 @@
     </row>
     <row r="44" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="B44" s="45" t="s">
@@ -17299,19 +18097,19 @@
         <v>#N/A</v>
       </c>
       <c r="F44" s="73" t="e">
-        <f>VLOOKUP($B44&amp;"3",'Raw Data'!$A:$X,F$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B44&amp;"3",'Raw Data'!$A:$X,F$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="G44" s="73" t="e">
-        <f>VLOOKUP($B44&amp;"3",'Raw Data'!$A:$X,G$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B44&amp;"3",'Raw Data'!$A:$X,G$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="H44" s="73" t="e">
-        <f>VLOOKUP($B44&amp;"3",'Raw Data'!$A:$X,H$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B44&amp;"3",'Raw Data'!$A:$X,H$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="I44" s="73" t="e">
-        <f>VLOOKUP($B44&amp;"3",'Raw Data'!$A:$X,I$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B44&amp;"3",'Raw Data'!$A:$X,I$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="J44" s="15"/>
@@ -17347,7 +18145,7 @@
     </row>
     <row r="45" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A45" s="15" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="B45" s="45" t="s">
@@ -17365,19 +18163,19 @@
         <v>#N/A</v>
       </c>
       <c r="F45" s="73" t="e">
-        <f>VLOOKUP($B45&amp;"3",'Raw Data'!$A:$X,F$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B45&amp;"3",'Raw Data'!$A:$X,F$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="G45" s="73" t="e">
-        <f>VLOOKUP($B45&amp;"3",'Raw Data'!$A:$X,G$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B45&amp;"3",'Raw Data'!$A:$X,G$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="H45" s="73" t="e">
-        <f>VLOOKUP($B45&amp;"3",'Raw Data'!$A:$X,H$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B45&amp;"3",'Raw Data'!$A:$X,H$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="I45" s="73" t="e">
-        <f>VLOOKUP($B45&amp;"3",'Raw Data'!$A:$X,I$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B45&amp;"3",'Raw Data'!$A:$X,I$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="J45" s="15"/>
@@ -17413,7 +18211,7 @@
     </row>
     <row r="46" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A46" s="15" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="B46" s="45" t="s">
@@ -17431,19 +18229,19 @@
         <v>#N/A</v>
       </c>
       <c r="F46" s="73" t="e">
-        <f>VLOOKUP($B46&amp;"3",'Raw Data'!$A:$X,F$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B46&amp;"3",'Raw Data'!$A:$X,F$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="G46" s="73" t="e">
-        <f>VLOOKUP($B46&amp;"3",'Raw Data'!$A:$X,G$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B46&amp;"3",'Raw Data'!$A:$X,G$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="H46" s="73" t="e">
-        <f>VLOOKUP($B46&amp;"3",'Raw Data'!$A:$X,H$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B46&amp;"3",'Raw Data'!$A:$X,H$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="I46" s="73" t="e">
-        <f>VLOOKUP($B46&amp;"3",'Raw Data'!$A:$X,I$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B46&amp;"3",'Raw Data'!$A:$X,I$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="J46" s="15"/>
@@ -17479,7 +18277,7 @@
     </row>
     <row r="47" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A47" s="15" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="B47" s="45" t="s">
@@ -17497,19 +18295,19 @@
         <v>#N/A</v>
       </c>
       <c r="F47" s="73" t="e">
-        <f>VLOOKUP($B47&amp;"3",'Raw Data'!$A:$X,F$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B47&amp;"3",'Raw Data'!$A:$X,F$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="G47" s="73" t="e">
-        <f>VLOOKUP($B47&amp;"3",'Raw Data'!$A:$X,G$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B47&amp;"3",'Raw Data'!$A:$X,G$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="H47" s="73" t="e">
-        <f>VLOOKUP($B47&amp;"3",'Raw Data'!$A:$X,H$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B47&amp;"3",'Raw Data'!$A:$X,H$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="I47" s="73" t="e">
-        <f>VLOOKUP($B47&amp;"3",'Raw Data'!$A:$X,I$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B47&amp;"3",'Raw Data'!$A:$X,I$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="J47" s="15"/>
@@ -17545,7 +18343,7 @@
     </row>
     <row r="48" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="B48" s="45" t="s">
@@ -17563,19 +18361,19 @@
         <v>#N/A</v>
       </c>
       <c r="F48" s="73" t="e">
-        <f>VLOOKUP($B48&amp;"3",'Raw Data'!$A:$X,F$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B48&amp;"3",'Raw Data'!$A:$X,F$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="G48" s="73" t="e">
-        <f>VLOOKUP($B48&amp;"3",'Raw Data'!$A:$X,G$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B48&amp;"3",'Raw Data'!$A:$X,G$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="H48" s="73" t="e">
-        <f>VLOOKUP($B48&amp;"3",'Raw Data'!$A:$X,H$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B48&amp;"3",'Raw Data'!$A:$X,H$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="I48" s="73" t="e">
-        <f>VLOOKUP($B48&amp;"3",'Raw Data'!$A:$X,I$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B48&amp;"3",'Raw Data'!$A:$X,I$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="J48" s="15"/>
@@ -17611,7 +18409,7 @@
     </row>
     <row r="49" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A49" s="15" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="B49" s="45" t="s">
@@ -17629,19 +18427,19 @@
         <v>#N/A</v>
       </c>
       <c r="F49" s="73" t="e">
-        <f>VLOOKUP($B49&amp;"3",'Raw Data'!$A:$X,F$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B49&amp;"3",'Raw Data'!$A:$X,F$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="G49" s="73" t="e">
-        <f>VLOOKUP($B49&amp;"3",'Raw Data'!$A:$X,G$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B49&amp;"3",'Raw Data'!$A:$X,G$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="H49" s="73" t="e">
-        <f>VLOOKUP($B49&amp;"3",'Raw Data'!$A:$X,H$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B49&amp;"3",'Raw Data'!$A:$X,H$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="I49" s="73" t="e">
-        <f>VLOOKUP($B49&amp;"3",'Raw Data'!$A:$X,I$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B49&amp;"3",'Raw Data'!$A:$X,I$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="J49" s="15"/>
@@ -17677,7 +18475,7 @@
     </row>
     <row r="50" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A50" s="15" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="B50" s="45" t="s">
@@ -17695,19 +18493,19 @@
         <v>#N/A</v>
       </c>
       <c r="F50" s="73" t="e">
-        <f>VLOOKUP($B50&amp;"3",'Raw Data'!$A:$X,F$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B50&amp;"3",'Raw Data'!$A:$X,F$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="G50" s="73" t="e">
-        <f>VLOOKUP($B50&amp;"3",'Raw Data'!$A:$X,G$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B50&amp;"3",'Raw Data'!$A:$X,G$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="H50" s="73" t="e">
-        <f>VLOOKUP($B50&amp;"3",'Raw Data'!$A:$X,H$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B50&amp;"3",'Raw Data'!$A:$X,H$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="I50" s="73" t="e">
-        <f>VLOOKUP($B50&amp;"3",'Raw Data'!$A:$X,I$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B50&amp;"3",'Raw Data'!$A:$X,I$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="J50" s="15"/>
@@ -17743,7 +18541,7 @@
     </row>
     <row r="51" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A51" s="15" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="B51" s="45" t="s">
@@ -17761,19 +18559,19 @@
         <v>#N/A</v>
       </c>
       <c r="F51" s="73" t="e">
-        <f>VLOOKUP($B51&amp;"3",'Raw Data'!$A:$X,F$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B51&amp;"3",'Raw Data'!$A:$X,F$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="G51" s="73" t="e">
-        <f>VLOOKUP($B51&amp;"3",'Raw Data'!$A:$X,G$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B51&amp;"3",'Raw Data'!$A:$X,G$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="H51" s="73" t="e">
-        <f>VLOOKUP($B51&amp;"3",'Raw Data'!$A:$X,H$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B51&amp;"3",'Raw Data'!$A:$X,H$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="I51" s="73" t="e">
-        <f>VLOOKUP($B51&amp;"3",'Raw Data'!$A:$X,I$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B51&amp;"3",'Raw Data'!$A:$X,I$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="J51" s="15"/>
@@ -17809,7 +18607,7 @@
     </row>
     <row r="52" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A52" s="15" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="B52" s="45" t="s">
@@ -17827,19 +18625,19 @@
         <v>#N/A</v>
       </c>
       <c r="F52" s="73" t="e">
-        <f>VLOOKUP($B52&amp;"3",'Raw Data'!$A:$X,F$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B52&amp;"3",'Raw Data'!$A:$X,F$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="G52" s="73" t="e">
-        <f>VLOOKUP($B52&amp;"3",'Raw Data'!$A:$X,G$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B52&amp;"3",'Raw Data'!$A:$X,G$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="H52" s="73" t="e">
-        <f>VLOOKUP($B52&amp;"3",'Raw Data'!$A:$X,H$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B52&amp;"3",'Raw Data'!$A:$X,H$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="I52" s="73" t="e">
-        <f>VLOOKUP($B52&amp;"3",'Raw Data'!$A:$X,I$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B52&amp;"3",'Raw Data'!$A:$X,I$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="J52" s="15"/>
@@ -17875,7 +18673,7 @@
     </row>
     <row r="53" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A53" s="15" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="B53" s="45" t="s">
@@ -17893,19 +18691,19 @@
         <v>#N/A</v>
       </c>
       <c r="F53" s="73" t="e">
-        <f>VLOOKUP($B53&amp;"3",'Raw Data'!$A:$X,F$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B53&amp;"3",'Raw Data'!$A:$X,F$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="G53" s="73" t="e">
-        <f>VLOOKUP($B53&amp;"3",'Raw Data'!$A:$X,G$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B53&amp;"3",'Raw Data'!$A:$X,G$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="H53" s="73" t="e">
-        <f>VLOOKUP($B53&amp;"3",'Raw Data'!$A:$X,H$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B53&amp;"3",'Raw Data'!$A:$X,H$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="I53" s="73" t="e">
-        <f>VLOOKUP($B53&amp;"3",'Raw Data'!$A:$X,I$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B53&amp;"3",'Raw Data'!$A:$X,I$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="J53" s="15"/>
@@ -17941,7 +18739,7 @@
     </row>
     <row r="54" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A54" s="15" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="B54" s="45" t="s">
@@ -17959,19 +18757,19 @@
         <v>#N/A</v>
       </c>
       <c r="F54" s="73" t="e">
-        <f>VLOOKUP($B54&amp;"3",'Raw Data'!$A:$X,F$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B54&amp;"3",'Raw Data'!$A:$X,F$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="G54" s="73" t="e">
-        <f>VLOOKUP($B54&amp;"3",'Raw Data'!$A:$X,G$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B54&amp;"3",'Raw Data'!$A:$X,G$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="H54" s="73" t="e">
-        <f>VLOOKUP($B54&amp;"3",'Raw Data'!$A:$X,H$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B54&amp;"3",'Raw Data'!$A:$X,H$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="I54" s="73" t="e">
-        <f>VLOOKUP($B54&amp;"3",'Raw Data'!$A:$X,I$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B54&amp;"3",'Raw Data'!$A:$X,I$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="J54" s="15"/>
@@ -18007,7 +18805,7 @@
     </row>
     <row r="55" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A55" s="15" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="B55" s="45" t="s">
@@ -18025,19 +18823,19 @@
         <v>#N/A</v>
       </c>
       <c r="F55" s="73" t="e">
-        <f>VLOOKUP($B55&amp;"3",'Raw Data'!$A:$X,F$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B55&amp;"3",'Raw Data'!$A:$X,F$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="G55" s="73" t="e">
-        <f>VLOOKUP($B55&amp;"3",'Raw Data'!$A:$X,G$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B55&amp;"3",'Raw Data'!$A:$X,G$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="H55" s="73" t="e">
-        <f>VLOOKUP($B55&amp;"3",'Raw Data'!$A:$X,H$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B55&amp;"3",'Raw Data'!$A:$X,H$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="I55" s="73" t="e">
-        <f>VLOOKUP($B55&amp;"3",'Raw Data'!$A:$X,I$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B55&amp;"3",'Raw Data'!$A:$X,I$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="J55" s="15"/>
@@ -18073,7 +18871,7 @@
     </row>
     <row r="56" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A56" s="15" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="B56" s="45" t="s">
@@ -18091,19 +18889,19 @@
         <v>#N/A</v>
       </c>
       <c r="F56" s="73" t="e">
-        <f>VLOOKUP($B56&amp;"3",'Raw Data'!$A:$X,F$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B56&amp;"3",'Raw Data'!$A:$X,F$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="G56" s="73" t="e">
-        <f>VLOOKUP($B56&amp;"3",'Raw Data'!$A:$X,G$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B56&amp;"3",'Raw Data'!$A:$X,G$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="H56" s="73" t="e">
-        <f>VLOOKUP($B56&amp;"3",'Raw Data'!$A:$X,H$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B56&amp;"3",'Raw Data'!$A:$X,H$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="I56" s="73" t="e">
-        <f>VLOOKUP($B56&amp;"3",'Raw Data'!$A:$X,I$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B56&amp;"3",'Raw Data'!$A:$X,I$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="J56" s="15"/>
@@ -18139,7 +18937,7 @@
     </row>
     <row r="57" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A57" s="15" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="B57" s="45" t="s">
@@ -18157,19 +18955,19 @@
         <v>#N/A</v>
       </c>
       <c r="F57" s="73" t="e">
-        <f>VLOOKUP($B57&amp;"3",'Raw Data'!$A:$X,F$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B57&amp;"3",'Raw Data'!$A:$X,F$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="G57" s="73" t="e">
-        <f>VLOOKUP($B57&amp;"3",'Raw Data'!$A:$X,G$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B57&amp;"3",'Raw Data'!$A:$X,G$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="H57" s="73" t="e">
-        <f>VLOOKUP($B57&amp;"3",'Raw Data'!$A:$X,H$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B57&amp;"3",'Raw Data'!$A:$X,H$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="I57" s="73" t="e">
-        <f>VLOOKUP($B57&amp;"3",'Raw Data'!$A:$X,I$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B57&amp;"3",'Raw Data'!$A:$X,I$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="J57" s="15"/>
@@ -18205,7 +19003,7 @@
     </row>
     <row r="58" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A58" s="15" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="B58" s="45" t="s">
@@ -18223,19 +19021,19 @@
         <v>#N/A</v>
       </c>
       <c r="F58" s="73" t="e">
-        <f>VLOOKUP($B58&amp;"3",'Raw Data'!$A:$X,F$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B58&amp;"3",'Raw Data'!$A:$X,F$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="G58" s="73" t="e">
-        <f>VLOOKUP($B58&amp;"3",'Raw Data'!$A:$X,G$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B58&amp;"3",'Raw Data'!$A:$X,G$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="H58" s="73" t="e">
-        <f>VLOOKUP($B58&amp;"3",'Raw Data'!$A:$X,H$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B58&amp;"3",'Raw Data'!$A:$X,H$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="I58" s="73" t="e">
-        <f>VLOOKUP($B58&amp;"3",'Raw Data'!$A:$X,I$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B58&amp;"3",'Raw Data'!$A:$X,I$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="J58" s="15"/>
@@ -18271,7 +19069,7 @@
     </row>
     <row r="59" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A59" s="15" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="B59" s="45" t="s">
@@ -18289,19 +19087,19 @@
         <v>#N/A</v>
       </c>
       <c r="F59" s="73" t="e">
-        <f>VLOOKUP($B59&amp;"3",'Raw Data'!$A:$X,F$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B59&amp;"3",'Raw Data'!$A:$X,F$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="G59" s="73" t="e">
-        <f>VLOOKUP($B59&amp;"3",'Raw Data'!$A:$X,G$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B59&amp;"3",'Raw Data'!$A:$X,G$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="H59" s="73" t="e">
-        <f>VLOOKUP($B59&amp;"3",'Raw Data'!$A:$X,H$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B59&amp;"3",'Raw Data'!$A:$X,H$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="I59" s="73" t="e">
-        <f>VLOOKUP($B59&amp;"3",'Raw Data'!$A:$X,I$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B59&amp;"3",'Raw Data'!$A:$X,I$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="J59" s="15"/>
@@ -18337,7 +19135,7 @@
     </row>
     <row r="60" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A60" s="15" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="B60" s="45" t="s">
@@ -18355,19 +19153,19 @@
         <v>#N/A</v>
       </c>
       <c r="F60" s="73" t="e">
-        <f>VLOOKUP($B60&amp;"3",'Raw Data'!$A:$X,F$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B60&amp;"3",'Raw Data'!$A:$X,F$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="G60" s="73" t="e">
-        <f>VLOOKUP($B60&amp;"3",'Raw Data'!$A:$X,G$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B60&amp;"3",'Raw Data'!$A:$X,G$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="H60" s="73" t="e">
-        <f>VLOOKUP($B60&amp;"3",'Raw Data'!$A:$X,H$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B60&amp;"3",'Raw Data'!$A:$X,H$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="I60" s="73" t="e">
-        <f>VLOOKUP($B60&amp;"3",'Raw Data'!$A:$X,I$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B60&amp;"3",'Raw Data'!$A:$X,I$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="J60" s="15"/>
@@ -18403,7 +19201,7 @@
     </row>
     <row r="61" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A61" s="15" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="B61" s="45" t="s">
@@ -18421,19 +19219,19 @@
         <v>#N/A</v>
       </c>
       <c r="F61" s="73" t="e">
-        <f>VLOOKUP($B61&amp;"3",'Raw Data'!$A:$X,F$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B61&amp;"3",'Raw Data'!$A:$X,F$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="G61" s="73" t="e">
-        <f>VLOOKUP($B61&amp;"3",'Raw Data'!$A:$X,G$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B61&amp;"3",'Raw Data'!$A:$X,G$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="H61" s="73" t="e">
-        <f>VLOOKUP($B61&amp;"3",'Raw Data'!$A:$X,H$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B61&amp;"3",'Raw Data'!$A:$X,H$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="I61" s="73" t="e">
-        <f>VLOOKUP($B61&amp;"3",'Raw Data'!$A:$X,I$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B61&amp;"3",'Raw Data'!$A:$X,I$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="J61" s="15"/>
@@ -18469,7 +19267,7 @@
     </row>
     <row r="62" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A62" s="15" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="B62" s="45" t="s">
@@ -18487,19 +19285,19 @@
         <v>#N/A</v>
       </c>
       <c r="F62" s="73" t="e">
-        <f>VLOOKUP($B62&amp;"3",'Raw Data'!$A:$X,F$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B62&amp;"3",'Raw Data'!$A:$X,F$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="G62" s="73" t="e">
-        <f>VLOOKUP($B62&amp;"3",'Raw Data'!$A:$X,G$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B62&amp;"3",'Raw Data'!$A:$X,G$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="H62" s="73" t="e">
-        <f>VLOOKUP($B62&amp;"3",'Raw Data'!$A:$X,H$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B62&amp;"3",'Raw Data'!$A:$X,H$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="I62" s="73" t="e">
-        <f>VLOOKUP($B62&amp;"3",'Raw Data'!$A:$X,I$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B62&amp;"3",'Raw Data'!$A:$X,I$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="J62" s="15"/>
@@ -18535,7 +19333,7 @@
     </row>
     <row r="63" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A63" s="15" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="B63" s="45" t="s">
@@ -18553,19 +19351,19 @@
         <v>#N/A</v>
       </c>
       <c r="F63" s="73" t="e">
-        <f>VLOOKUP($B63&amp;"3",'Raw Data'!$A:$X,F$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B63&amp;"3",'Raw Data'!$A:$X,F$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="G63" s="73" t="e">
-        <f>VLOOKUP($B63&amp;"3",'Raw Data'!$A:$X,G$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B63&amp;"3",'Raw Data'!$A:$X,G$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="H63" s="73" t="e">
-        <f>VLOOKUP($B63&amp;"3",'Raw Data'!$A:$X,H$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B63&amp;"3",'Raw Data'!$A:$X,H$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="I63" s="73" t="e">
-        <f>VLOOKUP($B63&amp;"3",'Raw Data'!$A:$X,I$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B63&amp;"3",'Raw Data'!$A:$X,I$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="J63" s="15"/>
@@ -18601,7 +19399,7 @@
     </row>
     <row r="64" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A64" s="15" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="B64" s="45" t="s">
@@ -18619,19 +19417,19 @@
         <v>#N/A</v>
       </c>
       <c r="F64" s="73" t="e">
-        <f>VLOOKUP($B64&amp;"3",'Raw Data'!$A:$X,F$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B64&amp;"3",'Raw Data'!$A:$X,F$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="G64" s="73" t="e">
-        <f>VLOOKUP($B64&amp;"3",'Raw Data'!$A:$X,G$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B64&amp;"3",'Raw Data'!$A:$X,G$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="H64" s="73" t="e">
-        <f>VLOOKUP($B64&amp;"3",'Raw Data'!$A:$X,H$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B64&amp;"3",'Raw Data'!$A:$X,H$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="I64" s="73" t="e">
-        <f>VLOOKUP($B64&amp;"3",'Raw Data'!$A:$X,I$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B64&amp;"3",'Raw Data'!$A:$X,I$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="J64" s="15"/>
@@ -18667,7 +19465,7 @@
     </row>
     <row r="65" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A65" s="15" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="B65" s="45" t="s">
@@ -18685,19 +19483,19 @@
         <v>#N/A</v>
       </c>
       <c r="F65" s="73" t="e">
-        <f>VLOOKUP($B65&amp;"3",'Raw Data'!$A:$X,F$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B65&amp;"3",'Raw Data'!$A:$X,F$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="G65" s="73" t="e">
-        <f>VLOOKUP($B65&amp;"3",'Raw Data'!$A:$X,G$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B65&amp;"3",'Raw Data'!$A:$X,G$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="H65" s="73" t="e">
-        <f>VLOOKUP($B65&amp;"3",'Raw Data'!$A:$X,H$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B65&amp;"3",'Raw Data'!$A:$X,H$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="I65" s="73" t="e">
-        <f>VLOOKUP($B65&amp;"3",'Raw Data'!$A:$X,I$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B65&amp;"3",'Raw Data'!$A:$X,I$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="J65" s="15"/>
@@ -18733,7 +19531,7 @@
     </row>
     <row r="66" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A66" s="15" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="B66" s="45" t="s">
@@ -18751,19 +19549,19 @@
         <v>#N/A</v>
       </c>
       <c r="F66" s="73" t="e">
-        <f>VLOOKUP($B66&amp;"3",'Raw Data'!$A:$X,F$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B66&amp;"3",'Raw Data'!$A:$X,F$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="G66" s="73" t="e">
-        <f>VLOOKUP($B66&amp;"3",'Raw Data'!$A:$X,G$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B66&amp;"3",'Raw Data'!$A:$X,G$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="H66" s="73" t="e">
-        <f>VLOOKUP($B66&amp;"3",'Raw Data'!$A:$X,H$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B66&amp;"3",'Raw Data'!$A:$X,H$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="I66" s="73" t="e">
-        <f>VLOOKUP($B66&amp;"3",'Raw Data'!$A:$X,I$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B66&amp;"3",'Raw Data'!$A:$X,I$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="J66" s="15"/>
@@ -18799,7 +19597,7 @@
     </row>
     <row r="67" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A67" s="15" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="B67" s="45" t="s">
@@ -18817,19 +19615,19 @@
         <v>#N/A</v>
       </c>
       <c r="F67" s="73" t="e">
-        <f>VLOOKUP($B67&amp;"3",'Raw Data'!$A:$X,F$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B67&amp;"3",'Raw Data'!$A:$X,F$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="G67" s="73" t="e">
-        <f>VLOOKUP($B67&amp;"3",'Raw Data'!$A:$X,G$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B67&amp;"3",'Raw Data'!$A:$X,G$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="H67" s="73" t="e">
-        <f>VLOOKUP($B67&amp;"3",'Raw Data'!$A:$X,H$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B67&amp;"3",'Raw Data'!$A:$X,H$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="I67" s="73" t="e">
-        <f>VLOOKUP($B67&amp;"3",'Raw Data'!$A:$X,I$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B67&amp;"3",'Raw Data'!$A:$X,I$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="J67" s="15"/>
@@ -18865,7 +19663,7 @@
     </row>
     <row r="68" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A68" s="15" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="B68" s="45" t="s">
@@ -18883,19 +19681,19 @@
         <v>#N/A</v>
       </c>
       <c r="F68" s="73" t="e">
-        <f>VLOOKUP($B68&amp;"3",'Raw Data'!$A:$X,F$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B68&amp;"3",'Raw Data'!$A:$X,F$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="G68" s="73" t="e">
-        <f>VLOOKUP($B68&amp;"3",'Raw Data'!$A:$X,G$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B68&amp;"3",'Raw Data'!$A:$X,G$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="H68" s="73" t="e">
-        <f>VLOOKUP($B68&amp;"3",'Raw Data'!$A:$X,H$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B68&amp;"3",'Raw Data'!$A:$X,H$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="I68" s="73" t="e">
-        <f>VLOOKUP($B68&amp;"3",'Raw Data'!$A:$X,I$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B68&amp;"3",'Raw Data'!$A:$X,I$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="J68" s="15"/>
@@ -18931,7 +19729,7 @@
     </row>
     <row r="69" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A69" s="15" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="B69" s="45" t="s">
@@ -18949,19 +19747,19 @@
         <v>#N/A</v>
       </c>
       <c r="F69" s="73" t="e">
-        <f>VLOOKUP($B69&amp;"3",'Raw Data'!$A:$X,F$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B69&amp;"3",'Raw Data'!$A:$X,F$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="G69" s="73" t="e">
-        <f>VLOOKUP($B69&amp;"3",'Raw Data'!$A:$X,G$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B69&amp;"3",'Raw Data'!$A:$X,G$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="H69" s="73" t="e">
-        <f>VLOOKUP($B69&amp;"3",'Raw Data'!$A:$X,H$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B69&amp;"3",'Raw Data'!$A:$X,H$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="I69" s="73" t="e">
-        <f>VLOOKUP($B69&amp;"3",'Raw Data'!$A:$X,I$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B69&amp;"3",'Raw Data'!$A:$X,I$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="J69" s="15"/>
@@ -18997,7 +19795,7 @@
     </row>
     <row r="70" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A70" s="15" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="B70" s="45" t="s">
@@ -19015,19 +19813,19 @@
         <v>#N/A</v>
       </c>
       <c r="F70" s="73" t="e">
-        <f>VLOOKUP($B70&amp;"3",'Raw Data'!$A:$X,F$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B70&amp;"3",'Raw Data'!$A:$X,F$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="G70" s="73" t="e">
-        <f>VLOOKUP($B70&amp;"3",'Raw Data'!$A:$X,G$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B70&amp;"3",'Raw Data'!$A:$X,G$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="H70" s="73" t="e">
-        <f>VLOOKUP($B70&amp;"3",'Raw Data'!$A:$X,H$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B70&amp;"3",'Raw Data'!$A:$X,H$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="I70" s="73" t="e">
-        <f>VLOOKUP($B70&amp;"3",'Raw Data'!$A:$X,I$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B70&amp;"3",'Raw Data'!$A:$X,I$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="J70" s="15"/>
@@ -19063,7 +19861,7 @@
     </row>
     <row r="71" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A71" s="15" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="B71" s="15" t="s">
@@ -19081,19 +19879,19 @@
         <v>#N/A</v>
       </c>
       <c r="F71" s="73" t="e">
-        <f>VLOOKUP($B71&amp;"3",'Raw Data'!$A:$X,F$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B71&amp;"3",'Raw Data'!$A:$X,F$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="G71" s="73" t="e">
-        <f>VLOOKUP($B71&amp;"3",'Raw Data'!$A:$X,G$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B71&amp;"3",'Raw Data'!$A:$X,G$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="H71" s="73" t="e">
-        <f>VLOOKUP($B71&amp;"3",'Raw Data'!$A:$X,H$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B71&amp;"3",'Raw Data'!$A:$X,H$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="I71" s="73" t="e">
-        <f>VLOOKUP($B71&amp;"3",'Raw Data'!$A:$X,I$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B71&amp;"3",'Raw Data'!$A:$X,I$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="J71" s="15"/>
@@ -19129,7 +19927,7 @@
     </row>
     <row r="72" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A72" s="15" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="B72" s="15" t="s">
@@ -19147,19 +19945,19 @@
         <v>#N/A</v>
       </c>
       <c r="F72" s="73" t="e">
-        <f>VLOOKUP($B72&amp;"3",'Raw Data'!$A:$X,F$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B72&amp;"3",'Raw Data'!$A:$X,F$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="G72" s="73" t="e">
-        <f>VLOOKUP($B72&amp;"3",'Raw Data'!$A:$X,G$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B72&amp;"3",'Raw Data'!$A:$X,G$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="H72" s="73" t="e">
-        <f>VLOOKUP($B72&amp;"3",'Raw Data'!$A:$X,H$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B72&amp;"3",'Raw Data'!$A:$X,H$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="I72" s="73" t="e">
-        <f>VLOOKUP($B72&amp;"3",'Raw Data'!$A:$X,I$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B72&amp;"3",'Raw Data'!$A:$X,I$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="J72" s="15"/>
@@ -19195,7 +19993,7 @@
     </row>
     <row r="73" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A73" s="15" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
       <c r="B73" s="15" t="s">
@@ -19213,19 +20011,19 @@
         <v>#N/A</v>
       </c>
       <c r="F73" s="73" t="e">
-        <f>VLOOKUP($B73&amp;"3",'Raw Data'!$A:$X,F$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B73&amp;"3",'Raw Data'!$A:$X,F$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="G73" s="73" t="e">
-        <f>VLOOKUP($B73&amp;"3",'Raw Data'!$A:$X,G$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B73&amp;"3",'Raw Data'!$A:$X,G$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="H73" s="73" t="e">
-        <f>VLOOKUP($B73&amp;"3",'Raw Data'!$A:$X,H$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B73&amp;"3",'Raw Data'!$A:$X,H$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="I73" s="73" t="e">
-        <f>VLOOKUP($B73&amp;"3",'Raw Data'!$A:$X,I$41,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B73&amp;"3",'Raw Data'!$A:$X,I$41,FALSE), NA())</f>
         <v>#N/A</v>
       </c>
       <c r="J73" s="15"/>
@@ -19507,44 +20305,44 @@
     </row>
     <row r="80" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A80" s="15"/>
-      <c r="B80" s="16"/>
-      <c r="C80" s="16"/>
-      <c r="D80" s="16"/>
-      <c r="E80" s="16"/>
-      <c r="F80" s="16"/>
-      <c r="G80" s="16"/>
-      <c r="H80" s="16"/>
-      <c r="I80" s="16"/>
-      <c r="J80" s="16"/>
-      <c r="K80" s="16"/>
-      <c r="L80" s="16"/>
-      <c r="M80" s="16"/>
-      <c r="N80" s="16"/>
-      <c r="O80" s="16"/>
-      <c r="P80" s="16"/>
-      <c r="Q80" s="16"/>
-      <c r="R80" s="16"/>
-      <c r="S80" s="16"/>
-      <c r="T80" s="16"/>
-      <c r="U80" s="16"/>
-      <c r="V80" s="16"/>
-      <c r="W80" s="16"/>
-      <c r="X80" s="16"/>
-      <c r="Y80" s="16"/>
-      <c r="Z80" s="16"/>
-      <c r="AA80" s="16"/>
-      <c r="AB80" s="16"/>
-      <c r="AC80" s="16"/>
-      <c r="AD80" s="16"/>
-      <c r="AE80" s="16"/>
-      <c r="AF80" s="16"/>
-      <c r="AG80" s="16"/>
-      <c r="AH80" s="16"/>
-      <c r="AI80" s="16"/>
-      <c r="AJ80" s="16"/>
-      <c r="AK80" s="16"/>
-      <c r="AL80" s="16"/>
-      <c r="AM80" s="16"/>
+      <c r="B80" s="15"/>
+      <c r="C80" s="15"/>
+      <c r="D80" s="15"/>
+      <c r="E80" s="15"/>
+      <c r="F80" s="15"/>
+      <c r="G80" s="15"/>
+      <c r="H80" s="15"/>
+      <c r="I80" s="15"/>
+      <c r="J80" s="15"/>
+      <c r="K80" s="15"/>
+      <c r="L80" s="15"/>
+      <c r="M80" s="15"/>
+      <c r="N80" s="15"/>
+      <c r="O80" s="15"/>
+      <c r="P80" s="15"/>
+      <c r="Q80" s="15"/>
+      <c r="R80" s="15"/>
+      <c r="S80" s="15"/>
+      <c r="T80" s="15"/>
+      <c r="U80" s="15"/>
+      <c r="V80" s="15"/>
+      <c r="W80" s="15"/>
+      <c r="X80" s="15"/>
+      <c r="Y80" s="15"/>
+      <c r="Z80" s="15"/>
+      <c r="AA80" s="15"/>
+      <c r="AB80" s="15"/>
+      <c r="AC80" s="15"/>
+      <c r="AD80" s="15"/>
+      <c r="AE80" s="15"/>
+      <c r="AF80" s="15"/>
+      <c r="AG80" s="15"/>
+      <c r="AH80" s="15"/>
+      <c r="AI80" s="15"/>
+      <c r="AJ80" s="15"/>
+      <c r="AK80" s="15"/>
+      <c r="AL80" s="15"/>
+      <c r="AM80" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19552,7 +20350,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:H32"/>
   <sheetViews>
@@ -19860,7 +20658,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>